<commit_message>
protein food study updated
</commit_message>
<xml_diff>
--- a/extra/studio cibi proteici.xlsx
+++ b/extra/studio cibi proteici.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Documents\uni\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676116B3-0367-4DDB-BC52-7AF5FE6A20ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2ECE417-0139-4B23-9877-C7A4F1414EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>proteine</t>
   </si>
@@ -83,10 +80,46 @@
     <t>prezzo/kg</t>
   </si>
   <si>
-    <t>pasta</t>
-  </si>
-  <si>
-    <t>pasta integrale</t>
+    <t>speck smart</t>
+  </si>
+  <si>
+    <t>besciamella smart</t>
+  </si>
+  <si>
+    <t>coppa smart</t>
+  </si>
+  <si>
+    <t>pasta integrale esslunga</t>
+  </si>
+  <si>
+    <t>pasta smart</t>
+  </si>
+  <si>
+    <t>emmental smart</t>
+  </si>
+  <si>
+    <t>maasdam smart</t>
+  </si>
+  <si>
+    <t>salmone smart</t>
+  </si>
+  <si>
+    <t>uova smart</t>
+  </si>
+  <si>
+    <t>carne secca</t>
+  </si>
+  <si>
+    <t>pane integrale esselunga</t>
+  </si>
+  <si>
+    <t>cordon bleu smart</t>
+  </si>
+  <si>
+    <t>spinacine smart</t>
+  </si>
+  <si>
+    <t>cotolette smart</t>
   </si>
 </sst>
 </file>
@@ -121,7 +154,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -223,17 +256,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -246,25 +268,22 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -272,18 +291,6 @@
     <cellStyle name="Valuta" xfId="1" builtinId="4"/>
   </cellStyles>
   <dxfs count="10">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-410]_-;\-* #,##0.00\ [$€-410]_-;_-* &quot;-&quot;??\ [$€-410]_-;_-@_-"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -415,6 +422,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -422,18 +438,21 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -450,20 +469,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84F67106-4EFF-43B6-B540-766A1D8E564D}" name="Tabella1" displayName="Tabella1" ref="A1:F12" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
-  <autoFilter ref="A1:F12" xr:uid="{84F67106-4EFF-43B6-B540-766A1D8E564D}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F12">
-    <sortCondition descending="1" ref="D1:D12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84F67106-4EFF-43B6-B540-766A1D8E564D}" name="Tabella1" displayName="Tabella1" ref="A1:F24" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="A1:F24" xr:uid="{84F67106-4EFF-43B6-B540-766A1D8E564D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F24">
+    <sortCondition descending="1" ref="D1:D24"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{30081959-5619-4B55-B7D9-1175EC07AC45}" name="/100g" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{14FCB0BC-8DE4-4AA7-8660-575F63F8B8A6}" name="proteine" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{C0B50CE8-FDFE-49A8-8945-F7C5D2CD5713}" name="calorie" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{419A7849-565C-4737-B49A-97B34AC7F736}" name="rapporto proteine/calorie" dataDxfId="3" dataCellStyle="Percentuale">
+    <tableColumn id="1" xr3:uid="{30081959-5619-4B55-B7D9-1175EC07AC45}" name="/100g" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{14FCB0BC-8DE4-4AA7-8660-575F63F8B8A6}" name="proteine" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{C0B50CE8-FDFE-49A8-8945-F7C5D2CD5713}" name="calorie" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{419A7849-565C-4737-B49A-97B34AC7F736}" name="rapporto proteine/calorie" dataDxfId="2" dataCellStyle="Percentuale">
       <calculatedColumnFormula>B2/C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{FA12BE60-94F7-4342-93BD-B6B457295831}" name="prezzo/kg" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{616FE227-9C0F-4D3A-A972-663A04B87FDE}" name="rapporto proteine/€" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{FA12BE60-94F7-4342-93BD-B6B457295831}" name="prezzo/kg" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{616FE227-9C0F-4D3A-A972-663A04B87FDE}" name="rapporto proteine/€" dataDxfId="0">
+      <calculatedColumnFormula>B2/E2</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -766,43 +787,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99DE0696-3519-4FAA-80C4-80DCCEE4AE17}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.21875" customWidth="1"/>
-    <col min="6" max="6" width="19.77734375" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3">
@@ -811,20 +833,20 @@
       <c r="C2" s="3">
         <v>150</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="14">
         <f>B2/C2</f>
         <v>0.22</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>36.200000000000003</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="13">
         <f>B2/E2</f>
         <v>0.91160220994475127</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3">
@@ -833,20 +855,20 @@
       <c r="C3" s="3">
         <v>117</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="14">
         <f>B3/C3</f>
         <v>0.18803418803418803</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>9.74</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="13">
         <f>B3/E3</f>
         <v>2.2587268993839835</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="3">
@@ -855,20 +877,20 @@
       <c r="C4" s="3">
         <v>96</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="14">
         <f>B4/C4</f>
         <v>0.1875</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>22.9</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="13">
         <f>B4/E4</f>
         <v>0.7860262008733625</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="3">
@@ -877,217 +899,496 @@
       <c r="C5" s="3">
         <v>123</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="14">
         <f>B5/C5</f>
         <v>0.16260162601626016</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>13.47</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="13">
         <f>B5/E5</f>
         <v>1.4847809948032664</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3">
+        <v>39</v>
+      </c>
+      <c r="C6" s="3">
+        <v>255</v>
+      </c>
+      <c r="D6" s="14">
+        <f>B6/C6</f>
+        <v>0.15294117647058825</v>
+      </c>
+      <c r="E6" s="5">
+        <v>131.6</v>
+      </c>
+      <c r="F6" s="13">
+        <f>B6/E6</f>
+        <v>0.29635258358662614</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="3">
+        <v>21</v>
+      </c>
+      <c r="C7" s="3">
+        <v>171</v>
+      </c>
+      <c r="D7" s="14">
+        <f>B7/C7</f>
+        <v>0.12280701754385964</v>
+      </c>
+      <c r="E7" s="5">
+        <v>26.45</v>
+      </c>
+      <c r="F7" s="13">
+        <f>B7/E7</f>
+        <v>0.79395085066162574</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3">
+        <v>28</v>
+      </c>
+      <c r="C8" s="3">
+        <v>231</v>
+      </c>
+      <c r="D8" s="14">
+        <f>B8/C8</f>
+        <v>0.12121212121212122</v>
+      </c>
+      <c r="E8" s="5">
+        <v>16.59</v>
+      </c>
+      <c r="F8" s="13">
+        <f>B8/E8</f>
+        <v>1.6877637130801688</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B9" s="3">
         <v>4.8</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C9" s="3">
         <v>41</v>
       </c>
-      <c r="D6" s="4">
-        <f>B6/C6</f>
+      <c r="D9" s="14">
+        <f>B9/C9</f>
         <v>0.11707317073170731</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E9" s="4">
         <v>1.7</v>
       </c>
-      <c r="F6" s="9">
-        <f>B6/E6</f>
+      <c r="F9" s="13">
+        <f>B9/E9</f>
         <v>2.8235294117647061</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B10" s="3">
         <v>27</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C10" s="3">
         <v>236</v>
       </c>
-      <c r="D7" s="4">
-        <f>B7/C7</f>
+      <c r="D10" s="14">
+        <f>B10/C10</f>
         <v>0.11440677966101695</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E10" s="5">
         <v>18.600000000000001</v>
       </c>
-      <c r="F7" s="9">
-        <f>B7/E7</f>
+      <c r="F10" s="13">
+        <f>B10/E10</f>
         <v>1.4516129032258063</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="3">
+        <v>26</v>
+      </c>
+      <c r="C11" s="3">
+        <v>258</v>
+      </c>
+      <c r="D11" s="14">
+        <f>B11/C11</f>
+        <v>0.10077519379844961</v>
+      </c>
+      <c r="E11" s="5">
+        <v>15.94</v>
+      </c>
+      <c r="F11" s="13">
+        <f>B11/E11</f>
+        <v>1.6311166875784191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="3">
+        <v>12.4</v>
+      </c>
+      <c r="C12" s="3">
+        <v>136</v>
+      </c>
+      <c r="D12" s="14">
+        <f>B12/C12</f>
+        <v>9.1176470588235303E-2</v>
+      </c>
+      <c r="E12" s="5">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="F12" s="13">
+        <f>B12/E12</f>
+        <v>2.4899598393574296</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="3">
+        <v>28.4</v>
+      </c>
+      <c r="C13" s="3">
+        <v>358</v>
+      </c>
+      <c r="D13" s="14">
+        <f>B13/C13</f>
+        <v>7.9329608938547486E-2</v>
+      </c>
+      <c r="E13" s="5">
+        <v>7.48</v>
+      </c>
+      <c r="F13" s="13">
+        <f>B13/E13</f>
+        <v>3.796791443850267</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="3">
+        <v>28</v>
+      </c>
+      <c r="C14" s="3">
+        <v>382</v>
+      </c>
+      <c r="D14" s="14">
+        <f>B14/C14</f>
+        <v>7.3298429319371722E-2</v>
+      </c>
+      <c r="E14" s="5">
+        <v>7.48</v>
+      </c>
+      <c r="F14" s="13">
+        <f>B14/E14</f>
+        <v>3.7433155080213902</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B15" s="3">
         <v>15</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C15" s="3">
         <v>240</v>
       </c>
-      <c r="D8" s="4">
-        <f>B8/C8</f>
+      <c r="D15" s="14">
+        <f>B15/C15</f>
         <v>6.25E-2</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E15" s="4">
         <v>2.76</v>
       </c>
-      <c r="F8" s="9">
-        <f>B8/E8</f>
+      <c r="F15" s="13">
+        <f>B15/E15</f>
         <v>5.4347826086956523</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B16" s="3">
         <v>20</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C16" s="3">
         <v>370</v>
       </c>
-      <c r="D9" s="4">
-        <f>B9/C9</f>
+      <c r="D16" s="14">
+        <f>B16/C16</f>
         <v>5.4054054054054057E-2</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="9" t="e">
-        <f>B9/E9</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="E16" s="5">
+        <v>9.67</v>
+      </c>
+      <c r="F16" s="13">
+        <f>B16/E16</f>
+        <v>2.0682523267838677</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B17" s="3">
         <v>15</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C17" s="3">
         <v>314</v>
       </c>
-      <c r="D10" s="4">
-        <f>B10/C10</f>
+      <c r="D17" s="14">
+        <f>B17/C17</f>
         <v>4.7770700636942678E-2</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="9" t="e">
-        <f>B10/E10</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="E17" s="5">
+        <v>3.99</v>
+      </c>
+      <c r="F17" s="13">
+        <f>B17/E17</f>
+        <v>3.7593984962406015</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="3">
+        <v>13</v>
+      </c>
+      <c r="C18" s="3">
+        <v>277</v>
+      </c>
+      <c r="D18" s="14">
+        <f>B18/C18</f>
+        <v>4.6931407942238268E-2</v>
+      </c>
+      <c r="E18" s="5">
+        <v>6.86</v>
+      </c>
+      <c r="F18" s="13">
+        <f>B18/E18</f>
+        <v>1.8950437317784257</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="3">
+        <v>12</v>
+      </c>
+      <c r="C19" s="3">
+        <v>267</v>
+      </c>
+      <c r="D19" s="14">
+        <f>B19/C19</f>
+        <v>4.49438202247191E-2</v>
+      </c>
+      <c r="E19" s="5">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="F19" s="13">
+        <f>B19/E19</f>
+        <v>1.4457831325301203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3">
+        <v>13.5</v>
+      </c>
+      <c r="C20" s="3">
+        <v>338</v>
+      </c>
+      <c r="D20" s="14">
+        <f>B20/C20</f>
+        <v>3.9940828402366867E-2</v>
+      </c>
+      <c r="E20" s="5">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="F20" s="13">
+        <f>B20/E20</f>
+        <v>6.1926605504587151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="3">
+        <v>11</v>
+      </c>
+      <c r="C21" s="3">
+        <v>282</v>
+      </c>
+      <c r="D21" s="14">
+        <f>B21/C21</f>
+        <v>3.9007092198581561E-2</v>
+      </c>
+      <c r="E21" s="5">
+        <v>5.99</v>
+      </c>
+      <c r="F21" s="13">
+        <f>B21/E21</f>
+        <v>1.8363939899833055</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="3">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="C22" s="3">
+        <v>257</v>
+      </c>
+      <c r="D22" s="14">
+        <f>B22/C22</f>
+        <v>3.5797665369649803E-2</v>
+      </c>
+      <c r="E22" s="5">
+        <v>2.83</v>
+      </c>
+      <c r="F22" s="13">
+        <f>B22/E22</f>
+        <v>3.250883392226148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="3">
+        <v>11.5</v>
+      </c>
+      <c r="C23" s="3">
+        <v>350</v>
+      </c>
+      <c r="D23" s="14">
+        <f>B23/C23</f>
+        <v>3.2857142857142856E-2</v>
+      </c>
+      <c r="E23" s="5">
+        <v>1.29</v>
+      </c>
+      <c r="F23" s="13">
+        <f>B23/E23</f>
+        <v>8.9147286821705425</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="3">
-        <v>13.5</v>
-      </c>
-      <c r="C11" s="3">
-        <v>338</v>
-      </c>
-      <c r="D11" s="4">
-        <f>B11/C11</f>
-        <v>3.9940828402366867E-2</v>
-      </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="14">
-        <v>11.5</v>
-      </c>
-      <c r="C12" s="14">
-        <v>350</v>
-      </c>
-      <c r="D12" s="15">
-        <f>B12/C12</f>
-        <v>3.2857142857142856E-2</v>
-      </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="17"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D14" s="1"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D16" s="1"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D17" s="1"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D18" s="1"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D19" s="1"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D20" s="1"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D21" s="1"/>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D22" s="1"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="11">
+        <v>3</v>
+      </c>
+      <c r="C24" s="11">
+        <v>110</v>
+      </c>
+      <c r="D24" s="14">
+        <f>B24/C24</f>
+        <v>2.7272727272727271E-2</v>
+      </c>
+      <c r="E24" s="12">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="F24" s="13">
+        <f>B24/E24</f>
+        <v>1.3761467889908257</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D27" s="1"/>
       <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D28" s="1"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D29" s="1"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D30" s="1"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D31" s="1"/>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D32" s="1"/>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D33" s="1"/>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="1"/>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated protein foods studies
</commit_message>
<xml_diff>
--- a/extra/studio cibi proteici.xlsx
+++ b/extra/studio cibi proteici.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Documents\uni\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2ECE417-0139-4B23-9877-C7A4F1414EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5171CC23-A619-4434-A355-D10449B8041C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>proteine</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>cotolette smart</t>
+  </si>
+  <si>
+    <t>gnocchi smart</t>
   </si>
 </sst>
 </file>
@@ -469,10 +472,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84F67106-4EFF-43B6-B540-766A1D8E564D}" name="Tabella1" displayName="Tabella1" ref="A1:F24" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
-  <autoFilter ref="A1:F24" xr:uid="{84F67106-4EFF-43B6-B540-766A1D8E564D}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F24">
-    <sortCondition descending="1" ref="D1:D24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84F67106-4EFF-43B6-B540-766A1D8E564D}" name="Tabella1" displayName="Tabella1" ref="A1:F25" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="A1:F25" xr:uid="{84F67106-4EFF-43B6-B540-766A1D8E564D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F25">
+    <sortCondition descending="1" ref="D1:D25"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{30081959-5619-4B55-B7D9-1175EC07AC45}" name="/100g" dataDxfId="5"/>
@@ -787,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99DE0696-3519-4FAA-80C4-80DCCEE4AE17}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,20 +1311,20 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24" s="3">
         <v>3</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="3">
         <v>110</v>
       </c>
       <c r="D24" s="14">
         <f>B24/C24</f>
         <v>2.7272727272727271E-2</v>
       </c>
-      <c r="E24" s="12">
+      <c r="E24" s="5">
         <v>2.1800000000000002</v>
       </c>
       <c r="F24" s="13">
@@ -1330,8 +1333,26 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D25" s="1"/>
-      <c r="E25" s="2"/>
+      <c r="A25" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="11">
+        <v>4.5</v>
+      </c>
+      <c r="C25" s="11">
+        <v>174</v>
+      </c>
+      <c r="D25" s="14">
+        <f>B25/C25</f>
+        <v>2.5862068965517241E-2</v>
+      </c>
+      <c r="E25" s="12">
+        <v>1</v>
+      </c>
+      <c r="F25" s="13">
+        <f>B25/E25</f>
+        <v>4.5</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
@@ -1370,6 +1391,7 @@
       <c r="E34" s="2"/>
     </row>
     <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D35" s="1"/>
       <c r="E35" s="2"/>
     </row>
     <row r="36" spans="4:5" x14ac:dyDescent="0.25">
@@ -1383,6 +1405,9 @@
     </row>
     <row r="39" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E40" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added ocrs and other documents
</commit_message>
<xml_diff>
--- a/extra/studio cibi proteici.xlsx
+++ b/extra/studio cibi proteici.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Documents\uni\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5171CC23-A619-4434-A355-D10449B8041C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515AEC94-5502-43A8-8649-CB53D6400111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="58">
   <si>
     <t>proteine</t>
   </si>
@@ -123,6 +124,90 @@
   </si>
   <si>
     <t>gnocchi smart</t>
+  </si>
+  <si>
+    <t>100g di pasta smart</t>
+  </si>
+  <si>
+    <t>2 latte di tonno smart</t>
+  </si>
+  <si>
+    <t>6 wurstel smart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150g di pane integrale </t>
+  </si>
+  <si>
+    <t>5 wurstel smart</t>
+  </si>
+  <si>
+    <t>3 latte di tonno smart</t>
+  </si>
+  <si>
+    <t>7 wurstel smart</t>
+  </si>
+  <si>
+    <t>un terzo di bottiglia di succo smart</t>
+  </si>
+  <si>
+    <t>150g di prosciutto cotto smart</t>
+  </si>
+  <si>
+    <t>1 latta di tonno smart</t>
+  </si>
+  <si>
+    <t>euro</t>
+  </si>
+  <si>
+    <t>250g pasta</t>
+  </si>
+  <si>
+    <t>92,5g sugo tigullio</t>
+  </si>
+  <si>
+    <t>100g mozzarella</t>
+  </si>
+  <si>
+    <t>latte riso e cocco</t>
+  </si>
+  <si>
+    <t>biscotti ritornelli</t>
+  </si>
+  <si>
+    <t>100g di pane integrale</t>
+  </si>
+  <si>
+    <t>5,22 wurstel smart</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>media</t>
+  </si>
+  <si>
+    <t>cal</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>2gg tot 12</t>
+  </si>
+  <si>
+    <t>2gg tot 13</t>
+  </si>
+  <si>
+    <t>per consumare i wurstel smart</t>
+  </si>
+  <si>
+    <t>fare 2 giorni in cui seguire il C e l'F</t>
+  </si>
+  <si>
+    <t>direttamente usando i wurtstel smart</t>
+  </si>
+  <si>
+    <t>per fare la media con wurstel penny</t>
   </si>
 </sst>
 </file>
@@ -133,7 +218,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-410]_-;\-* #,##0.00\ [$€-410]_-;_-* &quot;-&quot;??\ [$€-410]_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,13 +233,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -271,7 +380,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -287,6 +396,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -790,10 +904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99DE0696-3519-4FAA-80C4-80DCCEE4AE17}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D33" sqref="D31:F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,9 +918,11 @@
     <col min="4" max="4" width="26.7109375" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="8" max="8" width="33.28515625" customWidth="1"/>
+    <col min="13" max="13" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -826,7 +942,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -837,18 +953,36 @@
         <v>150</v>
       </c>
       <c r="D2" s="14">
-        <f>B2/C2</f>
+        <f t="shared" ref="D2:D25" si="0">B2/C2</f>
         <v>0.22</v>
       </c>
       <c r="E2" s="5">
         <v>36.200000000000003</v>
       </c>
       <c r="F2" s="13">
-        <f>B2/E2</f>
+        <f t="shared" ref="F2:F25" si="1">B2/E2</f>
         <v>0.91160220994475127</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -859,18 +993,42 @@
         <v>117</v>
       </c>
       <c r="D3" s="14">
-        <f>B3/C3</f>
+        <f t="shared" si="0"/>
         <v>0.18803418803418803</v>
       </c>
       <c r="E3" s="4">
         <v>9.74</v>
       </c>
       <c r="F3" s="13">
-        <f>B3/E3</f>
+        <f t="shared" si="1"/>
         <v>2.2587268993839835</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="3">
+        <v>185</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="16">
+        <v>0.33</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="3">
+        <v>185</v>
+      </c>
+      <c r="O3" s="3">
+        <v>0</v>
+      </c>
+      <c r="P3" s="16">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -881,18 +1039,45 @@
         <v>96</v>
       </c>
       <c r="D4" s="14">
-        <f>B4/C4</f>
+        <f t="shared" si="0"/>
         <v>0.1875</v>
       </c>
       <c r="E4" s="4">
         <v>22.9</v>
       </c>
       <c r="F4" s="13">
-        <f>B4/E4</f>
+        <f t="shared" si="1"/>
         <v>0.7860262008733625</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H4" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="17">
+        <f>(131)*2</f>
+        <v>262</v>
+      </c>
+      <c r="J4" s="3">
+        <f>25*2</f>
+        <v>50</v>
+      </c>
+      <c r="K4" s="3">
+        <f>1.09*2</f>
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" s="3">
+        <v>262</v>
+      </c>
+      <c r="O4" s="3">
+        <v>50</v>
+      </c>
+      <c r="P4" s="3">
+        <v>2.1800000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
@@ -903,18 +1088,45 @@
         <v>123</v>
       </c>
       <c r="D5" s="14">
-        <f>B5/C5</f>
+        <f t="shared" si="0"/>
         <v>0.16260162601626016</v>
       </c>
       <c r="E5" s="5">
         <v>13.47</v>
       </c>
       <c r="F5" s="13">
-        <f>B5/E5</f>
+        <f t="shared" si="1"/>
         <v>1.4847809948032664</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H5" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="3">
+        <f>$C$15*6</f>
+        <v>1440</v>
+      </c>
+      <c r="J5" s="3">
+        <f>6*$B$15</f>
+        <v>90</v>
+      </c>
+      <c r="K5" s="5">
+        <f>($E$15*0.1)*6</f>
+        <v>1.6559999999999997</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="N5" s="3">
+        <v>1440</v>
+      </c>
+      <c r="O5" s="3">
+        <v>90</v>
+      </c>
+      <c r="P5" s="3">
+        <v>1.6559999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>24</v>
       </c>
@@ -925,18 +1137,45 @@
         <v>255</v>
       </c>
       <c r="D6" s="14">
-        <f>B6/C6</f>
+        <f t="shared" si="0"/>
         <v>0.15294117647058825</v>
       </c>
       <c r="E6" s="5">
         <v>131.6</v>
       </c>
       <c r="F6" s="13">
-        <f>B6/E6</f>
+        <f t="shared" si="1"/>
         <v>0.29635258358662614</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H6" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="3">
+        <f>$C$23*1</f>
+        <v>350</v>
+      </c>
+      <c r="J6" s="3">
+        <f>$B$23*1</f>
+        <v>11.5</v>
+      </c>
+      <c r="K6" s="16">
+        <f>$E$23*0.1</f>
+        <v>0.129</v>
+      </c>
+      <c r="M6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6" s="3">
+        <v>386</v>
+      </c>
+      <c r="O6" s="3">
+        <v>13.8</v>
+      </c>
+      <c r="P6" s="3">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
@@ -947,18 +1186,44 @@
         <v>171</v>
       </c>
       <c r="D7" s="14">
-        <f>B7/C7</f>
+        <f t="shared" si="0"/>
         <v>0.12280701754385964</v>
       </c>
       <c r="E7" s="5">
         <v>26.45</v>
       </c>
       <c r="F7" s="13">
-        <f>B7/E7</f>
+        <f t="shared" si="1"/>
         <v>0.79395085066162574</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H7" s="3"/>
+      <c r="I7" s="3">
+        <f>SUM(I3:I6)</f>
+        <v>2237</v>
+      </c>
+      <c r="J7" s="3">
+        <f>SUM(J3:J6)</f>
+        <v>151.5</v>
+      </c>
+      <c r="K7" s="3">
+        <f>SUM(K3:K6)</f>
+        <v>4.2949999999999999</v>
+      </c>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3">
+        <f>SUM(N3:N6)</f>
+        <v>2273</v>
+      </c>
+      <c r="O7" s="3">
+        <f>SUM(O3:O6)</f>
+        <v>153.80000000000001</v>
+      </c>
+      <c r="P7" s="3">
+        <f>SUM(P3:P6)</f>
+        <v>4.5860000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
@@ -969,18 +1234,18 @@
         <v>231</v>
       </c>
       <c r="D8" s="14">
-        <f>B8/C8</f>
+        <f t="shared" si="0"/>
         <v>0.12121212121212122</v>
       </c>
       <c r="E8" s="5">
         <v>16.59</v>
       </c>
       <c r="F8" s="13">
-        <f>B8/E8</f>
+        <f t="shared" si="1"/>
         <v>1.6877637130801688</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -991,18 +1256,18 @@
         <v>41</v>
       </c>
       <c r="D9" s="14">
-        <f>B9/C9</f>
+        <f t="shared" si="0"/>
         <v>0.11707317073170731</v>
       </c>
       <c r="E9" s="4">
         <v>1.7</v>
       </c>
       <c r="F9" s="13">
-        <f>B9/E9</f>
+        <f t="shared" si="1"/>
         <v>2.8235294117647061</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
@@ -1013,18 +1278,36 @@
         <v>236</v>
       </c>
       <c r="D10" s="14">
-        <f>B10/C10</f>
+        <f t="shared" si="0"/>
         <v>0.11440677966101695</v>
       </c>
       <c r="E10" s="5">
         <v>18.600000000000001</v>
       </c>
       <c r="F10" s="13">
-        <f>B10/E10</f>
+        <f t="shared" si="1"/>
         <v>1.4516129032258063</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I10" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="N10" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="O10" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="P10" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
@@ -1035,18 +1318,43 @@
         <v>258</v>
       </c>
       <c r="D11" s="14">
-        <f>B11/C11</f>
+        <f t="shared" si="0"/>
         <v>0.10077519379844961</v>
       </c>
       <c r="E11" s="5">
         <v>15.94</v>
       </c>
       <c r="F11" s="13">
-        <f>B11/E11</f>
+        <f t="shared" si="1"/>
         <v>1.6311166875784191</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H11" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="3">
+        <v>185</v>
+      </c>
+      <c r="J11" s="3">
+        <f>0.4*3</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="K11" s="16">
+        <v>0.33</v>
+      </c>
+      <c r="M11" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="N11" s="3">
+        <v>185</v>
+      </c>
+      <c r="O11" s="3">
+        <v>0</v>
+      </c>
+      <c r="P11" s="16">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
@@ -1057,18 +1365,48 @@
         <v>136</v>
       </c>
       <c r="D12" s="14">
-        <f>B12/C12</f>
+        <f t="shared" si="0"/>
         <v>9.1176470588235303E-2</v>
       </c>
       <c r="E12" s="5">
         <v>4.9800000000000004</v>
       </c>
       <c r="F12" s="13">
-        <f>B12/E12</f>
+        <f t="shared" si="1"/>
         <v>2.4899598393574296</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H12" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="17">
+        <f>(131)*3</f>
+        <v>393</v>
+      </c>
+      <c r="J12" s="3">
+        <f>25*3</f>
+        <v>75</v>
+      </c>
+      <c r="K12" s="3">
+        <f>1.09*3</f>
+        <v>3.2700000000000005</v>
+      </c>
+      <c r="M12" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="N12" s="17">
+        <f>(131)*1</f>
+        <v>131</v>
+      </c>
+      <c r="O12" s="3">
+        <f>25*1</f>
+        <v>25</v>
+      </c>
+      <c r="P12" s="3">
+        <f>1.09*1</f>
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>21</v>
       </c>
@@ -1079,18 +1417,48 @@
         <v>358</v>
       </c>
       <c r="D13" s="14">
-        <f>B13/C13</f>
+        <f t="shared" si="0"/>
         <v>7.9329608938547486E-2</v>
       </c>
       <c r="E13" s="5">
         <v>7.48</v>
       </c>
       <c r="F13" s="13">
-        <f>B13/E13</f>
+        <f t="shared" si="1"/>
         <v>3.796791443850267</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" s="3">
+        <f>$C$15*5</f>
+        <v>1200</v>
+      </c>
+      <c r="J13" s="3">
+        <f>5*$B$15</f>
+        <v>75</v>
+      </c>
+      <c r="K13" s="16">
+        <f>($E$15*0.1)*5</f>
+        <v>1.38</v>
+      </c>
+      <c r="M13" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="N13" s="3">
+        <f>$C$15*6</f>
+        <v>1440</v>
+      </c>
+      <c r="O13" s="3">
+        <f>6*$B$15</f>
+        <v>90</v>
+      </c>
+      <c r="P13" s="16">
+        <f>($E$15*0.1)*6</f>
+        <v>1.6559999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>20</v>
       </c>
@@ -1101,18 +1469,37 @@
         <v>382</v>
       </c>
       <c r="D14" s="14">
-        <f>B14/C14</f>
+        <f t="shared" si="0"/>
         <v>7.3298429319371722E-2</v>
       </c>
       <c r="E14" s="5">
         <v>7.48</v>
       </c>
       <c r="F14" s="13">
-        <f>B14/E14</f>
+        <f t="shared" si="1"/>
         <v>3.7433155080213902</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="M14" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="N14" s="3">
+        <f>123*1.5</f>
+        <v>184.5</v>
+      </c>
+      <c r="O14" s="3">
+        <f>20*1.5</f>
+        <v>30</v>
+      </c>
+      <c r="P14" s="3">
+        <f>1.347*1.5</f>
+        <v>2.0205000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>5</v>
       </c>
@@ -1123,18 +1510,43 @@
         <v>240</v>
       </c>
       <c r="D15" s="14">
-        <f>B15/C15</f>
+        <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
       <c r="E15" s="4">
         <v>2.76</v>
       </c>
       <c r="F15" s="13">
-        <f>B15/E15</f>
+        <f t="shared" si="1"/>
         <v>5.4347826086956523</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H15" s="3"/>
+      <c r="I15" s="3">
+        <f>SUM(I11:I14)</f>
+        <v>1778</v>
+      </c>
+      <c r="J15" s="3">
+        <f>SUM(J11:J14)</f>
+        <v>151.19999999999999</v>
+      </c>
+      <c r="K15" s="3">
+        <f>SUM(K11:K14)</f>
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="M15" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="N15" s="3">
+        <v>386</v>
+      </c>
+      <c r="O15" s="3">
+        <v>13.8</v>
+      </c>
+      <c r="P15" s="3">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>9</v>
       </c>
@@ -1145,18 +1557,31 @@
         <v>370</v>
       </c>
       <c r="D16" s="14">
-        <f>B16/C16</f>
+        <f t="shared" si="0"/>
         <v>5.4054054054054057E-2</v>
       </c>
       <c r="E16" s="5">
         <v>9.67</v>
       </c>
       <c r="F16" s="13">
-        <f>B16/E16</f>
+        <f t="shared" si="1"/>
         <v>2.0682523267838677</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M16" s="3"/>
+      <c r="N16" s="17">
+        <f>SUM(N11:N15)</f>
+        <v>2326.5</v>
+      </c>
+      <c r="O16" s="3">
+        <f>SUM(O11:O15)</f>
+        <v>158.80000000000001</v>
+      </c>
+      <c r="P16" s="3">
+        <f>SUM(P11:P15)</f>
+        <v>5.5164999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>10</v>
       </c>
@@ -1167,18 +1592,18 @@
         <v>314</v>
       </c>
       <c r="D17" s="14">
-        <f>B17/C17</f>
+        <f t="shared" si="0"/>
         <v>4.7770700636942678E-2</v>
       </c>
       <c r="E17" s="5">
         <v>3.99</v>
       </c>
       <c r="F17" s="13">
-        <f>B17/E17</f>
+        <f t="shared" si="1"/>
         <v>3.7593984962406015</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>26</v>
       </c>
@@ -1189,18 +1614,18 @@
         <v>277</v>
       </c>
       <c r="D18" s="14">
-        <f>B18/C18</f>
+        <f t="shared" si="0"/>
         <v>4.6931407942238268E-2</v>
       </c>
       <c r="E18" s="5">
         <v>6.86</v>
       </c>
       <c r="F18" s="13">
-        <f>B18/E18</f>
+        <f t="shared" si="1"/>
         <v>1.8950437317784257</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>28</v>
       </c>
@@ -1211,18 +1636,36 @@
         <v>267</v>
       </c>
       <c r="D19" s="14">
-        <f>B19/C19</f>
+        <f t="shared" si="0"/>
         <v>4.49438202247191E-2</v>
       </c>
       <c r="E19" s="5">
         <v>8.3000000000000007</v>
       </c>
       <c r="F19" s="13">
-        <f>B19/E19</f>
+        <f t="shared" si="1"/>
         <v>1.4457831325301203</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I19" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="J19" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="K19" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="N19" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="O19" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="P19" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
@@ -1233,18 +1676,44 @@
         <v>338</v>
       </c>
       <c r="D20" s="14">
-        <f>B20/C20</f>
+        <f t="shared" si="0"/>
         <v>3.9940828402366867E-2</v>
       </c>
       <c r="E20" s="5">
         <v>2.1800000000000002</v>
       </c>
       <c r="F20" s="13">
-        <f>B20/E20</f>
+        <f t="shared" si="1"/>
         <v>6.1926605504587151</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H20" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" s="3">
+        <v>185</v>
+      </c>
+      <c r="J20" s="3">
+        <f>0.4*3</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="K20" s="16">
+        <v>0.33</v>
+      </c>
+      <c r="M20" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="N20" s="3">
+        <v>185</v>
+      </c>
+      <c r="O20" s="3">
+        <f>0.4*3</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="P20" s="16">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>27</v>
       </c>
@@ -1255,18 +1724,48 @@
         <v>282</v>
       </c>
       <c r="D21" s="14">
-        <f>B21/C21</f>
+        <f t="shared" si="0"/>
         <v>3.9007092198581561E-2</v>
       </c>
       <c r="E21" s="5">
         <v>5.99</v>
       </c>
       <c r="F21" s="13">
-        <f>B21/E21</f>
+        <f t="shared" si="1"/>
         <v>1.8363939899833055</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H21" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I21" s="17">
+        <f>(131)*2</f>
+        <v>262</v>
+      </c>
+      <c r="J21" s="3">
+        <f>25*2</f>
+        <v>50</v>
+      </c>
+      <c r="K21" s="3">
+        <f>1.09*2</f>
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="M21" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="N21" s="17">
+        <f>(131)*2</f>
+        <v>262</v>
+      </c>
+      <c r="O21" s="3">
+        <f>25*2</f>
+        <v>50</v>
+      </c>
+      <c r="P21" s="3">
+        <f>1.09*2</f>
+        <v>2.1800000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>25</v>
       </c>
@@ -1277,18 +1776,48 @@
         <v>257</v>
       </c>
       <c r="D22" s="14">
-        <f>B22/C22</f>
+        <f t="shared" si="0"/>
         <v>3.5797665369649803E-2</v>
       </c>
       <c r="E22" s="5">
         <v>2.83</v>
       </c>
       <c r="F22" s="13">
-        <f>B22/E22</f>
+        <f t="shared" si="1"/>
         <v>3.250883392226148</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H22" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="I22" s="3">
+        <f>$C$15*7</f>
+        <v>1680</v>
+      </c>
+      <c r="J22" s="3">
+        <f>7*$B$15</f>
+        <v>105</v>
+      </c>
+      <c r="K22" s="5">
+        <f>($E$15*0.1)*7</f>
+        <v>1.9319999999999997</v>
+      </c>
+      <c r="M22" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="N22" s="3">
+        <f>$C$15*6</f>
+        <v>1440</v>
+      </c>
+      <c r="O22" s="3">
+        <f>6*$B$15</f>
+        <v>90</v>
+      </c>
+      <c r="P22" s="5">
+        <f>($E$15*0.1)*6</f>
+        <v>1.6559999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>19</v>
       </c>
@@ -1299,18 +1828,37 @@
         <v>350</v>
       </c>
       <c r="D23" s="14">
-        <f>B23/C23</f>
+        <f t="shared" si="0"/>
         <v>3.2857142857142856E-2</v>
       </c>
       <c r="E23" s="5">
         <v>1.29</v>
       </c>
       <c r="F23" s="13">
-        <f>B23/E23</f>
+        <f t="shared" si="1"/>
         <v>8.9147286821705425</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H23" s="19"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="16"/>
+      <c r="M23" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="N23" s="3">
+        <f>257*1</f>
+        <v>257</v>
+      </c>
+      <c r="O23" s="3">
+        <f>9.2*1</f>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="P23" s="16">
+        <f>0.283*1</f>
+        <v>0.28299999999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>16</v>
       </c>
@@ -1321,18 +1869,35 @@
         <v>110</v>
       </c>
       <c r="D24" s="14">
-        <f>B24/C24</f>
+        <f t="shared" si="0"/>
         <v>2.7272727272727271E-2</v>
       </c>
       <c r="E24" s="5">
         <v>2.1800000000000002</v>
       </c>
       <c r="F24" s="13">
-        <f>B24/E24</f>
+        <f t="shared" si="1"/>
         <v>1.3761467889908257</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H24" s="3"/>
+      <c r="I24" s="3">
+        <f>SUM(I20:I23)</f>
+        <v>2127</v>
+      </c>
+      <c r="J24" s="3">
+        <f>SUM(J20:J23)</f>
+        <v>156.19999999999999</v>
+      </c>
+      <c r="K24" s="3">
+        <f>SUM(K20:K23)</f>
+        <v>4.4420000000000002</v>
+      </c>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>29</v>
       </c>
@@ -1343,77 +1908,342 @@
         <v>174</v>
       </c>
       <c r="D25" s="14">
-        <f>B25/C25</f>
+        <f t="shared" si="0"/>
         <v>2.5862068965517241E-2</v>
       </c>
       <c r="E25" s="12">
         <v>1</v>
       </c>
       <c r="F25" s="13">
-        <f>B25/E25</f>
+        <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M25" s="3"/>
+      <c r="N25" s="3">
+        <f>SUM(N20:N24)</f>
+        <v>2144</v>
+      </c>
+      <c r="O25" s="3">
+        <f>SUM(O20:O24)</f>
+        <v>150.39999999999998</v>
+      </c>
+      <c r="P25" s="3">
+        <f>SUM(P20:P24)</f>
+        <v>4.4490000000000007</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D27" s="1"/>
       <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J27" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="K27" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
       <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>57</v>
+      </c>
+      <c r="I28" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J28" s="3">
+        <v>1778</v>
+      </c>
+      <c r="K28" s="3">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="N28" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="O28" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="P28" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D29" s="1"/>
       <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>52</v>
+      </c>
+      <c r="I29" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="J29" s="3">
+        <v>2144</v>
+      </c>
+      <c r="K29" s="3">
+        <v>4.4489999999999998</v>
+      </c>
+      <c r="M29" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="N29" s="3">
+        <v>185</v>
+      </c>
+      <c r="O29" s="3">
+        <f>0.4*3</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="P29" s="16">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D30" s="1"/>
       <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D31" s="1"/>
-      <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D32" s="1"/>
-      <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D33" s="1"/>
-      <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D34" s="1"/>
-      <c r="E34" s="2"/>
-    </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D35" s="1"/>
-      <c r="E35" s="2"/>
-    </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E36" s="2"/>
-    </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>53</v>
+      </c>
+      <c r="I30" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="J30" s="15">
+        <f>AVERAGE(J28:J29)</f>
+        <v>1961</v>
+      </c>
+      <c r="K30" s="15">
+        <f>AVERAGE(K28:K29)</f>
+        <v>4.7145000000000001</v>
+      </c>
+      <c r="M30" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="N30" s="17">
+        <f>(131)*2</f>
+        <v>262</v>
+      </c>
+      <c r="O30" s="3">
+        <f>25*2</f>
+        <v>50</v>
+      </c>
+      <c r="P30" s="3">
+        <f>1.09*2</f>
+        <v>2.1800000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M31" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="N31" s="3">
+        <f>$C$15*5.22</f>
+        <v>1252.8</v>
+      </c>
+      <c r="O31" s="3">
+        <f>5.22*$B$15</f>
+        <v>78.3</v>
+      </c>
+      <c r="P31" s="16">
+        <f>($E$15*0.1)*5.22</f>
+        <v>1.4407199999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M32" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="N32" s="3">
+        <f>257*1</f>
+        <v>257</v>
+      </c>
+      <c r="O32" s="3">
+        <f>9.2*1</f>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="P32" s="16">
+        <f>0.283*1</f>
+        <v>0.28299999999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C33" s="1"/>
+      <c r="D33" s="2"/>
+      <c r="H33" t="s">
+        <v>54</v>
+      </c>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+    </row>
+    <row r="34" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C34" s="1"/>
+      <c r="D34" s="2"/>
+      <c r="H34" t="s">
+        <v>55</v>
+      </c>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3">
+        <f>SUM(N29:N33)</f>
+        <v>1956.8</v>
+      </c>
+      <c r="O34" s="3">
+        <f>SUM(O29:O33)</f>
+        <v>138.69999999999999</v>
+      </c>
+      <c r="P34" s="3">
+        <f>SUM(P29:P33)</f>
+        <v>4.2337199999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C35" s="1"/>
+      <c r="D35" s="2"/>
+      <c r="H35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C36" s="1"/>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E38" s="2"/>
     </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E39" s="2"/>
     </row>
-    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E40" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{619C59B3-5361-4003-B0C2-E8CD91BFF358}">
+  <dimension ref="A2:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2">
+        <f>359*2.5</f>
+        <v>897.5</v>
+      </c>
+      <c r="C2">
+        <f>14*2.5</f>
+        <v>35</v>
+      </c>
+      <c r="D2">
+        <f>0.14*2.5</f>
+        <v>0.35000000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3">
+        <f>362*0.925</f>
+        <v>334.85</v>
+      </c>
+      <c r="C3">
+        <f>6.1*0.925</f>
+        <v>5.6425000000000001</v>
+      </c>
+      <c r="D3">
+        <f>1.4*0.925</f>
+        <v>1.2949999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4">
+        <f>223*1</f>
+        <v>223</v>
+      </c>
+      <c r="C4">
+        <f>15.8*1</f>
+        <v>15.8</v>
+      </c>
+      <c r="D4">
+        <f>0.9*1</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5">
+        <f>56*1</f>
+        <v>56</v>
+      </c>
+      <c r="C5">
+        <f>0.3*1</f>
+        <v>0.3</v>
+      </c>
+      <c r="D5">
+        <f>0.2*1</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6">
+        <f>480*0.75</f>
+        <v>360</v>
+      </c>
+      <c r="C6">
+        <f>6.8*0.75</f>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D6">
+        <f>0.25*0.75</f>
+        <v>0.1875</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <f>SUM(B2:B8)</f>
+        <v>1871.35</v>
+      </c>
+      <c r="C9">
+        <f>SUM(C2:C8)</f>
+        <v>61.842499999999994</v>
+      </c>
+      <c r="D9">
+        <f>SUM(D2:D8)</f>
+        <v>2.9325000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
tex documents and update on foods
</commit_message>
<xml_diff>
--- a/extra/studio cibi proteici.xlsx
+++ b/extra/studio cibi proteici.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Documents\uni\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5788A61-1BBD-4677-863C-727CE4AEEF66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D573CF68-9FF0-4B87-B09D-A2EDE22199CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="81">
   <si>
     <t>proteine</t>
   </si>
@@ -159,21 +159,6 @@
     <t>euro</t>
   </si>
   <si>
-    <t>250g pasta</t>
-  </si>
-  <si>
-    <t>92,5g sugo tigullio</t>
-  </si>
-  <si>
-    <t>100g mozzarella</t>
-  </si>
-  <si>
-    <t>latte riso e cocco</t>
-  </si>
-  <si>
-    <t>biscotti ritornelli</t>
-  </si>
-  <si>
     <t>100g di pane integrale</t>
   </si>
   <si>
@@ -208,6 +193,90 @@
   </si>
   <si>
     <t>per fare la media con wurstel penny</t>
+  </si>
+  <si>
+    <t>piano settimanale</t>
+  </si>
+  <si>
+    <t>lunedì</t>
+  </si>
+  <si>
+    <t>martedì</t>
+  </si>
+  <si>
+    <t>mercoledì</t>
+  </si>
+  <si>
+    <t>giovedì</t>
+  </si>
+  <si>
+    <t>venerdì</t>
+  </si>
+  <si>
+    <t>sabato</t>
+  </si>
+  <si>
+    <t>domenica</t>
+  </si>
+  <si>
+    <t>wurstel penny</t>
+  </si>
+  <si>
+    <t>scatoletta di tonno</t>
+  </si>
+  <si>
+    <t>succo</t>
+  </si>
+  <si>
+    <t>fibre</t>
+  </si>
+  <si>
+    <t>6 wurstel p</t>
+  </si>
+  <si>
+    <t>2 tonno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100g pane </t>
+  </si>
+  <si>
+    <t>100g di pane</t>
+  </si>
+  <si>
+    <t>lun</t>
+  </si>
+  <si>
+    <t>totale</t>
+  </si>
+  <si>
+    <t>mar</t>
+  </si>
+  <si>
+    <t>mer</t>
+  </si>
+  <si>
+    <t>gio</t>
+  </si>
+  <si>
+    <t>dom</t>
+  </si>
+  <si>
+    <t>ven</t>
+  </si>
+  <si>
+    <t>7 wurstel p</t>
+  </si>
+  <si>
+    <t>8 wurstel p</t>
+  </si>
+  <si>
+    <t>media calorie</t>
+  </si>
+  <si>
+    <t>media proteine</t>
+  </si>
+  <si>
+    <t>media euro</t>
   </si>
 </sst>
 </file>
@@ -380,7 +449,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -401,6 +470,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -906,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99DE0696-3519-4FAA-80C4-80DCCEE4AE17}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1843,7 +1915,7 @@
       <c r="J23" s="3"/>
       <c r="K23" s="16"/>
       <c r="M23" s="15" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="N23" s="3">
         <f>257*1</f>
@@ -1940,7 +2012,7 @@
       <c r="D27" s="1"/>
       <c r="E27" s="2"/>
       <c r="J27" s="15" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="K27" s="15" t="s">
         <v>40</v>
@@ -1950,10 +2022,10 @@
       <c r="D28" s="1"/>
       <c r="E28" s="2"/>
       <c r="H28" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I28" s="15" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J28" s="3">
         <v>1778</v>
@@ -1975,10 +2047,10 @@
       <c r="D29" s="1"/>
       <c r="E29" s="2"/>
       <c r="H29" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="I29" s="15" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="J29" s="3">
         <v>2144</v>
@@ -2004,10 +2076,10 @@
       <c r="D30" s="1"/>
       <c r="E30" s="2"/>
       <c r="H30" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I30" s="15" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="J30" s="15">
         <f>AVERAGE(J28:J29)</f>
@@ -2035,7 +2107,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M31" s="15" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="N31" s="3">
         <f>$C$15*5.22</f>
@@ -2052,7 +2124,7 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M32" s="15" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="N32" s="3">
         <f>257*1</f>
@@ -2071,7 +2143,7 @@
       <c r="C33" s="1"/>
       <c r="D33" s="2"/>
       <c r="H33" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
@@ -2082,7 +2154,7 @@
       <c r="C34" s="1"/>
       <c r="D34" s="2"/>
       <c r="H34" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="M34" s="3"/>
       <c r="N34" s="3">
@@ -2102,7 +2174,7 @@
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
       <c r="H35" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="3:16" x14ac:dyDescent="0.25">
@@ -2133,117 +2205,854 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{619C59B3-5361-4003-B0C2-E8CD91BFF358}">
-  <dimension ref="A2:D9"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2">
-        <f>359*2.5</f>
-        <v>897.5</v>
-      </c>
-      <c r="C2">
-        <f>14*2.5</f>
-        <v>35</v>
-      </c>
-      <c r="D2">
-        <f>0.14*2.5</f>
-        <v>0.35000000000000003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3">
-        <f>362*0.925</f>
-        <v>334.85</v>
-      </c>
-      <c r="C3">
-        <f>6.1*0.925</f>
-        <v>5.6425000000000001</v>
-      </c>
-      <c r="D3">
-        <f>1.4*0.925</f>
-        <v>1.2949999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4">
-        <f>223*1</f>
-        <v>223</v>
-      </c>
-      <c r="C4">
-        <f>15.8*1</f>
-        <v>15.8</v>
-      </c>
-      <c r="D4">
-        <f>0.9*1</f>
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5">
-        <f>56*1</f>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K1" s="15"/>
+      <c r="L1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C5">
-        <f>0.3*1</f>
-        <v>0.3</v>
-      </c>
-      <c r="D5">
-        <f>0.2*1</f>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6">
-        <f>480*0.75</f>
-        <v>360</v>
-      </c>
-      <c r="C6">
-        <f>6.8*0.75</f>
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="D6">
-        <f>0.25*0.75</f>
-        <v>0.1875</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <f>SUM(B2:B8)</f>
-        <v>1871.35</v>
-      </c>
-      <c r="C9">
-        <f>SUM(C2:C8)</f>
-        <v>61.842499999999994</v>
-      </c>
-      <c r="D9">
-        <f>SUM(D2:D8)</f>
-        <v>2.9325000000000001</v>
+      <c r="E2" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" s="3">
+        <f>0.87*240</f>
+        <v>208.8</v>
+      </c>
+      <c r="M2" s="3">
+        <f>15*0.87</f>
+        <v>13.05</v>
+      </c>
+      <c r="N2" s="3"/>
+      <c r="O2" s="20">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <f>B19</f>
+        <v>1940.8000000000002</v>
+      </c>
+      <c r="C3" s="3">
+        <f>G19</f>
+        <v>1940.8000000000002</v>
+      </c>
+      <c r="D3" s="3">
+        <f>L19</f>
+        <v>1892.6000000000001</v>
+      </c>
+      <c r="E3" s="3">
+        <f>Q19</f>
+        <v>1892.6000000000001</v>
+      </c>
+      <c r="F3" s="3">
+        <f>B26</f>
+        <v>2101.4</v>
+      </c>
+      <c r="G3" s="3">
+        <f>G26</f>
+        <v>1940.8000000000002</v>
+      </c>
+      <c r="H3" s="3">
+        <f>L26</f>
+        <v>1892.6000000000001</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="L3" s="3">
+        <v>123</v>
+      </c>
+      <c r="M3" s="3">
+        <v>30</v>
+      </c>
+      <c r="N3" s="3"/>
+      <c r="O3" s="20">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3">
+        <f>C19</f>
+        <v>147.5</v>
+      </c>
+      <c r="C4" s="3">
+        <f>H19</f>
+        <v>147.5</v>
+      </c>
+      <c r="D4" s="3">
+        <f>M19</f>
+        <v>151.35000000000002</v>
+      </c>
+      <c r="E4" s="3">
+        <f>R19</f>
+        <v>151.35000000000002</v>
+      </c>
+      <c r="F4" s="3">
+        <f>C26</f>
+        <v>164.4</v>
+      </c>
+      <c r="G4" s="3">
+        <f>H26</f>
+        <v>147.5</v>
+      </c>
+      <c r="H4" s="3">
+        <f>M26</f>
+        <v>151.35000000000002</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="L4" s="3">
+        <v>185</v>
+      </c>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="20">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="21">
+        <f>D19</f>
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="C5" s="21">
+        <f>I19</f>
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="D5" s="21">
+        <f>N19</f>
+        <v>4.0500000000000007</v>
+      </c>
+      <c r="E5" s="21">
+        <f>S19</f>
+        <v>4.0500000000000007</v>
+      </c>
+      <c r="F5" s="21">
+        <f>D26</f>
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="G5" s="21">
+        <f>I26</f>
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="H5" s="21">
+        <f>N26</f>
+        <v>4.0500000000000007</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="L5" s="3">
+        <v>257</v>
+      </c>
+      <c r="M5" s="3">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="N5" s="3">
+        <v>7.2</v>
+      </c>
+      <c r="O5" s="20">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="3">
+        <f>AVERAGE(B3:H3)</f>
+        <v>1943.0857142857144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="3">
+        <f t="shared" ref="B8:B9" si="0">AVERAGE(B4:H4)</f>
+        <v>151.56428571428572</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="3">
+        <f t="shared" si="0"/>
+        <v>4.1071428571428568</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="K14" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="L14" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M14" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="N14" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="P14" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q14" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="R14" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="S14" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="3">
+        <f>$L$4</f>
+        <v>185</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="21">
+        <f>$O$4</f>
+        <v>0.33</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="3">
+        <f>$L$4</f>
+        <v>185</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
+      <c r="I15" s="21">
+        <f>$O$4</f>
+        <v>0.33</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="L15" s="3">
+        <f>$L$4</f>
+        <v>185</v>
+      </c>
+      <c r="M15" s="3">
+        <v>0</v>
+      </c>
+      <c r="N15" s="21">
+        <f>$O$4</f>
+        <v>0.33</v>
+      </c>
+      <c r="P15" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q15" s="3">
+        <f>$L$4</f>
+        <v>185</v>
+      </c>
+      <c r="R15" s="3">
+        <v>0</v>
+      </c>
+      <c r="S15" s="21">
+        <f>$O$4</f>
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="3">
+        <f>$L$2*6</f>
+        <v>1252.8000000000002</v>
+      </c>
+      <c r="C16" s="3">
+        <f>$M$2*6</f>
+        <v>78.300000000000011</v>
+      </c>
+      <c r="D16" s="21">
+        <f>$O$2*6</f>
+        <v>1.32</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="3">
+        <f>$L$2*6</f>
+        <v>1252.8000000000002</v>
+      </c>
+      <c r="H16" s="3">
+        <f>$M$2*6</f>
+        <v>78.300000000000011</v>
+      </c>
+      <c r="I16" s="21">
+        <f>$O$2*6</f>
+        <v>1.32</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="L16" s="3">
+        <f>$L$2*7</f>
+        <v>1461.6000000000001</v>
+      </c>
+      <c r="M16" s="3">
+        <f>$M$2*7</f>
+        <v>91.350000000000009</v>
+      </c>
+      <c r="N16" s="21">
+        <f>$O$2*7</f>
+        <v>1.54</v>
+      </c>
+      <c r="P16" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q16" s="3">
+        <f>$L$2*7</f>
+        <v>1461.6000000000001</v>
+      </c>
+      <c r="R16" s="3">
+        <f>$M$2*7</f>
+        <v>91.350000000000009</v>
+      </c>
+      <c r="S16" s="21">
+        <f>$O$2*7</f>
+        <v>1.54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="3">
+        <f>$L$3*2</f>
+        <v>246</v>
+      </c>
+      <c r="C17" s="3">
+        <f>$M$3*2</f>
+        <v>60</v>
+      </c>
+      <c r="D17" s="21">
+        <f>$O$3*2</f>
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="G17" s="3">
+        <f>$L$3*2</f>
+        <v>246</v>
+      </c>
+      <c r="H17" s="3">
+        <f>$M$3*2</f>
+        <v>60</v>
+      </c>
+      <c r="I17" s="21">
+        <f>$O$3*2</f>
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="K17" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="L17" s="3">
+        <f>$L$3*2</f>
+        <v>246</v>
+      </c>
+      <c r="M17" s="3">
+        <f>$M$3*2</f>
+        <v>60</v>
+      </c>
+      <c r="N17" s="21">
+        <f>$O$3*2</f>
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="P17" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q17" s="3">
+        <f>$L$3*2</f>
+        <v>246</v>
+      </c>
+      <c r="R17" s="3">
+        <f>$M$3*2</f>
+        <v>60</v>
+      </c>
+      <c r="S17" s="21">
+        <f>$O$3*2</f>
+        <v>2.1800000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="3">
+        <f>$L$5</f>
+        <v>257</v>
+      </c>
+      <c r="C18" s="3">
+        <f>$M$5</f>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D18" s="21">
+        <f>$O$5</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" s="3">
+        <f>$L$5</f>
+        <v>257</v>
+      </c>
+      <c r="H18" s="3">
+        <f>$M$5</f>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="I18" s="21">
+        <f>$O$5</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="K18" s="15"/>
+      <c r="L18" s="3">
+        <v>0</v>
+      </c>
+      <c r="M18" s="3">
+        <v>0</v>
+      </c>
+      <c r="N18" s="21">
+        <v>0</v>
+      </c>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="3">
+        <v>0</v>
+      </c>
+      <c r="R18" s="3">
+        <v>0</v>
+      </c>
+      <c r="S18" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="3">
+        <f>SUM(B15:B18)</f>
+        <v>1940.8000000000002</v>
+      </c>
+      <c r="C19" s="3">
+        <f>SUM(C15:C18)</f>
+        <v>147.5</v>
+      </c>
+      <c r="D19" s="21">
+        <f>SUM(D15:D18)</f>
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="G19" s="3">
+        <f>SUM(G15:G18)</f>
+        <v>1940.8000000000002</v>
+      </c>
+      <c r="H19" s="3">
+        <f>SUM(H15:H18)</f>
+        <v>147.5</v>
+      </c>
+      <c r="I19" s="21">
+        <f>SUM(I15:I18)</f>
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="K19" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="L19" s="3">
+        <f>SUM(L15:L18)</f>
+        <v>1892.6000000000001</v>
+      </c>
+      <c r="M19" s="3">
+        <f>SUM(M15:M18)</f>
+        <v>151.35000000000002</v>
+      </c>
+      <c r="N19" s="21">
+        <f>SUM(N15:N18)</f>
+        <v>4.0500000000000007</v>
+      </c>
+      <c r="P19" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q19" s="3">
+        <f>SUM(Q15:Q18)</f>
+        <v>1892.6000000000001</v>
+      </c>
+      <c r="R19" s="3">
+        <f>SUM(R15:R18)</f>
+        <v>151.35000000000002</v>
+      </c>
+      <c r="S19" s="21">
+        <f>SUM(S15:S18)</f>
+        <v>4.0500000000000007</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P20" s="22"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="K21" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="L21" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M21" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="N21" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="3">
+        <f>$L$4</f>
+        <v>185</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
+      <c r="D22" s="21">
+        <f>$O$4</f>
+        <v>0.33</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" s="3">
+        <f>$L$4</f>
+        <v>185</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0</v>
+      </c>
+      <c r="I22" s="21">
+        <f>$O$4</f>
+        <v>0.33</v>
+      </c>
+      <c r="K22" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="L22" s="3">
+        <f>$L$4</f>
+        <v>185</v>
+      </c>
+      <c r="M22" s="3">
+        <v>0</v>
+      </c>
+      <c r="N22" s="21">
+        <f>$O$4</f>
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="3">
+        <f>$L$2*8</f>
+        <v>1670.4</v>
+      </c>
+      <c r="C23" s="3">
+        <f>$M$2*8</f>
+        <v>104.4</v>
+      </c>
+      <c r="D23" s="21">
+        <f>$O$2*8</f>
+        <v>1.76</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="3">
+        <f>$L$2*6</f>
+        <v>1252.8000000000002</v>
+      </c>
+      <c r="H23" s="3">
+        <f>$M$2*6</f>
+        <v>78.300000000000011</v>
+      </c>
+      <c r="I23" s="21">
+        <f>$O$2*6</f>
+        <v>1.32</v>
+      </c>
+      <c r="K23" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="L23" s="3">
+        <f>$L$2*7</f>
+        <v>1461.6000000000001</v>
+      </c>
+      <c r="M23" s="3">
+        <f>$M$2*7</f>
+        <v>91.350000000000009</v>
+      </c>
+      <c r="N23" s="21">
+        <f>$O$2*7</f>
+        <v>1.54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="3">
+        <f>$L$3*2</f>
+        <v>246</v>
+      </c>
+      <c r="C24" s="3">
+        <f>$M$3*2</f>
+        <v>60</v>
+      </c>
+      <c r="D24" s="21">
+        <f>$O$3*2</f>
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="G24" s="3">
+        <f>$L$3*2</f>
+        <v>246</v>
+      </c>
+      <c r="H24" s="3">
+        <f>$M$3*2</f>
+        <v>60</v>
+      </c>
+      <c r="I24" s="21">
+        <f>$O$3*2</f>
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="K24" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="L24" s="3">
+        <f>$L$3*2</f>
+        <v>246</v>
+      </c>
+      <c r="M24" s="3">
+        <f>$M$3*2</f>
+        <v>60</v>
+      </c>
+      <c r="N24" s="21">
+        <f>$O$3*2</f>
+        <v>2.1800000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" s="15"/>
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="21">
+        <v>0</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="G25" s="3">
+        <f>$L$5</f>
+        <v>257</v>
+      </c>
+      <c r="H25" s="3">
+        <f>$M$5</f>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="I25" s="21">
+        <f>$O$5</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="K25" s="15"/>
+      <c r="L25" s="3">
+        <v>0</v>
+      </c>
+      <c r="M25" s="3">
+        <v>0</v>
+      </c>
+      <c r="N25" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="3">
+        <f>SUM(B22:B25)</f>
+        <v>2101.4</v>
+      </c>
+      <c r="C26" s="3">
+        <f>SUM(C22:C25)</f>
+        <v>164.4</v>
+      </c>
+      <c r="D26" s="21">
+        <f>SUM(D22:D25)</f>
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="G26" s="3">
+        <f>SUM(G22:G25)</f>
+        <v>1940.8000000000002</v>
+      </c>
+      <c r="H26" s="3">
+        <f>SUM(H22:H25)</f>
+        <v>147.5</v>
+      </c>
+      <c r="I26" s="21">
+        <f>SUM(I22:I25)</f>
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="K26" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="L26" s="3">
+        <f>SUM(L22:L25)</f>
+        <v>1892.6000000000001</v>
+      </c>
+      <c r="M26" s="3">
+        <f>SUM(M22:M25)</f>
+        <v>151.35000000000002</v>
+      </c>
+      <c r="N26" s="21">
+        <f>SUM(N22:N25)</f>
+        <v>4.0500000000000007</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="C3" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated latex documents and food document
</commit_message>
<xml_diff>
--- a/extra/studio cibi proteici.xlsx
+++ b/extra/studio cibi proteici.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Documents\uni\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D573CF68-9FF0-4B87-B09D-A2EDE22199CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B5E3E7E-1510-4CEB-B616-7D2932CBA09E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
     <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
+    <sheet name="Foglio3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="86">
   <si>
     <t>proteine</t>
   </si>
@@ -277,6 +278,21 @@
   </si>
   <si>
     <t>media euro</t>
+  </si>
+  <si>
+    <t>100g di popcorn</t>
+  </si>
+  <si>
+    <t>3 scatolette di tonno</t>
+  </si>
+  <si>
+    <t>pro</t>
+  </si>
+  <si>
+    <t>1 wurstel penny</t>
+  </si>
+  <si>
+    <t>4 etti di pasta smart</t>
   </si>
 </sst>
 </file>
@@ -449,7 +465,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -473,6 +489,17 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -2205,10 +2232,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{619C59B3-5361-4003-B0C2-E8CD91BFF358}">
-  <dimension ref="A1:S26"/>
+  <dimension ref="A1:X26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W16" sqref="W16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W32" sqref="W32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2216,9 +2243,12 @@
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" customWidth="1"/>
     <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="21" max="21" width="22.42578125" customWidth="1"/>
+    <col min="23" max="23" width="12.42578125" customWidth="1"/>
+    <col min="24" max="24" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="K1" s="15"/>
       <c r="L1" s="15" t="s">
         <v>1</v>
@@ -2232,8 +2262,12 @@
       <c r="O1" s="15" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="26"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>53</v>
       </c>
@@ -2274,7 +2308,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
@@ -2319,8 +2353,11 @@
       <c r="O3" s="20">
         <v>1.0900000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="V3" s="28"/>
+      <c r="W3" s="28"/>
+      <c r="X3" s="28"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>0</v>
       </c>
@@ -2364,7 +2401,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>40</v>
       </c>
@@ -2412,34 +2449,47 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="K6" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="L6" s="24">
+        <v>371</v>
+      </c>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="25">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="23">
         <f>AVERAGE(B3:H3)</f>
         <v>1943.0857142857144</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="23">
         <f t="shared" ref="B8:B9" si="0">AVERAGE(B4:H4)</f>
         <v>151.56428571428572</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="20">
         <f t="shared" si="0"/>
         <v>4.1071428571428568</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>69</v>
       </c>
@@ -2489,7 +2539,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>63</v>
       </c>
@@ -2547,7 +2597,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>65</v>
       </c>
@@ -3055,4 +3105,98 @@
     <ignoredError sqref="C3" formula="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F24F6A85-44F0-41EA-9C90-606DC79AD939}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2">
+        <f>123*3</f>
+        <v>369</v>
+      </c>
+      <c r="C2">
+        <f>30*3</f>
+        <v>90</v>
+      </c>
+      <c r="D2" s="29">
+        <f>1.09*3</f>
+        <v>3.2700000000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3">
+        <f>350*4</f>
+        <v>1400</v>
+      </c>
+      <c r="C3">
+        <f>11.5*4</f>
+        <v>46</v>
+      </c>
+      <c r="D3" s="29">
+        <f>0.13*4</f>
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4">
+        <f>209*1</f>
+        <v>209</v>
+      </c>
+      <c r="C4">
+        <f>13*1</f>
+        <v>13</v>
+      </c>
+      <c r="D4" s="29">
+        <f>0.22*1</f>
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <f>SUM(B2:B4)</f>
+        <v>1978</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:D5" si="0">SUM(C2:C4)</f>
+        <v>149</v>
+      </c>
+      <c r="D5" s="29">
+        <f t="shared" si="0"/>
+        <v>4.0100000000000007</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
bookmark and added es bookmark
</commit_message>
<xml_diff>
--- a/extra/studio cibi proteici.xlsx
+++ b/extra/studio cibi proteici.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Documents\uni\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78402063-9222-4481-A591-58ECD9A6A57F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBE15B1-92F8-4229-8CF8-138A0890CFD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,20 +25,52 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tommaso bertelli</author>
+  </authors>
+  <commentList>
+    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{4367CB62-7F9A-4AEB-9578-71F4155BADE4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>tommaso bertelli:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Interessonte
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="109">
   <si>
     <t>proteine</t>
   </si>
@@ -350,6 +382,21 @@
   </si>
   <si>
     <t>6 wurstel penny</t>
+  </si>
+  <si>
+    <t>banana (check peso)</t>
+  </si>
+  <si>
+    <t>1 banana</t>
+  </si>
+  <si>
+    <t>2 wurstel penny</t>
+  </si>
+  <si>
+    <t>130g prot veg myp abb</t>
+  </si>
+  <si>
+    <t>max 100 cal di bonus</t>
   </si>
 </sst>
 </file>
@@ -360,7 +407,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-410]_-;\-* #,##0.00\ [$€-410]_-;_-* &quot;-&quot;??\ [$€-410]_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -380,6 +427,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -522,7 +582,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -558,6 +618,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1067,19 +1130,19 @@
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="8" max="8" width="33.33203125" customWidth="1"/>
+    <col min="8" max="8" width="33.28515625" customWidth="1"/>
     <col min="13" max="13" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -1099,7 +1162,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -1139,7 +1202,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -1185,7 +1248,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -1234,7 +1297,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
@@ -1283,7 +1346,7 @@
         <v>1.6559999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>24</v>
       </c>
@@ -1332,7 +1395,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
@@ -1380,7 +1443,7 @@
         <v>4.5860000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
@@ -1402,7 +1465,7 @@
         <v>1.6877637130801688</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -1424,7 +1487,7 @@
         <v>2.8235294117647061</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
@@ -1464,7 +1527,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
@@ -1511,7 +1574,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
@@ -1563,7 +1626,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>21</v>
       </c>
@@ -1615,7 +1678,7 @@
         <v>1.6559999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>20</v>
       </c>
@@ -1656,7 +1719,7 @@
         <v>2.0205000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>5</v>
       </c>
@@ -1703,7 +1766,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>9</v>
       </c>
@@ -1738,7 +1801,7 @@
         <v>5.5164999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>10</v>
       </c>
@@ -1760,7 +1823,7 @@
         <v>3.7593984962406015</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>26</v>
       </c>
@@ -1782,7 +1845,7 @@
         <v>1.8950437317784257</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>28</v>
       </c>
@@ -1822,7 +1885,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
@@ -1870,7 +1933,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>27</v>
       </c>
@@ -1922,7 +1985,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>25</v>
       </c>
@@ -1974,7 +2037,7 @@
         <v>1.6559999999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>19</v>
       </c>
@@ -2015,7 +2078,7 @@
         <v>0.28299999999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>16</v>
       </c>
@@ -2054,7 +2117,7 @@
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>29</v>
       </c>
@@ -2089,7 +2152,7 @@
         <v>4.4490000000000007</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>86</v>
       </c>
@@ -2111,7 +2174,7 @@
         <v>3.1153846153846154</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D27" s="1"/>
       <c r="E27" s="2"/>
       <c r="J27" s="15" t="s">
@@ -2121,7 +2184,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
       <c r="E28" s="2"/>
       <c r="H28" t="s">
@@ -2146,7 +2209,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D29" s="1"/>
       <c r="E29" s="2"/>
       <c r="H29" t="s">
@@ -2175,7 +2238,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D30" s="1"/>
       <c r="E30" s="2"/>
       <c r="H30" t="s">
@@ -2208,7 +2271,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M31" s="15" t="s">
         <v>42</v>
       </c>
@@ -2225,7 +2288,7 @@
         <v>1.4407199999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M32" s="15" t="s">
         <v>41</v>
       </c>
@@ -2242,7 +2305,7 @@
         <v>0.28299999999999997</v>
       </c>
     </row>
-    <row r="33" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C33" s="1"/>
       <c r="D33" s="2"/>
       <c r="H33" t="s">
@@ -2253,7 +2316,7 @@
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
     </row>
-    <row r="34" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C34" s="1"/>
       <c r="D34" s="2"/>
       <c r="H34" t="s">
@@ -2273,27 +2336,27 @@
         <v>4.2337199999999999</v>
       </c>
     </row>
-    <row r="35" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
       <c r="H35" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E38" s="2"/>
     </row>
-    <row r="39" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E39" s="2"/>
     </row>
-    <row r="40" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E40" s="2"/>
     </row>
   </sheetData>
@@ -2314,17 +2377,17 @@
       <selection activeCell="K5" sqref="K5:O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" customWidth="1"/>
-    <col min="11" max="11" width="18.44140625" customWidth="1"/>
-    <col min="21" max="21" width="22.44140625" customWidth="1"/>
-    <col min="23" max="23" width="12.44140625" customWidth="1"/>
-    <col min="24" max="24" width="9.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="21" max="21" width="22.42578125" customWidth="1"/>
+    <col min="23" max="23" width="12.42578125" customWidth="1"/>
+    <col min="24" max="24" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="K1" s="15"/>
       <c r="L1" s="15" t="s">
         <v>1</v>
@@ -2343,7 +2406,7 @@
       <c r="W1" s="24"/>
       <c r="X1" s="23"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>53</v>
       </c>
@@ -2384,7 +2447,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
@@ -2433,7 +2496,7 @@
       <c r="W3" s="25"/>
       <c r="X3" s="25"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>0</v>
       </c>
@@ -2477,7 +2540,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>40</v>
       </c>
@@ -2525,7 +2588,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="K6" s="15" t="s">
         <v>81</v>
       </c>
@@ -2538,7 +2601,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>78</v>
       </c>
@@ -2547,7 +2610,7 @@
         <v>1943.0857142857144</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>79</v>
       </c>
@@ -2556,7 +2619,7 @@
         <v>151.56428571428572</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>80</v>
       </c>
@@ -2565,7 +2628,7 @@
         <v>4.1071428571428568</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>69</v>
       </c>
@@ -2615,7 +2678,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>63</v>
       </c>
@@ -2673,7 +2736,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>65</v>
       </c>
@@ -2735,7 +2798,7 @@
         <v>1.54</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>66</v>
       </c>
@@ -2797,7 +2860,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>67</v>
       </c>
@@ -2849,7 +2912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>70</v>
       </c>
@@ -2911,7 +2974,7 @@
         <v>4.0500000000000007</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>75</v>
       </c>
@@ -2949,7 +3012,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>63</v>
       </c>
@@ -2993,7 +3056,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>77</v>
       </c>
@@ -3040,7 +3103,7 @@
         <v>1.54</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>66</v>
       </c>
@@ -3087,7 +3150,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
       <c r="B25" s="3">
         <v>0</v>
@@ -3124,7 +3187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>70</v>
       </c>
@@ -3181,24 +3244,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F24F6A85-44F0-41EA-9C90-606DC79AD939}">
-  <dimension ref="A1:P22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F24F6A85-44F0-41EA-9C90-606DC79AD939}">
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.77734375" customWidth="1"/>
-    <col min="14" max="14" width="22.21875" customWidth="1"/>
-    <col min="15" max="15" width="9.88671875" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="14" max="14" width="22.28515625" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>45</v>
       </c>
@@ -3234,7 +3297,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -3280,7 +3343,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -3327,7 +3390,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -3353,29 +3416,29 @@
         <v>81</v>
       </c>
       <c r="I4" s="5">
-        <f t="shared" ref="I4" si="0">P3/25</f>
+        <f>P3/25</f>
         <v>1.6</v>
       </c>
       <c r="J4" s="3">
-        <f t="shared" ref="J4" si="1">H4/G4</f>
+        <f t="shared" ref="J4" si="0">H4/G4</f>
         <v>0.23823529411764705</v>
       </c>
       <c r="K4" s="30">
-        <f t="shared" ref="K4" si="2">H4/I4</f>
+        <f t="shared" ref="K4" si="1">H4/I4</f>
         <v>50.625</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5">
         <f>SUM(B2:B4)</f>
         <v>1978</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:D5" si="3">SUM(C2:C4)</f>
+        <f t="shared" ref="C5:D5" si="2">SUM(C2:C4)</f>
         <v>149</v>
       </c>
       <c r="D5" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>4.0100000000000007</v>
       </c>
       <c r="F5" s="15" t="s">
@@ -3391,7 +3454,7 @@
       <c r="J5" s="29"/>
       <c r="K5" s="28"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F6" s="15" t="s">
         <v>68</v>
       </c>
@@ -3401,12 +3464,12 @@
       <c r="H6" s="3">
         <v>9.1999999999999993</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="19">
         <v>0.28000000000000003</v>
       </c>
       <c r="J6" s="29"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>97</v>
       </c>
@@ -3419,8 +3482,20 @@
       <c r="D7" s="15" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F7" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="31">
+        <v>350</v>
+      </c>
+      <c r="H7" s="31">
+        <v>11.5</v>
+      </c>
+      <c r="I7" s="32">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>99</v>
       </c>
@@ -3436,8 +3511,20 @@
         <f>1.4*I4</f>
         <v>2.2399999999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F8" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="G8" s="31">
+        <v>75</v>
+      </c>
+      <c r="H8" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="I8" s="32">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>98</v>
       </c>
@@ -3454,7 +3541,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>70</v>
       </c>
@@ -3471,7 +3558,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>97</v>
       </c>
@@ -3485,7 +3572,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>101</v>
       </c>
@@ -3494,15 +3581,15 @@
         <v>272</v>
       </c>
       <c r="C13" s="21">
-        <f t="shared" ref="C13:D13" si="4">0.8*H4</f>
+        <f t="shared" ref="C13:D13" si="3">0.8*H4</f>
         <v>64.8</v>
       </c>
       <c r="D13" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.2800000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>100</v>
       </c>
@@ -3519,7 +3606,7 @@
         <v>1.54</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>70</v>
       </c>
@@ -3536,7 +3623,7 @@
         <v>2.8200000000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>97</v>
       </c>
@@ -3549,8 +3636,20 @@
       <c r="D17" s="15" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F17" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>101</v>
       </c>
@@ -3559,15 +3658,30 @@
         <v>272</v>
       </c>
       <c r="C18" s="21">
-        <f t="shared" ref="C18:D18" si="5">0.8*H4</f>
+        <f t="shared" ref="C18:D18" si="4">0.8*H4</f>
         <v>64.8</v>
       </c>
       <c r="D18" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.2800000000000002</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F18" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" s="21">
+        <f>1.3*$G$4</f>
+        <v>442</v>
+      </c>
+      <c r="H18" s="21">
+        <f>1.3*$H$4</f>
+        <v>105.3</v>
+      </c>
+      <c r="I18" s="5">
+        <f>1.3*$I$4</f>
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>103</v>
       </c>
@@ -3583,8 +3697,23 @@
         <f>0.22*6</f>
         <v>1.32</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F19" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="G19" s="3">
+        <f>209*2</f>
+        <v>418</v>
+      </c>
+      <c r="H19" s="3">
+        <f>13*2</f>
+        <v>26</v>
+      </c>
+      <c r="I19" s="4">
+        <f>0.22*2</f>
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>63</v>
       </c>
@@ -3599,8 +3728,22 @@
         <f>$I$5</f>
         <v>0.33</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F20" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" s="3">
+        <f>$G$5</f>
+        <v>185</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0</v>
+      </c>
+      <c r="I20" s="4">
+        <f>$I$5</f>
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>102</v>
       </c>
@@ -3616,8 +3759,23 @@
         <f>$I$6*1</f>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F21" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="G21" s="3">
+        <f>$G$6*1</f>
+        <v>257</v>
+      </c>
+      <c r="H21" s="3">
+        <f>$H$6*1</f>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="I21" s="4">
+        <f>$I$6*1</f>
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>70</v>
       </c>
@@ -3626,15 +3784,70 @@
         <v>1968</v>
       </c>
       <c r="C22" s="21">
-        <f t="shared" ref="C22:D22" si="6">SUM(C18:C21)</f>
+        <f t="shared" ref="C22:D22" si="5">SUM(C18:C21)</f>
         <v>152</v>
       </c>
       <c r="D22" s="5">
+        <f t="shared" si="5"/>
+        <v>3.2100000000000009</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="21">
+        <f>1*G7</f>
+        <v>350</v>
+      </c>
+      <c r="H22" s="21">
+        <f>1*H7</f>
+        <v>11.5</v>
+      </c>
+      <c r="I22" s="19">
+        <f>1*I7</f>
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F23" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="G23" s="21">
+        <f>1*G8</f>
+        <v>75</v>
+      </c>
+      <c r="H23" s="21">
+        <f t="shared" ref="H23:I23" si="6">1*H8</f>
+        <v>1.5</v>
+      </c>
+      <c r="I23" s="19">
         <f t="shared" si="6"/>
-        <v>3.2100000000000009</v>
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F24" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24" s="21">
+        <f>SUM(G18:G23)</f>
+        <v>1727</v>
+      </c>
+      <c r="H24" s="21">
+        <f>SUM(H18:H23)</f>
+        <v>153.5</v>
+      </c>
+      <c r="I24" s="19">
+        <f>SUM(I18:I23)</f>
+        <v>3.44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F26" s="33" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updates on food, and documents
</commit_message>
<xml_diff>
--- a/extra/studio cibi proteici.xlsx
+++ b/extra/studio cibi proteici.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Documents\uni\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AFB5502-2C30-4346-BD01-598713DE48CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622E6982-1F73-4FBD-BDEB-7C3CDEDC2B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="115">
   <si>
     <t>proteine</t>
   </si>
@@ -388,10 +388,25 @@
     <t>max 100 cal di bonus</t>
   </si>
   <si>
-    <t>4 wurstel penny</t>
-  </si>
-  <si>
     <t>100g di gnocchi smart</t>
+  </si>
+  <si>
+    <t>200g gnocchi smart</t>
+  </si>
+  <si>
+    <t>cena test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pro </t>
+  </si>
+  <si>
+    <t>100g pasta smart</t>
+  </si>
+  <si>
+    <t>100g yogurt bianco s</t>
+  </si>
+  <si>
+    <t>wurstel</t>
   </si>
 </sst>
 </file>
@@ -463,7 +478,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -582,13 +597,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -626,6 +650,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -1123,7 +1150,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1134,7 +1161,7 @@
   <dimension ref="A1:P40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3252,10 +3279,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F24F6A85-44F0-41EA-9C90-606DC79AD939}">
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3548,7 +3575,7 @@
         <v>0.66</v>
       </c>
       <c r="F9" s="32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G9" s="33">
         <v>174</v>
@@ -3576,6 +3603,48 @@
         <f>SUM(D8:D9)</f>
         <v>2.9</v>
       </c>
+      <c r="F10" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="G10" s="36">
+        <v>51</v>
+      </c>
+      <c r="H10" s="36">
+        <v>6</v>
+      </c>
+      <c r="I10" s="37">
+        <v>0.15</v>
+      </c>
+      <c r="J10">
+        <f>H10/G10</f>
+        <v>0.11764705882352941</v>
+      </c>
+      <c r="K10" s="2">
+        <f>H10/I10</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F11" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="G11" s="36">
+        <v>209</v>
+      </c>
+      <c r="H11" s="36">
+        <v>13</v>
+      </c>
+      <c r="I11" s="37">
+        <v>0.22</v>
+      </c>
+      <c r="J11">
+        <f>H11/G11</f>
+        <v>6.2200956937799042E-2</v>
+      </c>
+      <c r="K11" s="2">
+        <f>H11/I11</f>
+        <v>59.090909090909093</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
@@ -3642,7 +3711,7 @@
         <v>2.8200000000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>97</v>
       </c>
@@ -3667,8 +3736,9 @@
       <c r="I17" s="15" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K17" s="35"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>101</v>
       </c>
@@ -3700,7 +3770,7 @@
         <v>2.08</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>103</v>
       </c>
@@ -3717,22 +3787,22 @@
         <v>1.32</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="G19" s="3">
-        <f>209*4</f>
-        <v>836</v>
+        <f>209*3</f>
+        <v>627</v>
       </c>
       <c r="H19" s="3">
-        <f>13*4</f>
-        <v>52</v>
+        <f>13*3</f>
+        <v>39</v>
       </c>
       <c r="I19" s="4">
-        <f>0.22*4</f>
-        <v>0.88</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <f>0.22*3</f>
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>63</v>
       </c>
@@ -3762,7 +3832,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>102</v>
       </c>
@@ -3794,7 +3864,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>70</v>
       </c>
@@ -3815,7 +3885,7 @@
       <c r="H22" s="21"/>
       <c r="I22" s="19"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F23" s="15" t="s">
         <v>105</v>
       </c>
@@ -3832,26 +3902,68 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F24" s="15" t="s">
         <v>70</v>
       </c>
       <c r="G24" s="21">
         <f>SUM(G18:G23)</f>
-        <v>1795</v>
+        <v>1586</v>
       </c>
       <c r="H24" s="21">
         <f>SUM(H18:H23)</f>
-        <v>157.6</v>
+        <v>144.6</v>
       </c>
       <c r="I24" s="19">
         <f>SUM(I18:I23)</f>
-        <v>3.7500000000000004</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3.5300000000000007</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F26" s="31" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F28" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="I28" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F29" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="G29" s="3">
+        <v>348</v>
+      </c>
+      <c r="H29" s="3">
+        <v>9</v>
+      </c>
+      <c r="I29" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F30" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="G30" s="3">
+        <v>350</v>
+      </c>
+      <c r="H30" s="3">
+        <v>11.5</v>
+      </c>
+      <c r="I30" s="3">
+        <v>0.13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
am1 documents and food updates
</commit_message>
<xml_diff>
--- a/extra/studio cibi proteici.xlsx
+++ b/extra/studio cibi proteici.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Documents\uni\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622E6982-1F73-4FBD-BDEB-7C3CDEDC2B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E962A8CC-4001-47BC-8F66-C7286E828DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="128">
   <si>
     <t>proteine</t>
   </si>
@@ -382,9 +382,6 @@
     <t>1 banana</t>
   </si>
   <si>
-    <t>130g prot veg myp abb</t>
-  </si>
-  <si>
     <t>max 100 cal di bonus</t>
   </si>
   <si>
@@ -407,6 +404,48 @@
   </si>
   <si>
     <t>wurstel</t>
+  </si>
+  <si>
+    <t>merluzzo smart</t>
+  </si>
+  <si>
+    <t>100g petto di pollo esse</t>
+  </si>
+  <si>
+    <t>4 scoops</t>
+  </si>
+  <si>
+    <t>100ml latte esse</t>
+  </si>
+  <si>
+    <t>70g prot veg myp abb</t>
+  </si>
+  <si>
+    <t>500ml latte esse</t>
+  </si>
+  <si>
+    <t>1 scatoletta di tonno</t>
+  </si>
+  <si>
+    <t>100g uova smart</t>
+  </si>
+  <si>
+    <t>2 wurstel penny</t>
+  </si>
+  <si>
+    <t>105g prot veg myp abb</t>
+  </si>
+  <si>
+    <t>3 scoops</t>
+  </si>
+  <si>
+    <t>750ml latte esse</t>
+  </si>
+  <si>
+    <t>4scoops</t>
+  </si>
+  <si>
+    <t>1L latte esse</t>
   </si>
 </sst>
 </file>
@@ -590,19 +629,17 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -612,7 +649,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -645,16 +682,14 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1150,7 +1185,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1161,7 +1196,7 @@
   <dimension ref="A1:P40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2408,7 +2443,7 @@
   <dimension ref="A1:X26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:O5"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3279,10 +3314,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F24F6A85-44F0-41EA-9C90-606DC79AD939}">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:V40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3293,6 +3328,7 @@
     <col min="6" max="6" width="21.28515625" customWidth="1"/>
     <col min="14" max="14" width="22.28515625" customWidth="1"/>
     <col min="15" max="15" width="9.85546875" customWidth="1"/>
+    <col min="19" max="19" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -3359,7 +3395,7 @@
       <c r="I2" s="4">
         <v>1.0900000000000001</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="21">
         <f>H2/G2</f>
         <v>0.24390243902439024</v>
       </c>
@@ -3406,7 +3442,7 @@
         <f>P2/25</f>
         <v>2.6</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="21">
         <f>H3/G3</f>
         <v>0.23823529411764705</v>
       </c>
@@ -3453,12 +3489,12 @@
         <f>P3/25</f>
         <v>1.6</v>
       </c>
-      <c r="J4" s="3">
-        <f t="shared" ref="J4" si="0">H4/G4</f>
+      <c r="J4" s="21">
+        <f t="shared" ref="J4:J9" si="0">H4/G4</f>
         <v>0.21470588235294116</v>
       </c>
-      <c r="K4" s="30">
-        <f t="shared" ref="K4" si="1">H4/I4</f>
+      <c r="K4" s="28">
+        <f t="shared" ref="K4:K9" si="1">H4/I4</f>
         <v>45.625</v>
       </c>
     </row>
@@ -3485,8 +3521,14 @@
       <c r="I5" s="5">
         <v>0.33</v>
       </c>
-      <c r="J5" s="29"/>
-      <c r="K5" s="28"/>
+      <c r="J5" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K5" s="28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F6" s="15" t="s">
@@ -3501,7 +3543,14 @@
       <c r="I6" s="19">
         <v>0.28000000000000003</v>
       </c>
-      <c r="J6" s="29"/>
+      <c r="J6" s="21">
+        <f t="shared" si="0"/>
+        <v>3.5797665369649803E-2</v>
+      </c>
+      <c r="K6" s="28">
+        <f t="shared" si="1"/>
+        <v>32.857142857142854</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
@@ -3528,6 +3577,14 @@
       <c r="I7" s="5">
         <v>0.13</v>
       </c>
+      <c r="J7" s="21">
+        <f t="shared" si="0"/>
+        <v>3.2857142857142856E-2</v>
+      </c>
+      <c r="K7" s="28">
+        <f t="shared" si="1"/>
+        <v>88.461538461538453</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
@@ -3557,6 +3614,14 @@
       <c r="I8" s="5">
         <v>0.18</v>
       </c>
+      <c r="J8" s="21">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="K8" s="28">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333339</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
@@ -3574,17 +3639,25 @@
         <f>0.22*3</f>
         <v>0.66</v>
       </c>
-      <c r="F9" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="G9" s="33">
+      <c r="F9" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" s="3">
         <v>174</v>
       </c>
-      <c r="H9" s="33">
+      <c r="H9" s="3">
         <v>4.5</v>
       </c>
-      <c r="I9" s="34">
+      <c r="I9" s="5">
         <v>0.1</v>
+      </c>
+      <c r="J9" s="21">
+        <f t="shared" si="0"/>
+        <v>2.5862068965517241E-2</v>
+      </c>
+      <c r="K9" s="28">
+        <f t="shared" si="1"/>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -3603,46 +3676,46 @@
         <f>SUM(D8:D9)</f>
         <v>2.9</v>
       </c>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="G10" s="3">
+        <v>51</v>
+      </c>
+      <c r="H10" s="3">
+        <v>5.3</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="J10" s="21">
+        <f t="shared" ref="J10:J16" si="3">H10/G10</f>
+        <v>0.10392156862745097</v>
+      </c>
+      <c r="K10" s="21">
+        <f t="shared" ref="K10:K16" si="4">H10/I10</f>
+        <v>35.333333333333336</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F11" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="G10" s="36">
-        <v>51</v>
-      </c>
-      <c r="H10" s="36">
-        <v>6</v>
-      </c>
-      <c r="I10" s="37">
-        <v>0.15</v>
-      </c>
-      <c r="J10">
-        <f>H10/G10</f>
-        <v>0.11764705882352941</v>
-      </c>
-      <c r="K10" s="2">
-        <f>H10/I10</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F11" s="32" t="s">
-        <v>114</v>
-      </c>
-      <c r="G11" s="36">
+      <c r="G11" s="3">
         <v>209</v>
       </c>
-      <c r="H11" s="36">
+      <c r="H11" s="3">
         <v>13</v>
       </c>
-      <c r="I11" s="37">
+      <c r="I11" s="5">
         <v>0.22</v>
       </c>
-      <c r="J11">
-        <f>H11/G11</f>
+      <c r="J11" s="21">
+        <f t="shared" si="3"/>
         <v>6.2200956937799042E-2</v>
       </c>
-      <c r="K11" s="2">
-        <f>H11/I11</f>
+      <c r="K11" s="21">
+        <f t="shared" si="4"/>
         <v>59.090909090909093</v>
       </c>
     </row>
@@ -3659,6 +3732,26 @@
       <c r="D12" s="15" t="s">
         <v>40</v>
       </c>
+      <c r="F12" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="G12" s="3">
+        <v>84</v>
+      </c>
+      <c r="H12" s="3">
+        <v>16.7</v>
+      </c>
+      <c r="I12" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="J12" s="21">
+        <f t="shared" si="3"/>
+        <v>0.1988095238095238</v>
+      </c>
+      <c r="K12" s="21">
+        <f t="shared" si="4"/>
+        <v>20.874999999999996</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
@@ -3669,12 +3762,32 @@
         <v>272</v>
       </c>
       <c r="C13" s="21">
-        <f t="shared" ref="C13:D13" si="3">0.8*H4</f>
+        <f t="shared" ref="C13:D13" si="5">0.8*H4</f>
         <v>58.400000000000006</v>
       </c>
       <c r="D13" s="5">
+        <f t="shared" si="5"/>
+        <v>1.2800000000000002</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="G13" s="3">
+        <v>129</v>
+      </c>
+      <c r="H13" s="3">
+        <v>30</v>
+      </c>
+      <c r="I13" s="5">
+        <v>1.03</v>
+      </c>
+      <c r="J13" s="21">
         <f t="shared" si="3"/>
-        <v>1.2800000000000002</v>
+        <v>0.23255813953488372</v>
+      </c>
+      <c r="K13" s="21">
+        <f t="shared" si="4"/>
+        <v>29.126213592233007</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -3693,6 +3806,26 @@
         <f>0.22*7</f>
         <v>1.54</v>
       </c>
+      <c r="F14" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="G14" s="3">
+        <v>47</v>
+      </c>
+      <c r="H14" s="3">
+        <v>3.3</v>
+      </c>
+      <c r="I14" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="J14" s="21">
+        <f t="shared" si="3"/>
+        <v>7.0212765957446799E-2</v>
+      </c>
+      <c r="K14" s="21">
+        <f t="shared" si="4"/>
+        <v>32.999999999999993</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
@@ -3710,8 +3843,36 @@
         <f>SUM(D13:D14)</f>
         <v>2.8200000000000003</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F15" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="G15" s="11">
+        <v>136</v>
+      </c>
+      <c r="H15" s="11">
+        <v>12.4</v>
+      </c>
+      <c r="I15" s="12">
+        <v>0.49</v>
+      </c>
+      <c r="J15" s="32">
+        <f t="shared" si="3"/>
+        <v>9.1176470588235303E-2</v>
+      </c>
+      <c r="K15" s="32">
+        <f t="shared" si="4"/>
+        <v>25.306122448979593</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="35"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>97</v>
       </c>
@@ -3724,21 +3885,8 @@
       <c r="D17" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="F17" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H17" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="I17" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="K17" s="35"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>101</v>
       </c>
@@ -3747,30 +3895,15 @@
         <v>272</v>
       </c>
       <c r="C18" s="21">
-        <f t="shared" ref="C18:D18" si="4">0.8*H4</f>
+        <f t="shared" ref="C18:D18" si="6">0.8*H4</f>
         <v>58.400000000000006</v>
       </c>
       <c r="D18" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.2800000000000002</v>
       </c>
-      <c r="F18" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="G18" s="21">
-        <f>1.3*$G$4</f>
-        <v>442</v>
-      </c>
-      <c r="H18" s="21">
-        <f>1.3*$H$4</f>
-        <v>94.9</v>
-      </c>
-      <c r="I18" s="5">
-        <f>1.3*$I$4</f>
-        <v>2.08</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>103</v>
       </c>
@@ -3786,23 +3919,8 @@
         <f>0.22*6</f>
         <v>1.32</v>
       </c>
-      <c r="F19" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="G19" s="3">
-        <f>209*3</f>
-        <v>627</v>
-      </c>
-      <c r="H19" s="3">
-        <f>13*3</f>
-        <v>39</v>
-      </c>
-      <c r="I19" s="4">
-        <f>0.22*3</f>
-        <v>0.66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>63</v>
       </c>
@@ -3817,22 +3935,8 @@
         <f>$I$5</f>
         <v>0.33</v>
       </c>
-      <c r="F20" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G20" s="3">
-        <f>$G$5</f>
-        <v>185</v>
-      </c>
-      <c r="H20" s="3">
-        <v>0</v>
-      </c>
-      <c r="I20" s="4">
-        <f>$I$5</f>
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>102</v>
       </c>
@@ -3848,23 +3952,11 @@
         <f>$I$6*1</f>
         <v>0.28000000000000003</v>
       </c>
-      <c r="F21" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="G21" s="3">
-        <f>$G$6*1</f>
-        <v>257</v>
-      </c>
-      <c r="H21" s="3">
-        <f>$H$6*1</f>
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="I21" s="4">
-        <f>$I$6*1</f>
-        <v>0.28000000000000003</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="S21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>70</v>
       </c>
@@ -3873,101 +3965,547 @@
         <v>1968</v>
       </c>
       <c r="C22" s="21">
-        <f t="shared" ref="C22:D22" si="5">SUM(C18:C21)</f>
+        <f t="shared" ref="C22:D22" si="7">SUM(C18:C21)</f>
         <v>145.6</v>
       </c>
       <c r="D22" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.2100000000000009</v>
       </c>
-      <c r="F22" s="15"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="19"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F22" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="I22" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="K22" s="30"/>
+      <c r="N22" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="O22" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="P22" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q22" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="S22" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="T22" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="U22" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="V22" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F23" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="G23" s="21">
+        <f>1.4*$G$4</f>
+        <v>475.99999999999994</v>
+      </c>
+      <c r="H23" s="21">
+        <f>1.4*$H$4</f>
+        <v>102.19999999999999</v>
+      </c>
+      <c r="I23" s="5">
+        <f>1.4*$I$4</f>
+        <v>2.2399999999999998</v>
+      </c>
+      <c r="J23" t="s">
+        <v>116</v>
+      </c>
+      <c r="N23" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="O23" s="21">
+        <f>0.7*$G$4</f>
+        <v>237.99999999999997</v>
+      </c>
+      <c r="P23" s="21">
+        <f>0.7*$H$4</f>
+        <v>51.099999999999994</v>
+      </c>
+      <c r="Q23" s="19">
+        <f>0.7*$I$4</f>
+        <v>1.1199999999999999</v>
+      </c>
+      <c r="S23" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="T23" s="21">
+        <f>1.05*$G$4</f>
+        <v>357</v>
+      </c>
+      <c r="U23" s="21">
+        <f>1.05*$H$4</f>
+        <v>76.650000000000006</v>
+      </c>
+      <c r="V23" s="19">
+        <f>1.05*$I$4</f>
+        <v>1.6800000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F24" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="G24" s="3">
+        <f>209*3</f>
+        <v>627</v>
+      </c>
+      <c r="H24" s="3">
+        <f>13*3</f>
+        <v>39</v>
+      </c>
+      <c r="I24" s="4">
+        <f>0.22*3</f>
+        <v>0.66</v>
+      </c>
+      <c r="N24" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="O24" s="3">
+        <f>47*5</f>
+        <v>235</v>
+      </c>
+      <c r="P24" s="3">
+        <f>3.3*5</f>
+        <v>16.5</v>
+      </c>
+      <c r="Q24" s="19">
+        <f>0.1*5</f>
+        <v>0.5</v>
+      </c>
+      <c r="S24" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="T24" s="3">
+        <f>47*7.5</f>
+        <v>352.5</v>
+      </c>
+      <c r="U24" s="3">
+        <f>3.3*7.5</f>
+        <v>24.75</v>
+      </c>
+      <c r="V24" s="19">
+        <f>0.1*7.5</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F25" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" s="3">
+        <f>$G$5</f>
+        <v>185</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0</v>
+      </c>
+      <c r="I25" s="4">
+        <f>$I$5</f>
+        <v>0.33</v>
+      </c>
+      <c r="N25" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="O25" s="3">
+        <f>123*1</f>
+        <v>123</v>
+      </c>
+      <c r="P25" s="3">
+        <f>30*1</f>
+        <v>30</v>
+      </c>
+      <c r="Q25" s="19">
+        <f>1.09*1</f>
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="S25" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="T25" s="3">
+        <f>209*2</f>
+        <v>418</v>
+      </c>
+      <c r="U25" s="3">
+        <f>13*2</f>
+        <v>26</v>
+      </c>
+      <c r="V25" s="19">
+        <f>0.22*2</f>
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F26" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="G26" s="3">
+        <f>$G$6*1</f>
+        <v>257</v>
+      </c>
+      <c r="H26" s="3">
+        <f>$H$6*1</f>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="I26" s="4">
+        <f>$I$6*1</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="N26" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="O26" s="3">
+        <f>209*3</f>
+        <v>627</v>
+      </c>
+      <c r="P26" s="3">
+        <f>13*3</f>
+        <v>39</v>
+      </c>
+      <c r="Q26" s="19">
+        <f>0.22*3</f>
+        <v>0.66</v>
+      </c>
+      <c r="S26" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="T26" s="3">
+        <f>$G$6*1</f>
+        <v>257</v>
+      </c>
+      <c r="U26" s="3">
+        <f>$H$6*1</f>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="V26" s="19">
+        <f>$I$6*1</f>
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F27" s="15"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="19"/>
+      <c r="N27" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="O27" s="3">
+        <f>$G$6*1</f>
+        <v>257</v>
+      </c>
+      <c r="P27" s="3">
+        <f>$H$6*1</f>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="Q27" s="19">
+        <f>$I$6*1</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="S27" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="T27" s="3">
+        <v>350</v>
+      </c>
+      <c r="U27" s="3">
+        <v>11.5</v>
+      </c>
+      <c r="V27" s="19">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F28" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="G23" s="21">
+      <c r="G28" s="21">
         <f>1*G8</f>
         <v>75</v>
       </c>
-      <c r="H23" s="21">
-        <f t="shared" ref="H23:I23" si="6">1*H8</f>
+      <c r="H28" s="21">
+        <f>1*H8</f>
         <v>1.5</v>
       </c>
-      <c r="I23" s="19">
-        <f t="shared" si="6"/>
+      <c r="I28" s="19">
+        <f>1*I8</f>
         <v>0.18</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F24" s="15" t="s">
+      <c r="N28" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="O28" s="3">
+        <v>350</v>
+      </c>
+      <c r="P28" s="3">
+        <v>11.5</v>
+      </c>
+      <c r="Q28" s="19">
+        <v>0.13</v>
+      </c>
+      <c r="S28" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="T28" s="3">
+        <f>1*51</f>
+        <v>51</v>
+      </c>
+      <c r="U28" s="3">
+        <f>1*5.3</f>
+        <v>5.3</v>
+      </c>
+      <c r="V28" s="4">
+        <f>1*0.15</f>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F29" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="G24" s="21">
-        <f>SUM(G18:G23)</f>
-        <v>1586</v>
-      </c>
-      <c r="H24" s="21">
-        <f>SUM(H18:H23)</f>
-        <v>144.6</v>
-      </c>
-      <c r="I24" s="19">
-        <f>SUM(I18:I23)</f>
-        <v>3.5300000000000007</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F26" s="31" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F28" s="15" t="s">
+      <c r="G29" s="21">
+        <f>SUM(G23:G28)</f>
+        <v>1620</v>
+      </c>
+      <c r="H29" s="21">
+        <f>SUM(H23:H28)</f>
+        <v>151.89999999999998</v>
+      </c>
+      <c r="I29" s="19">
+        <f>SUM(I23:I28)</f>
+        <v>3.69</v>
+      </c>
+      <c r="N29" s="15"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="19"/>
+      <c r="S29" s="15"/>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+      <c r="V29" s="19"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="N30" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="O30" s="21">
+        <f>SUM(O23:O28)</f>
+        <v>1830</v>
+      </c>
+      <c r="P30" s="21">
+        <f>SUM(P23:P28)</f>
+        <v>157.29999999999998</v>
+      </c>
+      <c r="Q30" s="19">
+        <f>SUM(Q23:Q28)</f>
+        <v>3.7800000000000002</v>
+      </c>
+      <c r="S30" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="T30" s="21">
+        <f>SUM(T23:T29)</f>
+        <v>1785.5</v>
+      </c>
+      <c r="U30" s="21">
+        <f t="shared" ref="U30:V30" si="8">SUM(U23:U29)</f>
+        <v>153.4</v>
+      </c>
+      <c r="V30" s="19">
+        <f t="shared" si="8"/>
+        <v>3.43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F31" s="29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="N32" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="O32" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="P32" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q32" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F33" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="G33" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H33" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="G28" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H28" s="15" t="s">
+      <c r="I33" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="M33" t="s">
+        <v>126</v>
+      </c>
+      <c r="N33" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="O33" s="21">
+        <f>1.4*$G$4</f>
+        <v>475.99999999999994</v>
+      </c>
+      <c r="P33" s="21">
+        <f>1.4*$H$4</f>
+        <v>102.19999999999999</v>
+      </c>
+      <c r="Q33" s="19">
+        <f>1.4*$I$4</f>
+        <v>2.2399999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F34" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="G34" s="3">
+        <v>348</v>
+      </c>
+      <c r="H34" s="3">
+        <v>9</v>
+      </c>
+      <c r="I34" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="N34" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="O34" s="3">
+        <f>47*10</f>
+        <v>470</v>
+      </c>
+      <c r="P34" s="3">
+        <f>3.3*10</f>
+        <v>33</v>
+      </c>
+      <c r="Q34" s="19">
+        <f>0.1*10</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F35" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="I28" s="15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F29" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="G29" s="3">
-        <v>348</v>
-      </c>
-      <c r="H29" s="3">
-        <v>9</v>
-      </c>
-      <c r="I29" s="3">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F30" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="G30" s="3">
+      <c r="G35" s="3">
         <v>350</v>
       </c>
-      <c r="H30" s="3">
+      <c r="H35" s="3">
         <v>11.5</v>
       </c>
-      <c r="I30" s="3">
+      <c r="I35" s="3">
         <v>0.13</v>
+      </c>
+      <c r="N35" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="O35" s="3">
+        <f>209*2</f>
+        <v>418</v>
+      </c>
+      <c r="P35" s="3">
+        <f>13*2</f>
+        <v>26</v>
+      </c>
+      <c r="Q35" s="19">
+        <f>0.22*2</f>
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="36" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="N36" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="O36" s="3">
+        <f>$G$6*1</f>
+        <v>257</v>
+      </c>
+      <c r="P36" s="3">
+        <f>$H$6*1</f>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="Q36" s="19">
+        <f>$I$6*1</f>
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="N37" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="O37" s="3">
+        <v>350</v>
+      </c>
+      <c r="P37" s="3">
+        <v>11.5</v>
+      </c>
+      <c r="Q37" s="19">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="38" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="N38" s="15"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="4"/>
+    </row>
+    <row r="39" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="N39" s="15"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="19"/>
+    </row>
+    <row r="40" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="N40" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="O40" s="21">
+        <f>SUM(O33:O39)</f>
+        <v>1971</v>
+      </c>
+      <c r="P40" s="21">
+        <f t="shared" ref="P40:Q40" si="9">SUM(P33:P39)</f>
+        <v>181.89999999999998</v>
+      </c>
+      <c r="Q40" s="19">
+        <f t="shared" si="9"/>
+        <v>4.09</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
food update and added gal documents
</commit_message>
<xml_diff>
--- a/extra/studio cibi proteici.xlsx
+++ b/extra/studio cibi proteici.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Documents\uni\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E962A8CC-4001-47BC-8F66-C7286E828DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B60387-C89E-4C5B-AE7D-278EDBC2C2FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
   </bookViews>
@@ -21,6 +21,14 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -62,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="140">
   <si>
     <t>proteine</t>
   </si>
@@ -346,9 +354,6 @@
     <t>vegan blend</t>
   </si>
   <si>
-    <t>vegan blend abbonamento</t>
-  </si>
-  <si>
     <t>100g prot veg myp</t>
   </si>
   <si>
@@ -446,6 +451,45 @@
   </si>
   <si>
     <t>1L latte esse</t>
+  </si>
+  <si>
+    <t>vegan blend abb</t>
+  </si>
+  <si>
+    <t>confronto proteine</t>
+  </si>
+  <si>
+    <t>veg fragola</t>
+  </si>
+  <si>
+    <t>veg no gusto</t>
+  </si>
+  <si>
+    <t>whey mirtillo lampone</t>
+  </si>
+  <si>
+    <t>whey no gusto</t>
+  </si>
+  <si>
+    <t>100g</t>
+  </si>
+  <si>
+    <t>2 scoops</t>
+  </si>
+  <si>
+    <t>70g prot whey no g</t>
+  </si>
+  <si>
+    <t>250g yogurt bianco s</t>
+  </si>
+  <si>
+    <t>cena</t>
+  </si>
+  <si>
+    <t>tot</t>
+  </si>
+  <si>
+    <t>50g pane</t>
   </si>
 </sst>
 </file>
@@ -517,7 +561,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -643,13 +687,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -687,9 +742,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -3314,10 +3373,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F24F6A85-44F0-41EA-9C90-606DC79AD939}">
-  <dimension ref="A1:V40"/>
+  <dimension ref="A1:V49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
+      <selection activeCell="X43" sqref="X43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3329,9 +3388,10 @@
     <col min="14" max="14" width="22.28515625" customWidth="1"/>
     <col min="15" max="15" width="9.85546875" customWidth="1"/>
     <col min="19" max="19" width="21.28515625" customWidth="1"/>
+    <col min="20" max="20" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>45</v>
       </c>
@@ -3357,17 +3417,17 @@
       <c r="K1" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="15" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -3403,17 +3463,17 @@
         <f>H2/I2</f>
         <v>27.52293577981651</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="3">
         <v>2.5</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="3">
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -3430,7 +3490,7 @@
         <v>0.52</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G3" s="3">
         <v>340</v>
@@ -3450,17 +3510,17 @@
         <f>H3/I3</f>
         <v>31.153846153846153</v>
       </c>
-      <c r="N3" t="s">
-        <v>94</v>
-      </c>
-      <c r="O3">
+      <c r="N3" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="O3" s="3">
         <v>2.5</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="3">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -3477,10 +3537,10 @@
         <v>0.22</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G4" s="3">
-        <v>340</v>
+        <v>366</v>
       </c>
       <c r="H4" s="3">
         <v>73</v>
@@ -3490,15 +3550,24 @@
         <v>1.6</v>
       </c>
       <c r="J4" s="21">
-        <f t="shared" ref="J4:J9" si="0">H4/G4</f>
-        <v>0.21470588235294116</v>
+        <f t="shared" ref="J4" si="0">H4/G4</f>
+        <v>0.19945355191256831</v>
       </c>
       <c r="K4" s="28">
-        <f t="shared" ref="K4:K9" si="1">H4/I4</f>
+        <f t="shared" ref="K4" si="1">H4/I4</f>
         <v>45.625</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N4" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="O4" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="P4" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B5">
         <f>SUM(B2:B4)</f>
         <v>1978</v>
@@ -3522,15 +3591,24 @@
         <v>0.33</v>
       </c>
       <c r="J5" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="J5:J15" si="3">H5/G5</f>
         <v>0</v>
       </c>
       <c r="K5" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="K5:K15" si="4">H5/I5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N5" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="O5" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="P5" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F6" s="15" t="s">
         <v>68</v>
       </c>
@@ -3544,17 +3622,26 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="J6" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3.5797665369649803E-2</v>
       </c>
       <c r="K6" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>32.857142857142854</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N6" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="O6" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="P6" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>45</v>
@@ -3578,21 +3665,21 @@
         <v>0.13</v>
       </c>
       <c r="J7" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3.2857142857142856E-2</v>
       </c>
       <c r="K7" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>88.461538461538453</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" s="3">
         <f>1.4*G4</f>
-        <v>475.99999999999994</v>
+        <v>512.4</v>
       </c>
       <c r="C8" s="3">
         <f>1.4*H4</f>
@@ -3603,7 +3690,7 @@
         <v>2.2399999999999998</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G8" s="3">
         <v>75</v>
@@ -3615,17 +3702,38 @@
         <v>0.18</v>
       </c>
       <c r="J8" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.02</v>
       </c>
       <c r="K8" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>8.3333333333333339</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M8" t="s">
+        <v>133</v>
+      </c>
+      <c r="N8" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="O8" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="P8" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q8" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="R8" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="S8" s="15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B9" s="3">
         <f>209*3</f>
@@ -3640,7 +3748,7 @@
         <v>0.66</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G9" s="3">
         <v>174</v>
@@ -3652,21 +3760,42 @@
         <v>0.1</v>
       </c>
       <c r="J9" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2.5862068965517241E-2</v>
       </c>
       <c r="K9" s="28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N9" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="O9" s="3">
+        <v>366</v>
+      </c>
+      <c r="P9" s="3">
+        <v>73</v>
+      </c>
+      <c r="Q9" s="3">
+        <f>P3/(O3*10)</f>
+        <v>1.6</v>
+      </c>
+      <c r="R9" s="36">
+        <f>P9/O9</f>
+        <v>0.19945355191256831</v>
+      </c>
+      <c r="S9" s="19">
+        <f>P9/Q9</f>
+        <v>45.625</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>70</v>
       </c>
       <c r="B10" s="3">
         <f>SUM(B8:B9)</f>
-        <v>1103</v>
+        <v>1139.4000000000001</v>
       </c>
       <c r="C10" s="3">
         <f>SUM(C8:C9)</f>
@@ -3677,7 +3806,7 @@
         <v>2.9</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G10" s="3">
         <v>51</v>
@@ -3689,17 +3818,38 @@
         <v>0.15</v>
       </c>
       <c r="J10" s="21">
-        <f t="shared" ref="J10:J16" si="3">H10/G10</f>
+        <f t="shared" si="3"/>
         <v>0.10392156862745097</v>
       </c>
       <c r="K10" s="21">
-        <f t="shared" ref="K10:K16" si="4">H10/I10</f>
+        <f t="shared" si="4"/>
         <v>35.333333333333336</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N10" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="O10" s="3">
+        <v>340</v>
+      </c>
+      <c r="P10" s="3">
+        <v>81</v>
+      </c>
+      <c r="Q10" s="3">
+        <f t="shared" ref="Q10:Q12" si="5">P4/(O4*10)</f>
+        <v>1.6</v>
+      </c>
+      <c r="R10" s="36">
+        <f t="shared" ref="R10:R12" si="6">P10/O10</f>
+        <v>0.23823529411764705</v>
+      </c>
+      <c r="S10" s="19">
+        <f t="shared" ref="S10:S12" si="7">P10/Q10</f>
+        <v>50.625</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F11" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G11" s="3">
         <v>209</v>
@@ -3718,10 +3868,31 @@
         <f t="shared" si="4"/>
         <v>59.090909090909093</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N11" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="O11" s="3">
+        <v>366</v>
+      </c>
+      <c r="P11" s="3">
+        <v>73</v>
+      </c>
+      <c r="Q11" s="3">
+        <f t="shared" si="5"/>
+        <v>2.36</v>
+      </c>
+      <c r="R11" s="36">
+        <f t="shared" si="6"/>
+        <v>0.19945355191256831</v>
+      </c>
+      <c r="S11" s="19">
+        <f t="shared" si="7"/>
+        <v>30.932203389830509</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>45</v>
@@ -3733,7 +3904,7 @@
         <v>40</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G12" s="3">
         <v>84</v>
@@ -3752,25 +3923,46 @@
         <f t="shared" si="4"/>
         <v>20.874999999999996</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N12" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="O12" s="3">
+        <v>412</v>
+      </c>
+      <c r="P12" s="3">
+        <v>82</v>
+      </c>
+      <c r="Q12" s="3">
+        <f t="shared" si="5"/>
+        <v>2.36</v>
+      </c>
+      <c r="R12" s="36">
+        <f t="shared" si="6"/>
+        <v>0.19902912621359223</v>
+      </c>
+      <c r="S12" s="19">
+        <f t="shared" si="7"/>
+        <v>34.745762711864408</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B13" s="21">
         <f>0.8*G4</f>
-        <v>272</v>
+        <v>292.8</v>
       </c>
       <c r="C13" s="21">
-        <f t="shared" ref="C13:D13" si="5">0.8*H4</f>
+        <f t="shared" ref="C13:D13" si="8">0.8*H4</f>
         <v>58.400000000000006</v>
       </c>
       <c r="D13" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.2800000000000002</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G13" s="3">
         <v>129</v>
@@ -3790,9 +3982,9 @@
         <v>29.126213592233007</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B14" s="3">
         <f>209*7</f>
@@ -3807,7 +3999,7 @@
         <v>1.54</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G14" s="3">
         <v>47</v>
@@ -3827,13 +4019,13 @@
         <v>32.999999999999993</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>70</v>
       </c>
       <c r="B15" s="3">
         <f>SUM(B13:B14)</f>
-        <v>1735</v>
+        <v>1755.8</v>
       </c>
       <c r="C15" s="3">
         <f>SUM(C13:C14)</f>
@@ -3844,7 +4036,7 @@
         <v>2.8200000000000003</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G15" s="11">
         <v>136</v>
@@ -3864,7 +4056,7 @@
         <v>25.306122448979593</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F16" s="33"/>
       <c r="G16" s="33"/>
       <c r="H16" s="33"/>
@@ -3874,7 +4066,7 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>45</v>
@@ -3888,24 +4080,24 @@
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B18" s="21">
         <f>0.8*G4</f>
-        <v>272</v>
+        <v>292.8</v>
       </c>
       <c r="C18" s="21">
-        <f t="shared" ref="C18:D18" si="6">0.8*H4</f>
+        <f t="shared" ref="C18:D18" si="9">0.8*H4</f>
         <v>58.400000000000006</v>
       </c>
       <c r="D18" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.2800000000000002</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B19" s="3">
         <f>209*6</f>
@@ -3938,7 +4130,7 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B21" s="3">
         <f>$G$6*1</f>
@@ -3953,7 +4145,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="S21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
@@ -3962,18 +4154,18 @@
       </c>
       <c r="B22" s="21">
         <f>SUM(B18:B21)</f>
-        <v>1968</v>
+        <v>1988.8</v>
       </c>
       <c r="C22" s="21">
-        <f t="shared" ref="C22:D22" si="7">SUM(C18:C21)</f>
+        <f t="shared" ref="C22:D22" si="10">SUM(C18:C21)</f>
         <v>145.6</v>
       </c>
       <c r="D22" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>3.2100000000000009</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G22" s="15" t="s">
         <v>45</v>
@@ -3986,7 +4178,7 @@
       </c>
       <c r="K22" s="30"/>
       <c r="N22" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="O22" s="15" t="s">
         <v>45</v>
@@ -3998,7 +4190,7 @@
         <v>40</v>
       </c>
       <c r="S22" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="T22" s="15" t="s">
         <v>45</v>
@@ -4012,11 +4204,11 @@
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F23" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G23" s="21">
         <f>1.4*$G$4</f>
-        <v>475.99999999999994</v>
+        <v>512.4</v>
       </c>
       <c r="H23" s="21">
         <f>1.4*$H$4</f>
@@ -4027,14 +4219,14 @@
         <v>2.2399999999999998</v>
       </c>
       <c r="J23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N23" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="O23" s="21">
         <f>0.7*$G$4</f>
-        <v>237.99999999999997</v>
+        <v>256.2</v>
       </c>
       <c r="P23" s="21">
         <f>0.7*$H$4</f>
@@ -4045,11 +4237,11 @@
         <v>1.1199999999999999</v>
       </c>
       <c r="S23" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="T23" s="21">
         <f>1.05*$G$4</f>
-        <v>357</v>
+        <v>384.3</v>
       </c>
       <c r="U23" s="21">
         <f>1.05*$H$4</f>
@@ -4062,7 +4254,7 @@
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F24" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G24" s="3">
         <f>209*3</f>
@@ -4077,7 +4269,7 @@
         <v>0.66</v>
       </c>
       <c r="N24" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O24" s="3">
         <f>47*5</f>
@@ -4092,7 +4284,7 @@
         <v>0.5</v>
       </c>
       <c r="S24" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="T24" s="3">
         <f>47*7.5</f>
@@ -4123,7 +4315,7 @@
         <v>0.33</v>
       </c>
       <c r="N25" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O25" s="3">
         <f>123*1</f>
@@ -4138,7 +4330,7 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="S25" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="T25" s="3">
         <f>209*2</f>
@@ -4155,7 +4347,7 @@
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F26" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G26" s="3">
         <f>$G$6*1</f>
@@ -4170,7 +4362,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="N26" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="O26" s="3">
         <f>209*3</f>
@@ -4185,7 +4377,7 @@
         <v>0.66</v>
       </c>
       <c r="S26" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="T26" s="3">
         <f>$G$6*1</f>
@@ -4206,7 +4398,7 @@
       <c r="H27" s="21"/>
       <c r="I27" s="19"/>
       <c r="N27" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O27" s="3">
         <f>$G$6*1</f>
@@ -4221,7 +4413,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="S27" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="T27" s="3">
         <v>350</v>
@@ -4235,7 +4427,7 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F28" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G28" s="21">
         <f>1*G8</f>
@@ -4250,7 +4442,7 @@
         <v>0.18</v>
       </c>
       <c r="N28" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O28" s="3">
         <v>350</v>
@@ -4262,7 +4454,7 @@
         <v>0.13</v>
       </c>
       <c r="S28" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="T28" s="3">
         <f>1*51</f>
@@ -4283,7 +4475,7 @@
       </c>
       <c r="G29" s="21">
         <f>SUM(G23:G28)</f>
-        <v>1620</v>
+        <v>1656.4</v>
       </c>
       <c r="H29" s="21">
         <f>SUM(H23:H28)</f>
@@ -4308,7 +4500,7 @@
       </c>
       <c r="O30" s="21">
         <f>SUM(O23:O28)</f>
-        <v>1830</v>
+        <v>1848.2</v>
       </c>
       <c r="P30" s="21">
         <f>SUM(P23:P28)</f>
@@ -4323,25 +4515,25 @@
       </c>
       <c r="T30" s="21">
         <f>SUM(T23:T29)</f>
-        <v>1785.5</v>
+        <v>1812.8</v>
       </c>
       <c r="U30" s="21">
-        <f t="shared" ref="U30:V30" si="8">SUM(U23:U29)</f>
+        <f t="shared" ref="U30:V30" si="11">SUM(U23:U29)</f>
         <v>153.4</v>
       </c>
       <c r="V30" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>3.43</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F31" s="29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="N32" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="O32" s="15" t="s">
         <v>45</v>
@@ -4352,29 +4544,41 @@
       <c r="Q32" s="15" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="33" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="S32" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="T32" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="U32" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="V32" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F33" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G33" s="15" t="s">
         <v>45</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I33" s="15" t="s">
         <v>40</v>
       </c>
       <c r="M33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N33" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="O33" s="21">
         <f>1.4*$G$4</f>
-        <v>475.99999999999994</v>
+        <v>512.4</v>
       </c>
       <c r="P33" s="21">
         <f>1.4*$H$4</f>
@@ -4384,10 +4588,28 @@
         <f>1.4*$I$4</f>
         <v>2.2399999999999998</v>
       </c>
-    </row>
-    <row r="34" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="R33" t="s">
+        <v>134</v>
+      </c>
+      <c r="S33" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="T33" s="3">
+        <f>O12*0.7</f>
+        <v>288.39999999999998</v>
+      </c>
+      <c r="U33" s="3">
+        <f t="shared" ref="U33:V33" si="12">P12*0.7</f>
+        <v>57.4</v>
+      </c>
+      <c r="V33" s="19">
+        <f t="shared" si="12"/>
+        <v>1.6519999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F34" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G34" s="3">
         <v>348</v>
@@ -4399,7 +4621,7 @@
         <v>0.2</v>
       </c>
       <c r="N34" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O34" s="3">
         <f>47*10</f>
@@ -4413,10 +4635,25 @@
         <f>0.1*10</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="S34" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="T34" s="3">
+        <f>47*5</f>
+        <v>235</v>
+      </c>
+      <c r="U34" s="3">
+        <f>3.3*5</f>
+        <v>16.5</v>
+      </c>
+      <c r="V34" s="19">
+        <f>0.1*5</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="35" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F35" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G35" s="3">
         <v>350</v>
@@ -4428,7 +4665,7 @@
         <v>0.13</v>
       </c>
       <c r="N35" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O35" s="3">
         <f>209*2</f>
@@ -4442,10 +4679,25 @@
         <f>0.22*2</f>
         <v>0.44</v>
       </c>
-    </row>
-    <row r="36" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="S35" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="T35" s="3">
+        <f>209*3</f>
+        <v>627</v>
+      </c>
+      <c r="U35" s="3">
+        <f>13*3</f>
+        <v>39</v>
+      </c>
+      <c r="V35" s="19">
+        <f>0.22*3</f>
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="36" spans="6:22" x14ac:dyDescent="0.25">
       <c r="N36" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O36" s="3">
         <f>$G$6*1</f>
@@ -4459,10 +4711,25 @@
         <f>$I$6*1</f>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="37" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="S36" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="T36" s="3">
+        <f>$G$6*1</f>
+        <v>257</v>
+      </c>
+      <c r="U36" s="3">
+        <f>$H$6*1</f>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="V36" s="19">
+        <f>$I$6*1</f>
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="6:22" x14ac:dyDescent="0.25">
       <c r="N37" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O37" s="3">
         <v>350</v>
@@ -4473,34 +4740,188 @@
       <c r="Q37" s="19">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="38" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="S37" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="T37" s="3">
+        <f>51*2.5</f>
+        <v>127.5</v>
+      </c>
+      <c r="U37" s="3">
+        <f>5.3*2.5</f>
+        <v>13.25</v>
+      </c>
+      <c r="V37" s="5">
+        <f>0.15*2.5</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="38" spans="6:22" x14ac:dyDescent="0.25">
       <c r="N38" s="15"/>
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
       <c r="Q38" s="4"/>
-    </row>
-    <row r="39" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="S38" s="15"/>
+      <c r="T38" s="3"/>
+      <c r="U38" s="3"/>
+      <c r="V38" s="19"/>
+    </row>
+    <row r="39" spans="6:22" x14ac:dyDescent="0.25">
       <c r="N39" s="15"/>
       <c r="O39" s="3"/>
       <c r="P39" s="3"/>
       <c r="Q39" s="19"/>
-    </row>
-    <row r="40" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="S39" s="15"/>
+      <c r="T39" s="3"/>
+      <c r="U39" s="3"/>
+      <c r="V39" s="19"/>
+    </row>
+    <row r="40" spans="6:22" x14ac:dyDescent="0.25">
       <c r="N40" s="15" t="s">
         <v>70</v>
       </c>
       <c r="O40" s="21">
         <f>SUM(O33:O39)</f>
-        <v>1971</v>
+        <v>2007.4</v>
       </c>
       <c r="P40" s="21">
-        <f t="shared" ref="P40:Q40" si="9">SUM(P33:P39)</f>
+        <f t="shared" ref="P40:Q40" si="13">SUM(P33:P39)</f>
         <v>181.89999999999998</v>
       </c>
       <c r="Q40" s="19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>4.09</v>
+      </c>
+      <c r="S40" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="T40" s="3">
+        <f>SUM(T33:T39)</f>
+        <v>1534.9</v>
+      </c>
+      <c r="U40" s="3">
+        <f t="shared" ref="U40:V40" si="14">SUM(U33:U39)</f>
+        <v>135.35000000000002</v>
+      </c>
+      <c r="V40" s="19">
+        <f t="shared" si="14"/>
+        <v>3.4670000000000005</v>
+      </c>
+    </row>
+    <row r="41" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="S41" s="37"/>
+    </row>
+    <row r="42" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="S42" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="T42" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="U42" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="V42" s="38" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="S43" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="T43" s="39">
+        <f>209*2</f>
+        <v>418</v>
+      </c>
+      <c r="U43" s="39">
+        <f>13*2</f>
+        <v>26</v>
+      </c>
+      <c r="V43" s="19">
+        <f>0.22*2</f>
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="44" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="S44" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="T44" s="39">
+        <f>T40+T43</f>
+        <v>1952.9</v>
+      </c>
+      <c r="U44" s="39">
+        <f t="shared" ref="U44:V44" si="15">U40+U43</f>
+        <v>161.35000000000002</v>
+      </c>
+      <c r="V44" s="39">
+        <f t="shared" si="15"/>
+        <v>3.9070000000000005</v>
+      </c>
+    </row>
+    <row r="46" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="S46" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="T46" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="U46" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="V46" s="38" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="S47" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="T47" s="39">
+        <f>209*1</f>
+        <v>209</v>
+      </c>
+      <c r="U47" s="39">
+        <f>13*1</f>
+        <v>13</v>
+      </c>
+      <c r="V47" s="19">
+        <f>0.22*1</f>
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="48" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="S48" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="T48" s="3">
+        <f>$G$6*0.5</f>
+        <v>128.5</v>
+      </c>
+      <c r="U48" s="3">
+        <f>$H$6*0.5</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="V48" s="4">
+        <f>$I$6*0.5</f>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="19:22" x14ac:dyDescent="0.25">
+      <c r="S49" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="T49" s="39">
+        <f>T40+SUM(T47:T48)</f>
+        <v>1872.4</v>
+      </c>
+      <c r="U49" s="39">
+        <f t="shared" ref="U49:V49" si="16">U40+SUM(U47:U48)</f>
+        <v>152.95000000000002</v>
+      </c>
+      <c r="V49" s="19">
+        <f t="shared" si="16"/>
+        <v>3.8270000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added second semester documents
</commit_message>
<xml_diff>
--- a/extra/studio cibi proteici.xlsx
+++ b/extra/studio cibi proteici.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Documents\uni\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B60387-C89E-4C5B-AE7D-278EDBC2C2FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B97F458-2D64-49C3-B92A-1EA3BB4537DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
   </bookViews>
@@ -21,14 +21,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -70,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="148">
   <si>
     <t>proteine</t>
   </si>
@@ -490,6 +482,30 @@
   </si>
   <si>
     <t>50g pane</t>
+  </si>
+  <si>
+    <t>temporaneo</t>
+  </si>
+  <si>
+    <t>2 scat tonno</t>
+  </si>
+  <si>
+    <t>500g yogurt bianco s</t>
+  </si>
+  <si>
+    <t>4,5 wurstel penny</t>
+  </si>
+  <si>
+    <t>4 wurstel smart maxi</t>
+  </si>
+  <si>
+    <t>1 wurstel smart maxi</t>
+  </si>
+  <si>
+    <t>2 wurstel smart maxi</t>
+  </si>
+  <si>
+    <t>sistemare</t>
   </si>
 </sst>
 </file>
@@ -704,7 +720,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -746,9 +762,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -3373,10 +3387,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F24F6A85-44F0-41EA-9C90-606DC79AD939}">
-  <dimension ref="A1:V49"/>
+  <dimension ref="A1:V58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
-      <selection activeCell="X43" sqref="X43"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4300,6 +4314,18 @@
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>40</v>
+      </c>
       <c r="F25" s="15" t="s">
         <v>63</v>
       </c>
@@ -4346,6 +4372,21 @@
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" s="3">
+        <f>$G$6*1</f>
+        <v>257</v>
+      </c>
+      <c r="C26" s="3">
+        <f>$H$6*1</f>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D26" s="19">
+        <f>$I$6*1</f>
+        <v>0.28000000000000003</v>
+      </c>
       <c r="F26" s="15" t="s">
         <v>101</v>
       </c>
@@ -4393,6 +4434,20 @@
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="3">
+        <f>$G$5</f>
+        <v>185</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0</v>
+      </c>
+      <c r="D27" s="19">
+        <f>$I$5</f>
+        <v>0.33</v>
+      </c>
       <c r="F27" s="15"/>
       <c r="G27" s="21"/>
       <c r="H27" s="21"/>
@@ -4426,6 +4481,21 @@
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" s="3">
+        <f>123*2</f>
+        <v>246</v>
+      </c>
+      <c r="C28" s="3">
+        <f>30*2</f>
+        <v>60</v>
+      </c>
+      <c r="D28" s="22">
+        <f>1.09*2</f>
+        <v>2.1800000000000002</v>
+      </c>
       <c r="F28" s="15" t="s">
         <v>104</v>
       </c>
@@ -4470,6 +4540,21 @@
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B29" s="3">
+        <f>209*4.5</f>
+        <v>940.5</v>
+      </c>
+      <c r="C29" s="3">
+        <f>13*4.5</f>
+        <v>58.5</v>
+      </c>
+      <c r="D29" s="19">
+        <f>0.22*4.5</f>
+        <v>0.99</v>
+      </c>
       <c r="F29" s="15" t="s">
         <v>70</v>
       </c>
@@ -4495,6 +4580,21 @@
       <c r="V29" s="19"/>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="B30" s="3">
+        <f>51*5</f>
+        <v>255</v>
+      </c>
+      <c r="C30" s="3">
+        <f>5.3*5</f>
+        <v>26.5</v>
+      </c>
+      <c r="D30" s="19">
+        <f>0.15*5</f>
+        <v>0.75</v>
+      </c>
       <c r="N30" s="15" t="s">
         <v>70</v>
       </c>
@@ -4527,11 +4627,30 @@
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31" s="15"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
       <c r="F31" s="29" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="B32" s="3">
+        <f>SUM(B26:B31)</f>
+        <v>1883.5</v>
+      </c>
+      <c r="C32" s="3">
+        <f>SUM(C26:C31)</f>
+        <v>154.19999999999999</v>
+      </c>
+      <c r="D32" s="19">
+        <f>SUM(D26:D31)</f>
+        <v>4.53</v>
+      </c>
       <c r="N32" s="15" t="s">
         <v>96</v>
       </c>
@@ -4557,7 +4676,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F33" s="15" t="s">
         <v>108</v>
       </c>
@@ -4595,19 +4714,19 @@
         <v>135</v>
       </c>
       <c r="T33" s="3">
-        <f>O12*0.7</f>
+        <f>$O$12*0.7</f>
         <v>288.39999999999998</v>
       </c>
       <c r="U33" s="3">
-        <f t="shared" ref="U33:V33" si="12">P12*0.7</f>
+        <f>$P$12*0.7</f>
         <v>57.4</v>
       </c>
       <c r="V33" s="19">
-        <f t="shared" si="12"/>
+        <f>$Q$12*0.7</f>
         <v>1.6519999999999999</v>
       </c>
     </row>
-    <row r="34" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F34" s="15" t="s">
         <v>107</v>
       </c>
@@ -4651,7 +4770,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F35" s="15" t="s">
         <v>110</v>
       </c>
@@ -4695,7 +4814,19 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="36" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>40</v>
+      </c>
       <c r="N36" s="15" t="s">
         <v>101</v>
       </c>
@@ -4727,7 +4858,22 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="37" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B37" s="3">
+        <f>$G$6*1</f>
+        <v>257</v>
+      </c>
+      <c r="C37" s="3">
+        <f>$H$6*1</f>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D37" s="19">
+        <f>$I$6*1</f>
+        <v>0.28000000000000003</v>
+      </c>
       <c r="N37" s="15" t="s">
         <v>110</v>
       </c>
@@ -4756,7 +4902,21 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="38" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A38" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="3">
+        <f>$G$5</f>
+        <v>185</v>
+      </c>
+      <c r="C38" s="3">
+        <v>0</v>
+      </c>
+      <c r="D38" s="19">
+        <f>$I$5</f>
+        <v>0.33</v>
+      </c>
       <c r="N38" s="15"/>
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
@@ -4766,7 +4926,22 @@
       <c r="U38" s="3"/>
       <c r="V38" s="19"/>
     </row>
-    <row r="39" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A39" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B39" s="3">
+        <f>123*2</f>
+        <v>246</v>
+      </c>
+      <c r="C39" s="3">
+        <f>30*2</f>
+        <v>60</v>
+      </c>
+      <c r="D39" s="22">
+        <f>1.09*2</f>
+        <v>2.1800000000000002</v>
+      </c>
       <c r="N39" s="15"/>
       <c r="O39" s="3"/>
       <c r="P39" s="3"/>
@@ -4776,7 +4951,22 @@
       <c r="U39" s="3"/>
       <c r="V39" s="19"/>
     </row>
-    <row r="40" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A40" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="B40" s="3">
+        <f>240*4</f>
+        <v>960</v>
+      </c>
+      <c r="C40" s="3">
+        <f>15*4</f>
+        <v>60</v>
+      </c>
+      <c r="D40" s="19">
+        <f>0.26*4</f>
+        <v>1.04</v>
+      </c>
       <c r="N40" s="15" t="s">
         <v>70</v>
       </c>
@@ -4785,11 +4975,11 @@
         <v>2007.4</v>
       </c>
       <c r="P40" s="21">
-        <f t="shared" ref="P40:Q40" si="13">SUM(P33:P39)</f>
+        <f t="shared" ref="P40:Q40" si="12">SUM(P33:P39)</f>
         <v>181.89999999999998</v>
       </c>
       <c r="Q40" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>4.09</v>
       </c>
       <c r="S40" s="15" t="s">
@@ -4800,40 +4990,74 @@
         <v>1534.9</v>
       </c>
       <c r="U40" s="3">
-        <f t="shared" ref="U40:V40" si="14">SUM(U33:U39)</f>
+        <f t="shared" ref="U40:V40" si="13">SUM(U33:U39)</f>
         <v>135.35000000000002</v>
       </c>
       <c r="V40" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>3.4670000000000005</v>
       </c>
     </row>
-    <row r="41" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A41" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="B41" s="3">
+        <f>51*5</f>
+        <v>255</v>
+      </c>
+      <c r="C41" s="3">
+        <f>5.3*5</f>
+        <v>26.5</v>
+      </c>
+      <c r="D41" s="19">
+        <f>0.15*5</f>
+        <v>0.75</v>
+      </c>
       <c r="S41" s="37"/>
     </row>
-    <row r="42" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="S42" s="38" t="s">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A42" s="15"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="S42" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="T42" s="38" t="s">
+      <c r="T42" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="U42" s="38" t="s">
+      <c r="U42" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="V42" s="38" t="s">
+      <c r="V42" s="15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="S43" s="38" t="s">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A43" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="B43" s="3">
+        <f>SUM(B37:B42)</f>
+        <v>1903</v>
+      </c>
+      <c r="C43" s="3">
+        <f>SUM(C37:C42)</f>
+        <v>155.69999999999999</v>
+      </c>
+      <c r="D43" s="19">
+        <f>SUM(D37:D42)</f>
+        <v>4.58</v>
+      </c>
+      <c r="S43" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="T43" s="39">
+      <c r="T43" s="3">
         <f>209*2</f>
         <v>418</v>
       </c>
-      <c r="U43" s="39">
+      <c r="U43" s="3">
         <f>13*2</f>
         <v>26</v>
       </c>
@@ -4842,46 +5066,93 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="44" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="S44" s="38" t="s">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S44" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="T44" s="39">
+      <c r="T44" s="3">
         <f>T40+T43</f>
         <v>1952.9</v>
       </c>
-      <c r="U44" s="39">
-        <f t="shared" ref="U44:V44" si="15">U40+U43</f>
+      <c r="U44" s="3">
+        <f t="shared" ref="U44:V44" si="14">U40+U43</f>
         <v>161.35000000000002</v>
       </c>
-      <c r="V44" s="39">
-        <f t="shared" si="15"/>
+      <c r="V44" s="3">
+        <f t="shared" si="14"/>
         <v>3.9070000000000005</v>
       </c>
     </row>
-    <row r="46" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="S46" s="38" t="s">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A45" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A46" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B46" s="3">
+        <f>$O$12*0.7</f>
+        <v>288.39999999999998</v>
+      </c>
+      <c r="C46" s="3">
+        <f>$P$12*0.7</f>
+        <v>57.4</v>
+      </c>
+      <c r="D46" s="19">
+        <f>$Q$12*0.7</f>
+        <v>1.6519999999999999</v>
+      </c>
+      <c r="S46" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="T46" s="38" t="s">
+      <c r="T46" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="U46" s="38" t="s">
+      <c r="U46" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="V46" s="38" t="s">
+      <c r="V46" s="15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="47" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="S47" s="38" t="s">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A47" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B47" s="3">
+        <f>47*5</f>
+        <v>235</v>
+      </c>
+      <c r="C47" s="3">
+        <f>3.3*5</f>
+        <v>16.5</v>
+      </c>
+      <c r="D47" s="19">
+        <f>0.1*5</f>
+        <v>0.5</v>
+      </c>
+      <c r="F47" t="s">
+        <v>147</v>
+      </c>
+      <c r="S47" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="T47" s="39">
+      <c r="T47" s="3">
         <f>209*1</f>
         <v>209</v>
       </c>
-      <c r="U47" s="39">
+      <c r="U47" s="3">
         <f>13*1</f>
         <v>13</v>
       </c>
@@ -4890,7 +5161,22 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="48" spans="6:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A48" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="B48" s="3">
+        <f>240*2</f>
+        <v>480</v>
+      </c>
+      <c r="C48" s="3">
+        <f>15*2</f>
+        <v>30</v>
+      </c>
+      <c r="D48" s="19">
+        <f>0.26*2</f>
+        <v>0.52</v>
+      </c>
       <c r="S48" s="15" t="s">
         <v>139</v>
       </c>
@@ -4907,21 +5193,147 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="49" spans="19:22" x14ac:dyDescent="0.25">
-      <c r="S49" s="38" t="s">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A49" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B49" s="3">
+        <f>$G$6*1</f>
+        <v>257</v>
+      </c>
+      <c r="C49" s="3">
+        <f>$H$6*1</f>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D49" s="19">
+        <f>$I$6*1</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="S49" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="T49" s="39">
+      <c r="T49" s="3">
         <f>T40+SUM(T47:T48)</f>
         <v>1872.4</v>
       </c>
-      <c r="U49" s="39">
-        <f t="shared" ref="U49:V49" si="16">U40+SUM(U47:U48)</f>
+      <c r="U49" s="3">
+        <f t="shared" ref="U49:V49" si="15">U40+SUM(U47:U48)</f>
         <v>152.95000000000002</v>
       </c>
       <c r="V49" s="19">
+        <f t="shared" si="15"/>
+        <v>3.8270000000000004</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A50" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="B50" s="3">
+        <f>51*5</f>
+        <v>255</v>
+      </c>
+      <c r="C50" s="3">
+        <f>5.3*5</f>
+        <v>26.5</v>
+      </c>
+      <c r="D50" s="5">
+        <f>0.15*5</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A51" s="15"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="19"/>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A52" s="15"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="19"/>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A53" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B53" s="3">
+        <f>SUM(B46:B52)</f>
+        <v>1515.4</v>
+      </c>
+      <c r="C53" s="3">
+        <f t="shared" ref="C53:D53" si="16">SUM(C46:C52)</f>
+        <v>139.60000000000002</v>
+      </c>
+      <c r="D53" s="19">
         <f t="shared" si="16"/>
-        <v>3.8270000000000004</v>
+        <v>3.702</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A55" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="B55" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D55" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A56" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="B56" s="3">
+        <f>240*1</f>
+        <v>240</v>
+      </c>
+      <c r="C56" s="3">
+        <f>15*1</f>
+        <v>15</v>
+      </c>
+      <c r="D56" s="19">
+        <f>0.26*1</f>
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A57" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B57" s="3">
+        <f>$G$6*0.5</f>
+        <v>128.5</v>
+      </c>
+      <c r="C57" s="3">
+        <f>$H$6*0.5</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D57" s="4">
+        <f>$I$6*0.5</f>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A58" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="B58" s="3">
+        <f>B53+SUM(B56:B57)</f>
+        <v>1883.9</v>
+      </c>
+      <c r="C58" s="3">
+        <f t="shared" ref="C58:D58" si="17">C53+SUM(C56:C57)</f>
+        <v>159.20000000000002</v>
+      </c>
+      <c r="D58" s="3">
+        <f t="shared" si="17"/>
+        <v>4.1020000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update on food studies
</commit_message>
<xml_diff>
--- a/extra/studio cibi proteici.xlsx
+++ b/extra/studio cibi proteici.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Documents\uni\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B97F458-2D64-49C3-B92A-1EA3BB4537DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6831B008-48A2-460B-9FCF-4D8EC04DDF3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -62,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="153">
   <si>
     <t>proteine</t>
   </si>
@@ -505,7 +516,22 @@
     <t>2 wurstel smart maxi</t>
   </si>
   <si>
-    <t>sistemare</t>
+    <t>cena 1</t>
+  </si>
+  <si>
+    <t>cena 2</t>
+  </si>
+  <si>
+    <t>35g prot whey no g</t>
+  </si>
+  <si>
+    <t>250ml latte esse</t>
+  </si>
+  <si>
+    <t>test 1</t>
+  </si>
+  <si>
+    <t>test 2</t>
   </si>
 </sst>
 </file>
@@ -1272,19 +1298,19 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="8" max="8" width="33.28515625" customWidth="1"/>
+    <col min="8" max="8" width="33.33203125" customWidth="1"/>
     <col min="13" max="13" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -1304,7 +1330,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -1344,7 +1370,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -1390,7 +1416,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -1439,7 +1465,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
@@ -1488,7 +1514,7 @@
         <v>1.6559999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>24</v>
       </c>
@@ -1537,7 +1563,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
@@ -1585,7 +1611,7 @@
         <v>4.5860000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
@@ -1607,7 +1633,7 @@
         <v>1.6877637130801688</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -1629,7 +1655,7 @@
         <v>2.8235294117647061</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
@@ -1669,7 +1695,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
@@ -1716,7 +1742,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
@@ -1768,7 +1794,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>21</v>
       </c>
@@ -1820,7 +1846,7 @@
         <v>1.6559999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>20</v>
       </c>
@@ -1861,7 +1887,7 @@
         <v>2.0205000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>5</v>
       </c>
@@ -1908,7 +1934,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>9</v>
       </c>
@@ -1943,7 +1969,7 @@
         <v>5.5164999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>10</v>
       </c>
@@ -1965,7 +1991,7 @@
         <v>3.7593984962406015</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>26</v>
       </c>
@@ -1987,7 +2013,7 @@
         <v>1.8950437317784257</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>28</v>
       </c>
@@ -2027,7 +2053,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
@@ -2075,7 +2101,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>27</v>
       </c>
@@ -2127,7 +2153,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>25</v>
       </c>
@@ -2179,7 +2205,7 @@
         <v>1.6559999999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>19</v>
       </c>
@@ -2220,7 +2246,7 @@
         <v>0.28299999999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>16</v>
       </c>
@@ -2259,7 +2285,7 @@
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>29</v>
       </c>
@@ -2294,7 +2320,7 @@
         <v>4.4490000000000007</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>86</v>
       </c>
@@ -2316,7 +2342,7 @@
         <v>3.1153846153846154</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D27" s="1"/>
       <c r="E27" s="2"/>
       <c r="J27" s="15" t="s">
@@ -2326,7 +2352,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D28" s="1"/>
       <c r="E28" s="2"/>
       <c r="H28" t="s">
@@ -2351,7 +2377,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D29" s="1"/>
       <c r="E29" s="2"/>
       <c r="H29" t="s">
@@ -2380,7 +2406,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D30" s="1"/>
       <c r="E30" s="2"/>
       <c r="H30" t="s">
@@ -2413,7 +2439,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="M31" s="15" t="s">
         <v>42</v>
       </c>
@@ -2430,7 +2456,7 @@
         <v>1.4407199999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="M32" s="15" t="s">
         <v>41</v>
       </c>
@@ -2447,7 +2473,7 @@
         <v>0.28299999999999997</v>
       </c>
     </row>
-    <row r="33" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C33" s="1"/>
       <c r="D33" s="2"/>
       <c r="H33" t="s">
@@ -2458,7 +2484,7 @@
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
     </row>
-    <row r="34" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C34" s="1"/>
       <c r="D34" s="2"/>
       <c r="H34" t="s">
@@ -2478,27 +2504,27 @@
         <v>4.2337199999999999</v>
       </c>
     </row>
-    <row r="35" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
       <c r="H35" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:16" x14ac:dyDescent="0.3">
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:16" x14ac:dyDescent="0.3">
       <c r="E38" s="2"/>
     </row>
-    <row r="39" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:16" x14ac:dyDescent="0.3">
       <c r="E39" s="2"/>
     </row>
-    <row r="40" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:16" x14ac:dyDescent="0.3">
       <c r="E40" s="2"/>
     </row>
   </sheetData>
@@ -2519,17 +2545,17 @@
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" customWidth="1"/>
-    <col min="21" max="21" width="22.42578125" customWidth="1"/>
-    <col min="23" max="23" width="12.42578125" customWidth="1"/>
-    <col min="24" max="24" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" customWidth="1"/>
+    <col min="11" max="11" width="18.44140625" customWidth="1"/>
+    <col min="21" max="21" width="22.44140625" customWidth="1"/>
+    <col min="23" max="23" width="12.44140625" customWidth="1"/>
+    <col min="24" max="24" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="K1" s="15"/>
       <c r="L1" s="15" t="s">
         <v>1</v>
@@ -2548,7 +2574,7 @@
       <c r="W1" s="24"/>
       <c r="X1" s="23"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>53</v>
       </c>
@@ -2589,7 +2615,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
@@ -2638,7 +2664,7 @@
       <c r="W3" s="25"/>
       <c r="X3" s="25"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>0</v>
       </c>
@@ -2682,7 +2708,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>40</v>
       </c>
@@ -2730,7 +2756,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="K6" s="15" t="s">
         <v>81</v>
       </c>
@@ -2743,7 +2769,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>78</v>
       </c>
@@ -2752,7 +2778,7 @@
         <v>1943.0857142857144</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>79</v>
       </c>
@@ -2761,7 +2787,7 @@
         <v>151.56428571428572</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>80</v>
       </c>
@@ -2770,7 +2796,7 @@
         <v>4.1071428571428568</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>69</v>
       </c>
@@ -2820,7 +2846,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>63</v>
       </c>
@@ -2878,7 +2904,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>65</v>
       </c>
@@ -2940,7 +2966,7 @@
         <v>1.54</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>66</v>
       </c>
@@ -3002,7 +3028,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>67</v>
       </c>
@@ -3054,7 +3080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>70</v>
       </c>
@@ -3116,7 +3142,7 @@
         <v>4.0500000000000007</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>75</v>
       </c>
@@ -3154,7 +3180,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>63</v>
       </c>
@@ -3198,7 +3224,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>77</v>
       </c>
@@ -3245,7 +3271,7 @@
         <v>1.54</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
         <v>66</v>
       </c>
@@ -3292,7 +3318,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="15"/>
       <c r="B25" s="3">
         <v>0</v>
@@ -3329,7 +3355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
         <v>70</v>
       </c>
@@ -3387,25 +3413,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F24F6A85-44F0-41EA-9C90-606DC79AD939}">
-  <dimension ref="A1:V58"/>
+  <dimension ref="A1:V65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
-    <col min="14" max="14" width="22.28515625" customWidth="1"/>
-    <col min="15" max="15" width="9.85546875" customWidth="1"/>
-    <col min="19" max="19" width="21.28515625" customWidth="1"/>
-    <col min="20" max="20" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" customWidth="1"/>
+    <col min="14" max="14" width="22.33203125" customWidth="1"/>
+    <col min="15" max="15" width="9.88671875" customWidth="1"/>
+    <col min="19" max="19" width="21.33203125" customWidth="1"/>
+    <col min="20" max="20" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>45</v>
       </c>
@@ -3441,7 +3467,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -3487,7 +3513,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -3534,7 +3560,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -3581,7 +3607,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B5">
         <f>SUM(B2:B4)</f>
         <v>1978</v>
@@ -3622,7 +3648,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F6" s="15" t="s">
         <v>68</v>
       </c>
@@ -3653,7 +3679,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>96</v>
       </c>
@@ -3687,7 +3713,7 @@
         <v>88.461538461538453</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>98</v>
       </c>
@@ -3745,7 +3771,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>97</v>
       </c>
@@ -3803,7 +3829,7 @@
         <v>45.625</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>70</v>
       </c>
@@ -3861,7 +3887,7 @@
         <v>50.625</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F11" s="15" t="s">
         <v>112</v>
       </c>
@@ -3904,7 +3930,7 @@
         <v>30.932203389830509</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>96</v>
       </c>
@@ -3959,7 +3985,7 @@
         <v>34.745762711864408</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>100</v>
       </c>
@@ -3996,7 +4022,7 @@
         <v>29.126213592233007</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>99</v>
       </c>
@@ -4033,7 +4059,7 @@
         <v>32.999999999999993</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>70</v>
       </c>
@@ -4070,7 +4096,7 @@
         <v>25.306122448979593</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F16" s="33"/>
       <c r="G16" s="33"/>
       <c r="H16" s="33"/>
@@ -4078,7 +4104,7 @@
       <c r="J16" s="35"/>
       <c r="K16" s="35"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>96</v>
       </c>
@@ -4092,7 +4118,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>100</v>
       </c>
@@ -4109,7 +4135,7 @@
         <v>1.2800000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>102</v>
       </c>
@@ -4126,7 +4152,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>63</v>
       </c>
@@ -4142,7 +4168,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>101</v>
       </c>
@@ -4162,7 +4188,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>70</v>
       </c>
@@ -4216,7 +4242,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="F23" s="15" t="s">
         <v>98</v>
       </c>
@@ -4266,7 +4292,7 @@
         <v>1.6800000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="F24" s="15" t="s">
         <v>97</v>
       </c>
@@ -4313,7 +4339,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
         <v>140</v>
       </c>
@@ -4371,7 +4397,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
         <v>101</v>
       </c>
@@ -4433,7 +4459,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>63</v>
       </c>
@@ -4480,7 +4506,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>141</v>
       </c>
@@ -4539,7 +4565,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>143</v>
       </c>
@@ -4579,7 +4605,7 @@
       <c r="U29" s="3"/>
       <c r="V29" s="19"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
         <v>142</v>
       </c>
@@ -4626,7 +4652,7 @@
         <v>3.43</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31" s="15"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -4635,7 +4661,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
         <v>138</v>
       </c>
@@ -4676,7 +4702,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="F33" s="15" t="s">
         <v>108</v>
       </c>
@@ -4726,7 +4752,7 @@
         <v>1.6519999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="F34" s="15" t="s">
         <v>107</v>
       </c>
@@ -4770,7 +4796,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="F35" s="15" t="s">
         <v>110</v>
       </c>
@@ -4814,7 +4840,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36" s="15" t="s">
         <v>140</v>
       </c>
@@ -4858,7 +4884,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A37" s="15" t="s">
         <v>101</v>
       </c>
@@ -4902,7 +4928,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38" s="15" t="s">
         <v>63</v>
       </c>
@@ -4926,7 +4952,7 @@
       <c r="U38" s="3"/>
       <c r="V38" s="19"/>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39" s="15" t="s">
         <v>141</v>
       </c>
@@ -4951,7 +4977,7 @@
       <c r="U39" s="3"/>
       <c r="V39" s="19"/>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A40" s="15" t="s">
         <v>144</v>
       </c>
@@ -4998,7 +5024,7 @@
         <v>3.4670000000000005</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A41" s="15" t="s">
         <v>142</v>
       </c>
@@ -5016,7 +5042,7 @@
       </c>
       <c r="S41" s="37"/>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A42" s="15"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -5034,7 +5060,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A43" s="15" t="s">
         <v>138</v>
       </c>
@@ -5066,7 +5092,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
       <c r="S44" s="15" t="s">
         <v>138</v>
       </c>
@@ -5083,9 +5109,9 @@
         <v>3.9070000000000005</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A45" s="15" t="s">
-        <v>96</v>
+        <v>151</v>
       </c>
       <c r="B45" s="15" t="s">
         <v>45</v>
@@ -5096,8 +5122,20 @@
       <c r="D45" s="15" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F45" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="G45" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H45" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="I45" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A46" s="15" t="s">
         <v>135</v>
       </c>
@@ -5113,6 +5151,21 @@
         <f>$Q$12*0.7</f>
         <v>1.6519999999999999</v>
       </c>
+      <c r="F46" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="G46" s="3">
+        <f>$O$12*0.7</f>
+        <v>288.39999999999998</v>
+      </c>
+      <c r="H46" s="3">
+        <f>$P$12*0.7</f>
+        <v>57.4</v>
+      </c>
+      <c r="I46" s="19">
+        <f>$Q$12*0.7</f>
+        <v>1.6519999999999999</v>
+      </c>
       <c r="S46" s="15" t="s">
         <v>137</v>
       </c>
@@ -5126,7 +5179,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A47" s="15" t="s">
         <v>118</v>
       </c>
@@ -5142,8 +5195,20 @@
         <f>0.1*5</f>
         <v>0.5</v>
       </c>
-      <c r="F47" t="s">
-        <v>147</v>
+      <c r="F47" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="G47" s="3">
+        <f>47*5</f>
+        <v>235</v>
+      </c>
+      <c r="H47" s="3">
+        <f>3.3*5</f>
+        <v>16.5</v>
+      </c>
+      <c r="I47" s="19">
+        <f>0.1*5</f>
+        <v>0.5</v>
       </c>
       <c r="S47" s="15" t="s">
         <v>84</v>
@@ -5161,7 +5226,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A48" s="15" t="s">
         <v>146</v>
       </c>
@@ -5177,6 +5242,21 @@
         <f>0.26*2</f>
         <v>0.52</v>
       </c>
+      <c r="F48" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="G48" s="3">
+        <f>240*2</f>
+        <v>480</v>
+      </c>
+      <c r="H48" s="3">
+        <f>15*2</f>
+        <v>30</v>
+      </c>
+      <c r="I48" s="19">
+        <f>0.26*2</f>
+        <v>0.52</v>
+      </c>
       <c r="S48" s="15" t="s">
         <v>139</v>
       </c>
@@ -5193,7 +5273,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A49" s="15" t="s">
         <v>101</v>
       </c>
@@ -5209,6 +5289,21 @@
         <f>$I$6*1</f>
         <v>0.28000000000000003</v>
       </c>
+      <c r="F49" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="G49" s="3">
+        <f>$G$6*1</f>
+        <v>257</v>
+      </c>
+      <c r="H49" s="3">
+        <f>$H$6*1</f>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="I49" s="19">
+        <f>$I$6*1</f>
+        <v>0.28000000000000003</v>
+      </c>
       <c r="S49" s="15" t="s">
         <v>138</v>
       </c>
@@ -5225,55 +5320,82 @@
         <v>3.8270000000000004</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A50" s="15" t="s">
         <v>142</v>
       </c>
       <c r="B50" s="3">
-        <f>51*5</f>
-        <v>255</v>
+        <f>51*2.5</f>
+        <v>127.5</v>
       </c>
       <c r="C50" s="3">
-        <f>5.3*5</f>
-        <v>26.5</v>
-      </c>
-      <c r="D50" s="5">
-        <f>0.15*5</f>
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+        <f>5.3*2.5</f>
+        <v>13.25</v>
+      </c>
+      <c r="D50" s="19">
+        <f>0.15*2.5</f>
+        <v>0.375</v>
+      </c>
+      <c r="F50" s="15"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="19"/>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A51" s="15"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="19"/>
-    </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F51" s="15"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="19"/>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A52" s="15"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="19"/>
-    </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F52" s="15"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="19"/>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A53" s="15" t="s">
         <v>70</v>
       </c>
       <c r="B53" s="3">
         <f>SUM(B46:B52)</f>
-        <v>1515.4</v>
+        <v>1387.9</v>
       </c>
       <c r="C53" s="3">
         <f t="shared" ref="C53:D53" si="16">SUM(C46:C52)</f>
-        <v>139.60000000000002</v>
+        <v>126.35000000000001</v>
       </c>
       <c r="D53" s="19">
         <f t="shared" si="16"/>
-        <v>3.702</v>
-      </c>
-    </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+        <v>3.327</v>
+      </c>
+      <c r="F53" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="G53" s="3">
+        <f>SUM(G46:G52)</f>
+        <v>1260.4000000000001</v>
+      </c>
+      <c r="H53" s="3">
+        <f t="shared" ref="H53:I53" si="17">SUM(H46:H52)</f>
+        <v>113.10000000000001</v>
+      </c>
+      <c r="I53" s="19">
+        <f t="shared" si="17"/>
+        <v>2.952</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A55" s="15" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="B55" s="15" t="s">
         <v>45</v>
@@ -5284,8 +5406,20 @@
       <c r="D55" s="15" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F55" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="G55" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H55" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="I55" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A56" s="15" t="s">
         <v>145</v>
       </c>
@@ -5301,39 +5435,228 @@
         <f>0.26*1</f>
         <v>0.26</v>
       </c>
-    </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="F56" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="G56" s="3">
+        <f>$O$12*0.35</f>
+        <v>144.19999999999999</v>
+      </c>
+      <c r="H56" s="3">
+        <f>$P$12*0.35</f>
+        <v>28.7</v>
+      </c>
+      <c r="I56" s="19">
+        <f>$Q$12*0.35</f>
+        <v>0.82599999999999996</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A57" s="15" t="s">
-        <v>139</v>
+        <v>110</v>
       </c>
       <c r="B57" s="3">
-        <f>$G$6*0.5</f>
-        <v>128.5</v>
+        <v>350</v>
       </c>
       <c r="C57" s="3">
-        <f>$H$6*0.5</f>
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="D57" s="4">
-        <f>$I$6*0.5</f>
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A58" s="15" t="s">
+        <v>11.5</v>
+      </c>
+      <c r="D57" s="19">
+        <v>0.13</v>
+      </c>
+      <c r="F57" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="G57" s="3">
+        <f>47*2.5</f>
+        <v>117.5</v>
+      </c>
+      <c r="H57" s="3">
+        <f>3.3*2.5</f>
+        <v>8.25</v>
+      </c>
+      <c r="I57" s="19">
+        <f>0.1*2.5</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A58" s="15"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="F58" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="G58" s="3">
+        <v>350</v>
+      </c>
+      <c r="H58" s="3">
+        <v>11.5</v>
+      </c>
+      <c r="I58" s="19">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A59" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="B58" s="3">
-        <f>B53+SUM(B56:B57)</f>
-        <v>1883.9</v>
-      </c>
-      <c r="C58" s="3">
-        <f t="shared" ref="C58:D58" si="17">C53+SUM(C56:C57)</f>
-        <v>159.20000000000002</v>
-      </c>
-      <c r="D58" s="3">
-        <f t="shared" si="17"/>
-        <v>4.1020000000000003</v>
+      <c r="B59" s="3">
+        <f>B53+SUM(B56:B58)</f>
+        <v>1977.9</v>
+      </c>
+      <c r="C59" s="3">
+        <f>C53+SUM(C56:C58)</f>
+        <v>152.85000000000002</v>
+      </c>
+      <c r="D59" s="20">
+        <f>D53+SUM(D56:D58)</f>
+        <v>3.7170000000000001</v>
+      </c>
+      <c r="F59" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="G59" s="3">
+        <f>G53+SUM(G56:G58)</f>
+        <v>1872.1000000000001</v>
+      </c>
+      <c r="H59" s="3">
+        <f>H53+SUM(H56:H58)</f>
+        <v>161.55000000000001</v>
+      </c>
+      <c r="I59" s="20">
+        <f>I53+SUM(I56:I58)</f>
+        <v>4.1579999999999995</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A61" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="B61" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D61" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F61" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="G61" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H61" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="I61" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A62" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="B62" s="3">
+        <f>240*2</f>
+        <v>480</v>
+      </c>
+      <c r="C62" s="3">
+        <f>15*2</f>
+        <v>30</v>
+      </c>
+      <c r="D62" s="19">
+        <f>0.26*2</f>
+        <v>0.52</v>
+      </c>
+      <c r="F62" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="G62" s="3">
+        <f>$O$12*0.35</f>
+        <v>144.19999999999999</v>
+      </c>
+      <c r="H62" s="3">
+        <f>$P$12*0.35</f>
+        <v>28.7</v>
+      </c>
+      <c r="I62" s="19">
+        <f>$Q$12*0.35</f>
+        <v>0.82599999999999996</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A63" s="15"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="19"/>
+      <c r="F63" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="G63" s="3">
+        <f>47*2.5</f>
+        <v>117.5</v>
+      </c>
+      <c r="H63" s="3">
+        <f>3.3*2.5</f>
+        <v>8.25</v>
+      </c>
+      <c r="I63" s="19">
+        <f>0.1*2.5</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A64" s="15"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="F64" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="G64" s="3">
+        <v>348</v>
+      </c>
+      <c r="H64" s="3">
+        <v>9</v>
+      </c>
+      <c r="I64" s="19">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="B65" s="3">
+        <f>B53+SUM(B62:B64)</f>
+        <v>1867.9</v>
+      </c>
+      <c r="C65" s="3">
+        <f t="shared" ref="C65:D65" si="18">C53+SUM(C62:C64)</f>
+        <v>156.35000000000002</v>
+      </c>
+      <c r="D65" s="19">
+        <f t="shared" si="18"/>
+        <v>3.847</v>
+      </c>
+      <c r="F65" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="G65" s="3">
+        <f>G53+SUM(G62:G64)</f>
+        <v>1870.1000000000001</v>
+      </c>
+      <c r="H65" s="3">
+        <f t="shared" ref="H65" si="19">H53+SUM(H62:H64)</f>
+        <v>159.05000000000001</v>
+      </c>
+      <c r="I65" s="19">
+        <f t="shared" ref="I65" si="20">I53+SUM(I62:I64)</f>
+        <v>4.2279999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edited physics es todo
</commit_message>
<xml_diff>
--- a/extra/studio cibi proteici.xlsx
+++ b/extra/studio cibi proteici.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Documents\uni\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B0EC30-0B2A-42C2-AB44-5A27194770FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1F2857-5410-4C28-861C-0EA982FB1BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
   </bookViews>
@@ -3408,7 +3408,7 @@
   <dimension ref="A1:V71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="P63" sqref="P63"/>
+      <selection activeCell="N58" sqref="N58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
edited protein food studies and renamed a file
</commit_message>
<xml_diff>
--- a/extra/studio cibi proteici.xlsx
+++ b/extra/studio cibi proteici.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Documents\uni\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FB6B16-91F3-47D7-97CA-CAA57D8529B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B763331C-B9D2-4BA6-9B67-2BC094B001F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="164">
   <si>
     <t>proteine</t>
   </si>
@@ -387,12 +387,6 @@
     <t>banana (check peso)</t>
   </si>
   <si>
-    <t>1 banana</t>
-  </si>
-  <si>
-    <t>max 100 cal di bonus</t>
-  </si>
-  <si>
     <t>100g di gnocchi smart</t>
   </si>
   <si>
@@ -417,12 +411,6 @@
     <t>merluzzo smart</t>
   </si>
   <si>
-    <t>100g petto di pollo esse</t>
-  </si>
-  <si>
-    <t>4 scoops</t>
-  </si>
-  <si>
     <t>100ml latte esse</t>
   </si>
   <si>
@@ -550,6 +538,33 @@
   </si>
   <si>
     <t>5 sottilette smart</t>
+  </si>
+  <si>
+    <t>100g petto di pollo smart</t>
+  </si>
+  <si>
+    <t>random</t>
+  </si>
+  <si>
+    <t>1/3L latte esse</t>
+  </si>
+  <si>
+    <t>300g petto di pollo</t>
+  </si>
+  <si>
+    <t>200g riso</t>
+  </si>
+  <si>
+    <t>100g sott sm (5 fette)</t>
+  </si>
+  <si>
+    <t>200g riso basm smart</t>
+  </si>
+  <si>
+    <t>400g petto di pollo sm</t>
+  </si>
+  <si>
+    <t>100g fuso di tacchino</t>
   </si>
 </sst>
 </file>
@@ -621,7 +636,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -733,15 +748,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -755,7 +761,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -789,12 +795,19 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -3421,8 +3434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F24F6A85-44F0-41EA-9C90-606DC79AD939}">
   <dimension ref="A1:V77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="F83" sqref="F83"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="93" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3557,7 +3570,7 @@
         <v>31.153846153846153</v>
       </c>
       <c r="N3" s="15" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="O3" s="3">
         <v>2.5</v>
@@ -3604,7 +3617,7 @@
         <v>45.625</v>
       </c>
       <c r="N4" s="15" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="O4" s="3">
         <v>2.5</v>
@@ -3637,15 +3650,15 @@
         <v>0.33</v>
       </c>
       <c r="J5" s="21">
-        <f t="shared" ref="J5:J16" si="3">H5/G5</f>
+        <f t="shared" ref="J5:J17" si="3">H5/G5</f>
         <v>0</v>
       </c>
       <c r="K5" s="28">
-        <f t="shared" ref="K5:K16" si="4">H5/I5</f>
+        <f t="shared" ref="K5:K17" si="4">H5/I5</f>
         <v>0</v>
       </c>
       <c r="N5" s="15" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="O5" s="3">
         <v>2.5</v>
@@ -3676,7 +3689,7 @@
         <v>32.857142857142854</v>
       </c>
       <c r="N6" s="15" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="O6" s="3">
         <v>2.5</v>
@@ -3756,10 +3769,10 @@
         <v>8.3333333333333339</v>
       </c>
       <c r="M8" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="N8" s="15" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="O8" s="15" t="s">
         <v>45</v>
@@ -3794,7 +3807,7 @@
         <v>0.66</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G9" s="3">
         <v>174</v>
@@ -3814,7 +3827,7 @@
         <v>45</v>
       </c>
       <c r="N9" s="15" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="O9" s="3">
         <v>366</v>
@@ -3826,7 +3839,7 @@
         <f>P3/(O3*10)</f>
         <v>1.6</v>
       </c>
-      <c r="R9" s="33">
+      <c r="R9" s="31">
         <f>P9/O9</f>
         <v>0.19945355191256831</v>
       </c>
@@ -3852,7 +3865,7 @@
         <v>2.9</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G10" s="3">
         <v>51</v>
@@ -3872,7 +3885,7 @@
         <v>35.333333333333336</v>
       </c>
       <c r="N10" s="15" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="O10" s="3">
         <v>340</v>
@@ -3884,7 +3897,7 @@
         <f t="shared" ref="Q10:Q12" si="5">P4/(O4*10)</f>
         <v>1.6</v>
       </c>
-      <c r="R10" s="33">
+      <c r="R10" s="31">
         <f t="shared" ref="R10:R12" si="6">P10/O10</f>
         <v>0.23823529411764705</v>
       </c>
@@ -3895,7 +3908,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F11" s="15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G11" s="3">
         <v>209</v>
@@ -3915,7 +3928,7 @@
         <v>59.090909090909093</v>
       </c>
       <c r="N11" s="15" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="O11" s="3">
         <v>366</v>
@@ -3927,7 +3940,7 @@
         <f t="shared" si="5"/>
         <v>2.36</v>
       </c>
-      <c r="R11" s="33">
+      <c r="R11" s="31">
         <f t="shared" si="6"/>
         <v>0.19945355191256831</v>
       </c>
@@ -3950,7 +3963,7 @@
         <v>40</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G12" s="3">
         <v>84</v>
@@ -3970,7 +3983,7 @@
         <v>20.874999999999996</v>
       </c>
       <c r="N12" s="15" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="O12" s="3">
         <v>412</v>
@@ -3982,7 +3995,7 @@
         <f t="shared" si="5"/>
         <v>2.36</v>
       </c>
-      <c r="R12" s="33">
+      <c r="R12" s="31">
         <f t="shared" si="6"/>
         <v>0.19902912621359223</v>
       </c>
@@ -4008,7 +4021,7 @@
         <v>1.2800000000000002</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>114</v>
+        <v>155</v>
       </c>
       <c r="G13" s="3">
         <v>129</v>
@@ -4017,7 +4030,7 @@
         <v>30</v>
       </c>
       <c r="I13" s="5">
-        <v>1.03</v>
+        <v>0.84</v>
       </c>
       <c r="J13" s="21">
         <f t="shared" si="3"/>
@@ -4025,7 +4038,7 @@
       </c>
       <c r="K13" s="21">
         <f t="shared" si="4"/>
-        <v>29.126213592233007</v>
+        <v>35.714285714285715</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
@@ -4045,7 +4058,7 @@
         <v>1.54</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G14" s="3">
         <v>47</v>
@@ -4081,8 +4094,8 @@
         <f>SUM(D13:D14)</f>
         <v>2.8200000000000003</v>
       </c>
-      <c r="F15" s="31" t="s">
-        <v>120</v>
+      <c r="F15" s="29" t="s">
+        <v>116</v>
       </c>
       <c r="G15" s="11">
         <v>136</v>
@@ -4093,18 +4106,18 @@
       <c r="I15" s="12">
         <v>0.49</v>
       </c>
-      <c r="J15" s="32">
+      <c r="J15" s="30">
         <f t="shared" si="3"/>
         <v>9.1176470588235303E-2</v>
       </c>
-      <c r="K15" s="32">
+      <c r="K15" s="30">
         <f t="shared" si="4"/>
         <v>25.306122448979593</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F16" s="15" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G16" s="3">
         <v>169</v>
@@ -4137,6 +4150,26 @@
       <c r="D17" s="15" t="s">
         <v>40</v>
       </c>
+      <c r="F17" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="G17" s="33">
+        <v>126</v>
+      </c>
+      <c r="H17" s="33">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="I17" s="35">
+        <v>0.4</v>
+      </c>
+      <c r="J17" s="34">
+        <f t="shared" si="3"/>
+        <v>0.14206349206349206</v>
+      </c>
+      <c r="K17" s="34">
+        <f t="shared" si="4"/>
+        <v>44.749999999999993</v>
+      </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
@@ -4205,7 +4238,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="S21" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
@@ -4224,19 +4257,12 @@
         <f t="shared" si="10"/>
         <v>3.2100000000000009</v>
       </c>
-      <c r="F22" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H22" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="I22" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="K22" s="30"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="36"/>
       <c r="N22" s="15" t="s">
         <v>96</v>
       </c>
@@ -4263,26 +4289,13 @@
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="F23" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="G23" s="21">
-        <f>1.4*$G$4</f>
-        <v>512.4</v>
-      </c>
-      <c r="H23" s="21">
-        <f>1.4*$H$4</f>
-        <v>102.19999999999999</v>
-      </c>
-      <c r="I23" s="5">
-        <f>1.4*$I$4</f>
-        <v>2.2399999999999998</v>
-      </c>
-      <c r="J23" t="s">
-        <v>115</v>
-      </c>
+      <c r="F23" s="37"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="37"/>
       <c r="N23" s="15" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="O23" s="21">
         <f>0.7*$G$4</f>
@@ -4297,7 +4310,7 @@
         <v>1.1199999999999999</v>
       </c>
       <c r="S23" s="15" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="T23" s="21">
         <f>1.05*$G$4</f>
@@ -4313,23 +4326,13 @@
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="F24" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="G24" s="3">
-        <f>209*3</f>
-        <v>627</v>
-      </c>
-      <c r="H24" s="3">
-        <f>13*3</f>
-        <v>39</v>
-      </c>
-      <c r="I24" s="4">
-        <f>0.22*3</f>
-        <v>0.66</v>
-      </c>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="37"/>
       <c r="N24" s="15" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="O24" s="3">
         <f>47*5</f>
@@ -4344,7 +4347,7 @@
         <v>0.5</v>
       </c>
       <c r="S24" s="15" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="T24" s="3">
         <f>47*7.5</f>
@@ -4361,7 +4364,7 @@
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B25" s="15" t="s">
         <v>45</v>
@@ -4372,22 +4375,13 @@
       <c r="D25" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="F25" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G25" s="3">
-        <f>$G$5</f>
-        <v>185</v>
-      </c>
-      <c r="H25" s="3">
-        <v>0</v>
-      </c>
-      <c r="I25" s="4">
-        <f>$I$5</f>
-        <v>0.33</v>
-      </c>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="37"/>
       <c r="N25" s="15" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="O25" s="3">
         <f>123*1</f>
@@ -4402,7 +4396,7 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="S25" s="15" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="T25" s="3">
         <f>209*2</f>
@@ -4433,21 +4427,11 @@
         <f>$I$6*1</f>
         <v>0.28000000000000003</v>
       </c>
-      <c r="F26" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="G26" s="3">
-        <f>$G$6*1</f>
-        <v>257</v>
-      </c>
-      <c r="H26" s="3">
-        <f>$H$6*1</f>
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="I26" s="4">
-        <f>$I$6*1</f>
-        <v>0.28000000000000003</v>
-      </c>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="37"/>
       <c r="N26" s="15" t="s">
         <v>97</v>
       </c>
@@ -4494,10 +4478,11 @@
         <f>$I$5</f>
         <v>0.33</v>
       </c>
-      <c r="F27" s="15"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="19"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="37"/>
       <c r="N27" s="15" t="s">
         <v>101</v>
       </c>
@@ -4514,7 +4499,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="S27" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="T27" s="3">
         <v>350</v>
@@ -4528,7 +4513,7 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B28" s="3">
         <f>123*2</f>
@@ -4542,23 +4527,13 @@
         <f>1.09*2</f>
         <v>2.1800000000000002</v>
       </c>
-      <c r="F28" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="G28" s="21">
-        <f>1*G8</f>
-        <v>75</v>
-      </c>
-      <c r="H28" s="21">
-        <f>1*H8</f>
-        <v>1.5</v>
-      </c>
-      <c r="I28" s="19">
-        <f>1*I8</f>
-        <v>0.18</v>
-      </c>
+      <c r="F28" s="37"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="41"/>
+      <c r="J28" s="37"/>
       <c r="N28" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="O28" s="3">
         <v>350</v>
@@ -4570,7 +4545,7 @@
         <v>0.13</v>
       </c>
       <c r="S28" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="T28" s="3">
         <f>1*51</f>
@@ -4587,7 +4562,7 @@
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B29" s="3">
         <f>209*4.5</f>
@@ -4601,21 +4576,11 @@
         <f>0.22*4.5</f>
         <v>0.99</v>
       </c>
-      <c r="F29" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="G29" s="21">
-        <f>SUM(G23:G28)</f>
-        <v>1656.4</v>
-      </c>
-      <c r="H29" s="21">
-        <f>SUM(H23:H28)</f>
-        <v>151.89999999999998</v>
-      </c>
-      <c r="I29" s="19">
-        <f>SUM(I23:I28)</f>
-        <v>3.69</v>
-      </c>
+      <c r="F29" s="37"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="37"/>
       <c r="N29" s="15"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
@@ -4627,7 +4592,7 @@
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B30" s="3">
         <f>51*5</f>
@@ -4641,6 +4606,11 @@
         <f>0.15*5</f>
         <v>0.75</v>
       </c>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="37"/>
       <c r="N30" s="15" t="s">
         <v>70</v>
       </c>
@@ -4677,13 +4647,15 @@
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
-      <c r="F31" s="29" t="s">
-        <v>105</v>
-      </c>
+      <c r="F31" s="37"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="37"/>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B32" s="3">
         <f>SUM(B26:B31)</f>
@@ -4724,19 +4696,19 @@
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="F33" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G33" s="15" t="s">
         <v>45</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I33" s="15" t="s">
         <v>40</v>
       </c>
       <c r="M33" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="N33" s="15" t="s">
         <v>98</v>
@@ -4754,10 +4726,10 @@
         <v>2.2399999999999998</v>
       </c>
       <c r="R33" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="S33" s="15" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="T33" s="3">
         <f>$O$12*0.7</f>
@@ -4774,7 +4746,7 @@
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="F34" s="15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G34" s="3">
         <v>348</v>
@@ -4786,7 +4758,7 @@
         <v>0.2</v>
       </c>
       <c r="N34" s="15" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="O34" s="3">
         <f>47*10</f>
@@ -4801,7 +4773,7 @@
         <v>1</v>
       </c>
       <c r="S34" s="15" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="T34" s="3">
         <f>47*5</f>
@@ -4818,7 +4790,7 @@
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="F35" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G35" s="3">
         <v>350</v>
@@ -4830,7 +4802,7 @@
         <v>0.13</v>
       </c>
       <c r="N35" s="15" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="O35" s="3">
         <f>209*2</f>
@@ -4862,7 +4834,7 @@
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36" s="15" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B36" s="15" t="s">
         <v>45</v>
@@ -4921,7 +4893,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="N37" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="O37" s="3">
         <v>350</v>
@@ -4933,7 +4905,7 @@
         <v>0.13</v>
       </c>
       <c r="S37" s="15" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="T37" s="3">
         <f>51*2.5</f>
@@ -4974,7 +4946,7 @@
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39" s="15" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B39" s="3">
         <f>123*2</f>
@@ -4999,7 +4971,7 @@
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A40" s="15" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B40" s="3">
         <f>240*4</f>
@@ -5046,7 +5018,7 @@
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A41" s="15" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B41" s="3">
         <f>51*5</f>
@@ -5060,7 +5032,7 @@
         <f>0.15*5</f>
         <v>0.75</v>
       </c>
-      <c r="S41" s="34"/>
+      <c r="S41" s="32"/>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A42" s="15"/>
@@ -5068,7 +5040,7 @@
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="S42" s="15" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="T42" s="15" t="s">
         <v>45</v>
@@ -5082,7 +5054,7 @@
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A43" s="15" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B43" s="3">
         <f>SUM(B37:B42)</f>
@@ -5097,7 +5069,7 @@
         <v>4.58</v>
       </c>
       <c r="S43" s="15" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="T43" s="3">
         <f>209*2</f>
@@ -5114,7 +5086,7 @@
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.3">
       <c r="S44" s="15" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="T44" s="3">
         <f>T40+T43</f>
@@ -5131,7 +5103,7 @@
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A45" s="15" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B45" s="15" t="s">
         <v>45</v>
@@ -5143,7 +5115,7 @@
         <v>87</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="G45" s="15" t="s">
         <v>45</v>
@@ -5154,10 +5126,22 @@
       <c r="I45" s="15" t="s">
         <v>87</v>
       </c>
+      <c r="N45" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="O45" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="P45" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q45" s="15" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A46" s="15" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B46" s="3">
         <f>$O$12*0.7</f>
@@ -5172,7 +5156,7 @@
         <v>1.6519999999999999</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="G46" s="3">
         <f>$O$12*0.7</f>
@@ -5186,8 +5170,23 @@
         <f>$Q$12*0.7</f>
         <v>1.6519999999999999</v>
       </c>
+      <c r="N46" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="O46" s="3">
+        <f>(47*10)/3</f>
+        <v>156.66666666666666</v>
+      </c>
+      <c r="P46" s="3">
+        <f>(3.3*10)/3</f>
+        <v>11</v>
+      </c>
+      <c r="Q46" s="19">
+        <f>(0.1*10)/3</f>
+        <v>0.33333333333333331</v>
+      </c>
       <c r="S46" s="15" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="T46" s="15" t="s">
         <v>45</v>
@@ -5201,7 +5200,7 @@
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A47" s="15" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B47" s="3">
         <f>47*5</f>
@@ -5216,7 +5215,7 @@
         <v>0.5</v>
       </c>
       <c r="F47" s="15" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="G47" s="3">
         <f>47*5</f>
@@ -5230,6 +5229,21 @@
         <f>0.1*5</f>
         <v>0.5</v>
       </c>
+      <c r="N47" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="O47" s="3">
+        <f>240*2</f>
+        <v>480</v>
+      </c>
+      <c r="P47" s="3">
+        <f>15*2</f>
+        <v>30</v>
+      </c>
+      <c r="Q47" s="19">
+        <f>0.26*2</f>
+        <v>0.52</v>
+      </c>
       <c r="S47" s="15" t="s">
         <v>84</v>
       </c>
@@ -5248,7 +5262,7 @@
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A48" s="15" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B48" s="3">
         <f>240*2</f>
@@ -5263,7 +5277,7 @@
         <v>0.52</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G48" s="3">
         <f>240*2</f>
@@ -5277,8 +5291,23 @@
         <f>0.26*2</f>
         <v>0.52</v>
       </c>
+      <c r="N48" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="O48" s="3">
+        <f>G13*3</f>
+        <v>387</v>
+      </c>
+      <c r="P48" s="3">
+        <f>H13*3</f>
+        <v>90</v>
+      </c>
+      <c r="Q48" s="19">
+        <f>I13*3</f>
+        <v>2.52</v>
+      </c>
       <c r="S48" s="15" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="T48" s="3">
         <f>$G$6*0.5</f>
@@ -5324,8 +5353,12 @@
         <f>$I$6*1</f>
         <v>0.28000000000000003</v>
       </c>
+      <c r="N49" s="15"/>
+      <c r="O49" s="3"/>
+      <c r="P49" s="3"/>
+      <c r="Q49" s="19"/>
       <c r="S49" s="15" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="T49" s="3">
         <f>T40+SUM(T47:T48)</f>
@@ -5342,7 +5375,7 @@
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A50" s="15" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B50" s="3">
         <f>51*5</f>
@@ -5360,6 +5393,10 @@
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" s="19"/>
+      <c r="N50" s="15"/>
+      <c r="O50" s="3"/>
+      <c r="P50" s="3"/>
+      <c r="Q50" s="19"/>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A51" s="15"/>
@@ -5370,6 +5407,21 @@
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
       <c r="I51" s="19"/>
+      <c r="N51" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="O51" s="3">
+        <f>350*2</f>
+        <v>700</v>
+      </c>
+      <c r="P51" s="3">
+        <f>11.5*2</f>
+        <v>23</v>
+      </c>
+      <c r="Q51" s="19">
+        <f>0.15*2</f>
+        <v>0.3</v>
+      </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A52" s="15"/>
@@ -5380,6 +5432,10 @@
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
       <c r="I52" s="19"/>
+      <c r="N52" s="15"/>
+      <c r="O52" s="3"/>
+      <c r="P52" s="3"/>
+      <c r="Q52" s="19"/>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A53" s="15" t="s">
@@ -5412,10 +5468,25 @@
         <f t="shared" si="17"/>
         <v>2.952</v>
       </c>
+      <c r="N53" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="O53" s="3">
+        <f>SUM(O46:O52)</f>
+        <v>1723.6666666666665</v>
+      </c>
+      <c r="P53" s="3">
+        <f t="shared" ref="P53:Q53" si="18">SUM(P46:P52)</f>
+        <v>154</v>
+      </c>
+      <c r="Q53" s="19">
+        <f t="shared" si="18"/>
+        <v>3.6733333333333329</v>
+      </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A55" s="15" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B55" s="15" t="s">
         <v>45</v>
@@ -5427,7 +5498,7 @@
         <v>87</v>
       </c>
       <c r="F55" s="15" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G55" s="15" t="s">
         <v>45</v>
@@ -5437,6 +5508,18 @@
       </c>
       <c r="I55" s="15" t="s">
         <v>87</v>
+      </c>
+      <c r="N55" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="O55" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="P55" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q55" s="15" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.3">
@@ -5445,7 +5528,7 @@
       <c r="C56" s="3"/>
       <c r="D56" s="19"/>
       <c r="F56" s="15" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="G56" s="3">
         <f>$O$12*0.35</f>
@@ -5459,10 +5542,25 @@
         <f>$Q$12*0.35</f>
         <v>0.82599999999999996</v>
       </c>
+      <c r="N56" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="O56" s="3">
+        <f>(47*5)</f>
+        <v>235</v>
+      </c>
+      <c r="P56" s="3">
+        <f>(3.3*5)</f>
+        <v>16.5</v>
+      </c>
+      <c r="Q56" s="19">
+        <f>(0.1*5)</f>
+        <v>0.5</v>
+      </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A57" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B57" s="3">
         <v>350</v>
@@ -5474,7 +5572,7 @@
         <v>0.13</v>
       </c>
       <c r="F57" s="15" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G57" s="3">
         <f>47*2.5</f>
@@ -5487,6 +5585,18 @@
       <c r="I57" s="19">
         <f>0.1*2.5</f>
         <v>0.25</v>
+      </c>
+      <c r="N57" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="O57" s="3">
+        <v>169</v>
+      </c>
+      <c r="P57" s="3">
+        <v>15.4</v>
+      </c>
+      <c r="Q57" s="5">
+        <v>0.47</v>
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.3">
@@ -5495,7 +5605,7 @@
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="F58" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G58" s="3">
         <v>350</v>
@@ -5506,10 +5616,25 @@
       <c r="I58" s="19">
         <v>0.13</v>
       </c>
+      <c r="N58" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="O58" s="3">
+        <f>G13*3</f>
+        <v>387</v>
+      </c>
+      <c r="P58" s="3">
+        <f>H13*3</f>
+        <v>90</v>
+      </c>
+      <c r="Q58" s="19">
+        <f>I13*3</f>
+        <v>2.52</v>
+      </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A59" s="15" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B59" s="3">
         <f>B53+SUM(B56:B58)</f>
@@ -5524,7 +5649,7 @@
         <v>3.8319999999999999</v>
       </c>
       <c r="F59" s="15" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G59" s="3">
         <f>G53+SUM(G56:G58)</f>
@@ -5538,10 +5663,31 @@
         <f>I53+SUM(I56:I58)</f>
         <v>4.1579999999999995</v>
       </c>
+      <c r="N59" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="O59" s="3">
+        <f>350*2</f>
+        <v>700</v>
+      </c>
+      <c r="P59" s="3">
+        <f>7.4*2</f>
+        <v>14.8</v>
+      </c>
+      <c r="Q59" s="19">
+        <f>0.2*2</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="N60" s="15"/>
+      <c r="O60" s="3"/>
+      <c r="P60" s="3"/>
+      <c r="Q60" s="19"/>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A61" s="15" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B61" s="15" t="s">
         <v>45</v>
@@ -5553,7 +5699,7 @@
         <v>87</v>
       </c>
       <c r="F61" s="15" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G61" s="15" t="s">
         <v>45</v>
@@ -5564,10 +5710,14 @@
       <c r="I61" s="15" t="s">
         <v>87</v>
       </c>
+      <c r="N61" s="15"/>
+      <c r="O61" s="3"/>
+      <c r="P61" s="3"/>
+      <c r="Q61" s="3"/>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A62" s="15" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B62" s="3">
         <f>240*1</f>
@@ -5582,7 +5732,7 @@
         <v>0.26</v>
       </c>
       <c r="F62" s="15" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="G62" s="3">
         <f>$O$12*0.35</f>
@@ -5595,6 +5745,21 @@
       <c r="I62" s="19">
         <f>$Q$12*0.35</f>
         <v>0.82599999999999996</v>
+      </c>
+      <c r="N62" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="O62" s="3">
+        <f>240*2</f>
+        <v>480</v>
+      </c>
+      <c r="P62" s="3">
+        <f>15*2</f>
+        <v>30</v>
+      </c>
+      <c r="Q62" s="19">
+        <f>0.26*2</f>
+        <v>0.52</v>
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.3">
@@ -5603,7 +5768,7 @@
       <c r="C63" s="3"/>
       <c r="D63" s="19"/>
       <c r="F63" s="15" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G63" s="3">
         <f>47*2.5</f>
@@ -5616,6 +5781,21 @@
       <c r="I63" s="19">
         <f>0.1*2.5</f>
         <v>0.25</v>
+      </c>
+      <c r="N63" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="O63" s="3">
+        <f>SUM(O56:O62)</f>
+        <v>1971</v>
+      </c>
+      <c r="P63" s="3">
+        <f>SUM(P56:P62)</f>
+        <v>166.70000000000002</v>
+      </c>
+      <c r="Q63" s="19">
+        <f>SUM(Q56:Q62)</f>
+        <v>4.41</v>
       </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.3">
@@ -5624,7 +5804,7 @@
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
       <c r="F64" s="15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G64" s="3">
         <v>348</v>
@@ -5638,39 +5818,39 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="15" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B65" s="3">
         <f>B53+SUM(B62:B64)</f>
         <v>1755.4</v>
       </c>
       <c r="C65" s="3">
-        <f t="shared" ref="C65:D65" si="18">C53+SUM(C62:C64)</f>
+        <f t="shared" ref="C65:D65" si="19">C53+SUM(C62:C64)</f>
         <v>154.60000000000002</v>
       </c>
       <c r="D65" s="19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>3.9619999999999997</v>
       </c>
       <c r="F65" s="15" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G65" s="3">
         <f>G53+SUM(G62:G64)</f>
         <v>1870.1000000000001</v>
       </c>
       <c r="H65" s="3">
-        <f t="shared" ref="H65" si="19">H53+SUM(H62:H64)</f>
+        <f t="shared" ref="H65" si="20">H53+SUM(H62:H64)</f>
         <v>159.05000000000001</v>
       </c>
       <c r="I65" s="19">
-        <f t="shared" ref="I65" si="20">I53+SUM(I62:I64)</f>
+        <f t="shared" ref="I65" si="21">I53+SUM(I62:I64)</f>
         <v>4.2279999999999998</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="15" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B67" s="15" t="s">
         <v>45</v>
@@ -5682,7 +5862,7 @@
         <v>87</v>
       </c>
       <c r="F67" s="15" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="G67" s="15" t="s">
         <v>45</v>
@@ -5696,7 +5876,7 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="15" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B68" s="3">
         <f>68*2</f>
@@ -5711,7 +5891,7 @@
         <v>0.4</v>
       </c>
       <c r="F68" s="15" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="G68" s="3">
         <f>$O$12*0.35</f>
@@ -5732,7 +5912,7 @@
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
       <c r="F69" s="15" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G69" s="3">
         <f>47*2.5</f>
@@ -5753,7 +5933,7 @@
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
       <c r="F70" s="15" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G70" s="3">
         <f>240*1</f>
@@ -5770,39 +5950,39 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="15" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B71" s="3">
         <f>B53+SUM(B68:B70)</f>
         <v>1651.4</v>
       </c>
       <c r="C71" s="3">
-        <f t="shared" ref="C71:D71" si="21">C53+SUM(C68:C70)</f>
+        <f t="shared" ref="C71:D71" si="22">C53+SUM(C68:C70)</f>
         <v>152.00000000000003</v>
       </c>
       <c r="D71" s="19">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>4.1020000000000003</v>
       </c>
       <c r="F71" s="15" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G71" s="3">
         <f>G53+SUM(G68:G70)</f>
         <v>1762.1000000000001</v>
       </c>
       <c r="H71" s="3">
-        <f t="shared" ref="H71:I71" si="22">H53+SUM(H68:H70)</f>
+        <f t="shared" ref="H71:I71" si="23">H53+SUM(H68:H70)</f>
         <v>165.05</v>
       </c>
       <c r="I71" s="19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>4.2880000000000003</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="15" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B73" s="15" t="s">
         <v>45</v>
@@ -5816,7 +5996,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="15" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B74" s="3">
         <v>-255</v>
@@ -5830,7 +6010,7 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="15" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B75" s="3">
         <f>240*2</f>
@@ -5847,35 +6027,35 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="15" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B76" s="3">
         <f>G16*1</f>
         <v>169</v>
       </c>
       <c r="C76" s="3">
-        <f t="shared" ref="C76:D76" si="23">H16*1</f>
+        <f t="shared" ref="C76:D76" si="24">H16*1</f>
         <v>15.4</v>
       </c>
       <c r="D76" s="19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.47</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="15" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B77" s="3">
         <f>B53+SUM(B74:B76)</f>
         <v>1909.4</v>
       </c>
       <c r="C77" s="3">
-        <f t="shared" ref="C77:D77" si="24">C53+SUM(C74:C76)</f>
+        <f t="shared" ref="C77:D77" si="25">C53+SUM(C74:C76)</f>
         <v>158.50000000000003</v>
       </c>
       <c r="D77" s="19">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>3.9420000000000002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added books and various documents
</commit_message>
<xml_diff>
--- a/extra/studio cibi proteici.xlsx
+++ b/extra/studio cibi proteici.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Documents\uni\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43372118-ADE5-4910-9D49-14553E8C6A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CA2918-6389-4D4E-A9DE-099C7A5EEA2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -22,17 +22,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -74,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="201">
   <si>
     <t>proteine</t>
   </si>
@@ -643,19 +632,40 @@
     <t>1 yogurt magro smart</t>
   </si>
   <si>
-    <t>300g petto di pollo s</t>
-  </si>
-  <si>
-    <t>100g emmental</t>
-  </si>
-  <si>
-    <t>1 wurstel s</t>
-  </si>
-  <si>
     <t>riso smart chicco lungo 5kg</t>
   </si>
   <si>
-    <t>300g riso</t>
+    <t>pasta nice (in sconto)</t>
+  </si>
+  <si>
+    <t>200g emmental</t>
+  </si>
+  <si>
+    <t>200g petto di pollo s</t>
+  </si>
+  <si>
+    <t>maionese?</t>
+  </si>
+  <si>
+    <t>pomodori secchi?</t>
+  </si>
+  <si>
+    <t>aglio?</t>
+  </si>
+  <si>
+    <t>cipolla?</t>
+  </si>
+  <si>
+    <t>maio light</t>
+  </si>
+  <si>
+    <t>mayo</t>
+  </si>
+  <si>
+    <t>mayo light 20g</t>
+  </si>
+  <si>
+    <t>250g pasta integrale</t>
   </si>
 </sst>
 </file>
@@ -864,7 +874,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -910,7 +920,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1420,19 +1429,19 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="8" max="8" width="33.33203125" customWidth="1"/>
+    <col min="8" max="8" width="33.28515625" customWidth="1"/>
     <col min="13" max="13" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -1452,7 +1461,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -1492,7 +1501,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -1538,7 +1547,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -1587,7 +1596,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
@@ -1636,7 +1645,7 @@
         <v>1.6559999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>24</v>
       </c>
@@ -1685,7 +1694,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
@@ -1733,7 +1742,7 @@
         <v>4.5860000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
@@ -1755,7 +1764,7 @@
         <v>1.6877637130801688</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -1777,7 +1786,7 @@
         <v>2.8235294117647061</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
@@ -1817,7 +1826,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
@@ -1864,7 +1873,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
@@ -1916,7 +1925,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>21</v>
       </c>
@@ -1968,7 +1977,7 @@
         <v>1.6559999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>20</v>
       </c>
@@ -2009,7 +2018,7 @@
         <v>2.0205000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>5</v>
       </c>
@@ -2056,7 +2065,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>9</v>
       </c>
@@ -2091,7 +2100,7 @@
         <v>5.5164999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>10</v>
       </c>
@@ -2113,7 +2122,7 @@
         <v>3.7593984962406015</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>26</v>
       </c>
@@ -2135,7 +2144,7 @@
         <v>1.8950437317784257</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>28</v>
       </c>
@@ -2175,7 +2184,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
@@ -2223,7 +2232,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>27</v>
       </c>
@@ -2275,7 +2284,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>25</v>
       </c>
@@ -2327,7 +2336,7 @@
         <v>1.6559999999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>19</v>
       </c>
@@ -2368,7 +2377,7 @@
         <v>0.28299999999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>16</v>
       </c>
@@ -2407,7 +2416,7 @@
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>29</v>
       </c>
@@ -2442,7 +2451,7 @@
         <v>4.4490000000000007</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>86</v>
       </c>
@@ -2464,7 +2473,7 @@
         <v>3.1153846153846154</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D27" s="1"/>
       <c r="E27" s="2"/>
       <c r="J27" s="15" t="s">
@@ -2474,7 +2483,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
       <c r="E28" s="2"/>
       <c r="H28" t="s">
@@ -2499,7 +2508,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D29" s="1"/>
       <c r="E29" s="2"/>
       <c r="H29" t="s">
@@ -2528,7 +2537,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D30" s="1"/>
       <c r="E30" s="2"/>
       <c r="H30" t="s">
@@ -2561,7 +2570,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M31" s="15" t="s">
         <v>42</v>
       </c>
@@ -2578,7 +2587,7 @@
         <v>1.4407199999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M32" s="15" t="s">
         <v>41</v>
       </c>
@@ -2595,7 +2604,7 @@
         <v>0.28299999999999997</v>
       </c>
     </row>
-    <row r="33" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C33" s="1"/>
       <c r="D33" s="2"/>
       <c r="H33" t="s">
@@ -2606,7 +2615,7 @@
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
     </row>
-    <row r="34" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C34" s="1"/>
       <c r="D34" s="2"/>
       <c r="H34" t="s">
@@ -2626,27 +2635,27 @@
         <v>4.2337199999999999</v>
       </c>
     </row>
-    <row r="35" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
       <c r="H35" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E38" s="2"/>
     </row>
-    <row r="39" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E39" s="2"/>
     </row>
-    <row r="40" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E40" s="2"/>
     </row>
   </sheetData>
@@ -2667,17 +2676,17 @@
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" customWidth="1"/>
-    <col min="11" max="11" width="18.44140625" customWidth="1"/>
-    <col min="21" max="21" width="22.44140625" customWidth="1"/>
-    <col min="23" max="23" width="12.44140625" customWidth="1"/>
-    <col min="24" max="24" width="9.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="21" max="21" width="22.42578125" customWidth="1"/>
+    <col min="23" max="23" width="12.42578125" customWidth="1"/>
+    <col min="24" max="24" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="K1" s="15"/>
       <c r="L1" s="15" t="s">
         <v>1</v>
@@ -2696,7 +2705,7 @@
       <c r="W1" s="24"/>
       <c r="X1" s="23"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>53</v>
       </c>
@@ -2737,7 +2746,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
@@ -2786,7 +2795,7 @@
       <c r="W3" s="25"/>
       <c r="X3" s="25"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>0</v>
       </c>
@@ -2830,7 +2839,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>40</v>
       </c>
@@ -2878,7 +2887,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="K6" s="15" t="s">
         <v>81</v>
       </c>
@@ -2891,7 +2900,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>78</v>
       </c>
@@ -2900,7 +2909,7 @@
         <v>1943.0857142857144</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>79</v>
       </c>
@@ -2909,7 +2918,7 @@
         <v>151.56428571428572</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>80</v>
       </c>
@@ -2918,7 +2927,7 @@
         <v>4.1071428571428568</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>69</v>
       </c>
@@ -2968,7 +2977,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>63</v>
       </c>
@@ -3026,7 +3035,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>65</v>
       </c>
@@ -3088,7 +3097,7 @@
         <v>1.54</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>66</v>
       </c>
@@ -3150,7 +3159,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>67</v>
       </c>
@@ -3202,7 +3211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>70</v>
       </c>
@@ -3264,7 +3273,7 @@
         <v>4.0500000000000007</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>75</v>
       </c>
@@ -3302,7 +3311,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>63</v>
       </c>
@@ -3346,7 +3355,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>77</v>
       </c>
@@ -3393,7 +3402,7 @@
         <v>1.54</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>66</v>
       </c>
@@ -3440,7 +3449,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
       <c r="B25" s="3">
         <v>0</v>
@@ -3477,7 +3486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>70</v>
       </c>
@@ -3541,19 +3550,19 @@
       <selection activeCell="O49" sqref="O49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" customWidth="1"/>
-    <col min="14" max="14" width="22.33203125" customWidth="1"/>
-    <col min="15" max="15" width="9.88671875" customWidth="1"/>
-    <col min="19" max="19" width="21.33203125" customWidth="1"/>
-    <col min="20" max="20" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" customWidth="1"/>
+    <col min="14" max="14" width="22.28515625" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" customWidth="1"/>
+    <col min="19" max="19" width="21.28515625" customWidth="1"/>
+    <col min="20" max="20" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>45</v>
       </c>
@@ -3589,7 +3598,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -3635,7 +3644,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -3682,7 +3691,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -3729,7 +3738,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B5">
         <f>SUM(B2:B4)</f>
         <v>1978</v>
@@ -3770,7 +3779,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F6" s="15" t="s">
         <v>68</v>
       </c>
@@ -3801,7 +3810,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>96</v>
       </c>
@@ -3835,7 +3844,7 @@
         <v>88.461538461538453</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>98</v>
       </c>
@@ -3893,7 +3902,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>97</v>
       </c>
@@ -3951,7 +3960,7 @@
         <v>45.625</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>70</v>
       </c>
@@ -4009,7 +4018,7 @@
         <v>50.625</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F11" s="15" t="s">
         <v>110</v>
       </c>
@@ -4052,7 +4061,7 @@
         <v>30.932203389830509</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>96</v>
       </c>
@@ -4107,7 +4116,7 @@
         <v>34.745762711864408</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>100</v>
       </c>
@@ -4144,7 +4153,7 @@
         <v>27.738095238095241</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>99</v>
       </c>
@@ -4181,7 +4190,7 @@
         <v>32.999999999999993</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>70</v>
       </c>
@@ -4218,7 +4227,7 @@
         <v>25.306122448979593</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F16" s="15" t="s">
         <v>153</v>
       </c>
@@ -4240,7 +4249,7 @@
         <v>32.765957446808514</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>96</v>
       </c>
@@ -4274,7 +4283,7 @@
         <v>44.749999999999993</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>100</v>
       </c>
@@ -4311,7 +4320,7 @@
         <v>6.25</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>102</v>
       </c>
@@ -4348,7 +4357,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>63</v>
       </c>
@@ -4384,7 +4393,7 @@
         <v>17.045454545454547</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>101</v>
       </c>
@@ -4424,7 +4433,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>70</v>
       </c>
@@ -4485,7 +4494,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F23" s="15" t="s">
         <v>179</v>
       </c>
@@ -4537,7 +4546,7 @@
         <v>1.6800000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F24" s="15" t="s">
         <v>182</v>
       </c>
@@ -4589,7 +4598,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>136</v>
       </c>
@@ -4653,7 +4662,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>101</v>
       </c>
@@ -4720,7 +4729,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>63</v>
       </c>
@@ -4769,7 +4778,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>137</v>
       </c>
@@ -4813,7 +4822,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>139</v>
       </c>
@@ -4841,7 +4850,7 @@
       <c r="U29" s="3"/>
       <c r="V29" s="19"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>138</v>
       </c>
@@ -4888,13 +4897,13 @@
         <v>3.43</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
         <v>134</v>
       </c>
@@ -4935,7 +4944,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M33" t="s">
         <v>121</v>
       </c>
@@ -4973,7 +4982,7 @@
         <v>1.6519999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="N34" s="15" t="s">
         <v>122</v>
       </c>
@@ -5005,7 +5014,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="N35" s="15" t="s">
         <v>117</v>
       </c>
@@ -5037,7 +5046,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
         <v>136</v>
       </c>
@@ -5081,7 +5090,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
         <v>101</v>
       </c>
@@ -5125,7 +5134,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
         <v>63</v>
       </c>
@@ -5149,7 +5158,7 @@
       <c r="U38" s="3"/>
       <c r="V38" s="19"/>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
         <v>137</v>
       </c>
@@ -5174,7 +5183,7 @@
       <c r="U39" s="3"/>
       <c r="V39" s="19"/>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
         <v>140</v>
       </c>
@@ -5221,7 +5230,7 @@
         <v>3.4670000000000005</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
         <v>138</v>
       </c>
@@ -5251,7 +5260,7 @@
       </c>
       <c r="S41" s="32"/>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="15"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -5281,7 +5290,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
         <v>134</v>
       </c>
@@ -5325,7 +5334,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="S44" s="15" t="s">
         <v>134</v>
       </c>
@@ -5342,7 +5351,7 @@
         <v>3.9070000000000005</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
         <v>147</v>
       </c>
@@ -5380,7 +5389,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
         <v>131</v>
       </c>
@@ -5439,7 +5448,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
         <v>114</v>
       </c>
@@ -5501,7 +5510,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
         <v>142</v>
       </c>
@@ -5563,7 +5572,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="s">
         <v>101</v>
       </c>
@@ -5625,7 +5634,7 @@
         <v>3.8270000000000004</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" s="15" t="s">
         <v>138</v>
       </c>
@@ -5661,7 +5670,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="15"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -5686,7 +5695,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="15"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -5700,7 +5709,7 @@
       <c r="P52" s="3"/>
       <c r="Q52" s="19"/>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="15" t="s">
         <v>70</v>
       </c>
@@ -5747,7 +5756,7 @@
         <v>4.9633333333333329</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="s">
         <v>143</v>
       </c>
@@ -5785,7 +5794,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="15"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -5821,7 +5830,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="15" t="s">
         <v>108</v>
       </c>
@@ -5862,7 +5871,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" s="15"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -5895,7 +5904,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="s">
         <v>134</v>
       </c>
@@ -5942,13 +5951,13 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="N60" s="15"/>
       <c r="O60" s="3"/>
       <c r="P60" s="3"/>
       <c r="Q60" s="19"/>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="s">
         <v>144</v>
       </c>
@@ -5978,7 +5987,7 @@
       <c r="P61" s="3"/>
       <c r="Q61" s="3"/>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62" s="15" t="s">
         <v>141</v>
       </c>
@@ -6025,7 +6034,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A63" s="15"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -6061,7 +6070,7 @@
         <v>4.41</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A64" s="15"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -6079,7 +6088,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="15" t="s">
         <v>134</v>
       </c>
@@ -6123,7 +6132,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N66" s="15" t="s">
         <v>138</v>
       </c>
@@ -6140,7 +6149,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="15" t="s">
         <v>149</v>
       </c>
@@ -6181,7 +6190,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="15" t="s">
         <v>150</v>
       </c>
@@ -6228,7 +6237,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="15"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -6264,7 +6273,7 @@
         <v>1.68</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="15"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -6300,7 +6309,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="15" t="s">
         <v>134</v>
       </c>
@@ -6347,7 +6356,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N72" s="15" t="s">
         <v>167</v>
       </c>
@@ -6364,7 +6373,7 @@
         <v>0.245</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="15" t="s">
         <v>151</v>
       </c>
@@ -6393,7 +6402,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="15" t="s">
         <v>152</v>
       </c>
@@ -6422,7 +6431,7 @@
         <v>4.4783333333333335</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="15" t="s">
         <v>142</v>
       </c>
@@ -6439,7 +6448,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" s="15" t="s">
         <v>154</v>
       </c>
@@ -6456,7 +6465,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" s="15" t="s">
         <v>134</v>
       </c>
@@ -6473,7 +6482,7 @@
         <v>3.9420000000000002</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="15" t="s">
         <v>173</v>
       </c>
@@ -6499,7 +6508,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="36" t="s">
         <v>174</v>
       </c>
@@ -6531,7 +6540,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="36" t="s">
         <v>138</v>
       </c>
@@ -6563,7 +6572,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="15" t="s">
         <v>101</v>
       </c>
@@ -6595,7 +6604,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="15" t="s">
         <v>168</v>
       </c>
@@ -6627,7 +6636,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="37" t="s">
         <v>165</v>
       </c>
@@ -6659,7 +6668,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="37" t="s">
         <v>176</v>
       </c>
@@ -6691,7 +6700,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="15"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -6712,7 +6721,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="15"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -6722,7 +6731,7 @@
       <c r="H88" s="3"/>
       <c r="I88" s="19"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="15"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -6732,7 +6741,7 @@
       <c r="H89" s="3"/>
       <c r="I89" s="19"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="15"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -6742,7 +6751,7 @@
       <c r="H90" s="3"/>
       <c r="I90" s="19"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="15" t="s">
         <v>134</v>
       </c>
@@ -6774,7 +6783,7 @@
         <v>4.7633333333333336</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="15" t="s">
         <v>173</v>
       </c>
@@ -6800,7 +6809,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="36" t="s">
         <v>174</v>
       </c>
@@ -6832,7 +6841,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="36" t="s">
         <v>138</v>
       </c>
@@ -6864,7 +6873,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="15" t="s">
         <v>101</v>
       </c>
@@ -6896,7 +6905,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="15" t="s">
         <v>168</v>
       </c>
@@ -6928,7 +6937,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="37" t="s">
         <v>165</v>
       </c>
@@ -6960,7 +6969,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="37" t="s">
         <v>181</v>
       </c>
@@ -6992,7 +7001,7 @@
         <v>1.125</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="15"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
@@ -7010,7 +7019,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="15"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
@@ -7020,7 +7029,7 @@
       <c r="H101" s="3"/>
       <c r="I101" s="19"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="15"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
@@ -7030,7 +7039,7 @@
       <c r="H102" s="3"/>
       <c r="I102" s="19"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="15"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
@@ -7040,7 +7049,7 @@
       <c r="H103" s="3"/>
       <c r="I103" s="19"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="15" t="s">
         <v>134</v>
       </c>
@@ -7072,7 +7081,7 @@
         <v>4.708333333333333</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="15" t="s">
         <v>173</v>
       </c>
@@ -7098,7 +7107,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="36" t="s">
         <v>174</v>
       </c>
@@ -7130,7 +7139,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="36" t="s">
         <v>138</v>
       </c>
@@ -7162,7 +7171,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="15" t="s">
         <v>101</v>
       </c>
@@ -7194,7 +7203,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="15" t="s">
         <v>168</v>
       </c>
@@ -7226,7 +7235,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="37" t="s">
         <v>165</v>
       </c>
@@ -7258,7 +7267,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="37" t="s">
         <v>185</v>
       </c>
@@ -7290,7 +7299,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="15"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
@@ -7311,7 +7320,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="15"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
@@ -7321,7 +7330,7 @@
       <c r="H114" s="3"/>
       <c r="I114" s="19"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="15"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
@@ -7331,7 +7340,7 @@
       <c r="H115" s="3"/>
       <c r="I115" s="19"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="15"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
@@ -7341,7 +7350,7 @@
       <c r="H116" s="3"/>
       <c r="I116" s="19"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="15" t="s">
         <v>134</v>
       </c>
@@ -7373,7 +7382,7 @@
         <v>4.5458333333333334</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="15" t="s">
         <v>173</v>
       </c>
@@ -7399,7 +7408,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="36" t="s">
         <v>174</v>
       </c>
@@ -7431,7 +7440,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="36" t="s">
         <v>138</v>
       </c>
@@ -7463,7 +7472,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="15" t="s">
         <v>101</v>
       </c>
@@ -7495,7 +7504,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="15" t="s">
         <v>168</v>
       </c>
@@ -7527,7 +7536,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="37" t="s">
         <v>165</v>
       </c>
@@ -7559,7 +7568,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="37" t="s">
         <v>138</v>
       </c>
@@ -7591,7 +7600,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="15"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
@@ -7612,7 +7621,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="15"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
@@ -7622,7 +7631,7 @@
       <c r="H127" s="3"/>
       <c r="I127" s="19"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="15"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
@@ -7632,7 +7641,7 @@
       <c r="H128" s="3"/>
       <c r="I128" s="19"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="15"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
@@ -7642,7 +7651,7 @@
       <c r="H129" s="3"/>
       <c r="I129" s="19"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="15" t="s">
         <v>134</v>
       </c>
@@ -7683,19 +7692,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1786E1A-8123-4323-AA3C-08DDA05A7259}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="15" t="s">
         <v>45</v>
@@ -7713,7 +7723,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>62</v>
       </c>
@@ -7735,7 +7745,7 @@
         <v>27.52293577981651</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>63</v>
       </c>
@@ -7755,7 +7765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>68</v>
       </c>
@@ -7788,8 +7798,20 @@
       <c r="K4" s="3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M4" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>30</v>
       </c>
@@ -7825,8 +7847,23 @@
         <f>0.1*3</f>
         <v>0.30000000000000004</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M5" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="N5" s="3">
+        <f>47*3</f>
+        <v>141</v>
+      </c>
+      <c r="O5" s="3">
+        <f>3.3*3</f>
+        <v>9.8999999999999986</v>
+      </c>
+      <c r="P5" s="3">
+        <f>0.1*3</f>
+        <v>0.30000000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>103</v>
       </c>
@@ -7862,8 +7899,23 @@
         <f>0.15*5</f>
         <v>0.75</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M6" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="N6" s="3">
+        <f>51*5</f>
+        <v>255</v>
+      </c>
+      <c r="O6" s="3">
+        <f>5.3*5</f>
+        <v>26.5</v>
+      </c>
+      <c r="P6" s="3">
+        <f>0.15*5</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>104</v>
       </c>
@@ -7885,22 +7937,37 @@
         <v>45</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="I7" s="3">
-        <f>100*3</f>
-        <v>300</v>
+        <f>100*2</f>
+        <v>200</v>
       </c>
       <c r="J7" s="3">
-        <f>23.2*3</f>
-        <v>69.599999999999994</v>
+        <f>23.2*2</f>
+        <v>46.4</v>
       </c>
       <c r="K7" s="3">
-        <f>0.84*3</f>
-        <v>2.52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+        <f>0.8*2</f>
+        <v>1.6</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="N7" s="3">
+        <f>100*2</f>
+        <v>200</v>
+      </c>
+      <c r="O7" s="3">
+        <f>23.2*2</f>
+        <v>46.4</v>
+      </c>
+      <c r="P7" s="3">
+        <f>0.8*2</f>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>109</v>
       </c>
@@ -7922,22 +7989,37 @@
         <v>35.333333333333336</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I8" s="3">
-        <f>382*1</f>
-        <v>382</v>
+        <f>382*2</f>
+        <v>764</v>
       </c>
       <c r="J8" s="3">
-        <f>28*1</f>
-        <v>28</v>
+        <f>28*2</f>
+        <v>56</v>
       </c>
       <c r="K8" s="3">
-        <f>0.75*1</f>
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+        <f>0.75*2</f>
+        <v>1.5</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="N8" s="3">
+        <f>382*2</f>
+        <v>764</v>
+      </c>
+      <c r="O8" s="3">
+        <f>28*2</f>
+        <v>56</v>
+      </c>
+      <c r="P8" s="3">
+        <f>0.75*2</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>110</v>
       </c>
@@ -7959,19 +8041,25 @@
         <v>59.090909090909093</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="I9" s="3">
-        <v>209</v>
-      </c>
-      <c r="J9" s="3">
-        <v>13</v>
-      </c>
-      <c r="K9" s="3">
-        <v>0.22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+        <f>2*27.7</f>
+        <v>55.4</v>
+      </c>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="M9" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="N9" s="3">
+        <f>2*72</f>
+        <v>144</v>
+      </c>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>111</v>
       </c>
@@ -7993,22 +8081,37 @@
         <v>20.874999999999996</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="I10" s="3">
-        <f>350*3</f>
-        <v>1050</v>
+        <f>350*2.5</f>
+        <v>875</v>
       </c>
       <c r="J10" s="3">
         <f>3*3</f>
         <v>9</v>
       </c>
       <c r="K10" s="3">
-        <f>0.19*3</f>
-        <v>0.57000000000000006</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+        <f>0.24*2.5</f>
+        <v>0.6</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="N10" s="3">
+        <f>350*2.5</f>
+        <v>875</v>
+      </c>
+      <c r="O10" s="3">
+        <f>3*3</f>
+        <v>9</v>
+      </c>
+      <c r="P10" s="3">
+        <f>0.24*2.5</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>155</v>
       </c>
@@ -8019,7 +8122,7 @@
         <v>23.3</v>
       </c>
       <c r="D11" s="5">
-        <v>0.84</v>
+        <v>0.8</v>
       </c>
       <c r="E11" s="21">
         <f t="shared" si="0"/>
@@ -8027,25 +8130,40 @@
       </c>
       <c r="F11" s="21">
         <f t="shared" si="1"/>
-        <v>27.738095238095241</v>
+        <v>29.125</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>134</v>
       </c>
       <c r="I11" s="3">
         <f>SUM(I5:I10)</f>
-        <v>2337</v>
+        <v>2290.4</v>
       </c>
       <c r="J11" s="3">
         <f t="shared" ref="J11:K11" si="2">SUM(J5:J10)</f>
-        <v>156</v>
+        <v>147.80000000000001</v>
       </c>
       <c r="K11" s="3">
         <f t="shared" si="2"/>
-        <v>5.1100000000000003</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+        <v>4.75</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="N11" s="3">
+        <f>SUM(N5:N10)</f>
+        <v>2379</v>
+      </c>
+      <c r="O11" s="3">
+        <f t="shared" ref="O11:P11" si="3">SUM(O5:O10)</f>
+        <v>147.80000000000001</v>
+      </c>
+      <c r="P11" s="3">
+        <f t="shared" si="3"/>
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>112</v>
       </c>
@@ -8067,7 +8185,7 @@
         <v>32.999999999999993</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>116</v>
       </c>
@@ -8088,8 +8206,11 @@
         <f t="shared" si="1"/>
         <v>25.306122448979593</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H13" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>153</v>
       </c>
@@ -8110,8 +8231,11 @@
         <f t="shared" si="1"/>
         <v>32.765957446808514</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H14" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>163</v>
       </c>
@@ -8132,8 +8256,11 @@
         <f t="shared" si="1"/>
         <v>44.749999999999993</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>169</v>
       </c>
@@ -8154,8 +8281,11 @@
         <f t="shared" si="1"/>
         <v>6.25</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H16" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>170</v>
       </c>
@@ -8177,7 +8307,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>171</v>
       </c>
@@ -8199,7 +8329,7 @@
         <v>17.045454545454547</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>172</v>
       </c>
@@ -8221,7 +8351,7 @@
         <v>7.8602620087336241</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>175</v>
       </c>
@@ -8243,7 +8373,7 @@
         <v>22.891566265060241</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>179</v>
       </c>
@@ -8265,7 +8395,7 @@
         <v>15.714285714285715</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>182</v>
       </c>
@@ -8287,7 +8417,7 @@
         <v>24.444444444444443</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>183</v>
       </c>
@@ -8309,7 +8439,7 @@
         <v>37.333333333333336</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>186</v>
       </c>
@@ -8331,26 +8461,64 @@
         <v>29.571428571428573</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="39" t="s">
-        <v>192</v>
-      </c>
-      <c r="B25" s="40">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="B25" s="3">
         <v>350</v>
       </c>
-      <c r="C25" s="40">
+      <c r="C25" s="3">
         <v>3</v>
       </c>
-      <c r="D25" s="26">
+      <c r="D25" s="19">
         <v>0.19</v>
       </c>
-      <c r="E25" s="41">
+      <c r="E25" s="21">
         <f>C25/B25</f>
         <v>8.5714285714285719E-3</v>
       </c>
       <c r="F25" s="21">
         <f>C25/D25</f>
         <v>15.789473684210526</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="B26" s="3">
+        <v>350</v>
+      </c>
+      <c r="C26" s="3">
+        <v>7</v>
+      </c>
+      <c r="D26" s="38">
+        <v>0.16</v>
+      </c>
+      <c r="E26" s="21">
+        <f>C26/B26</f>
+        <v>0.02</v>
+      </c>
+      <c r="F26" s="21">
+        <f>C26/D26</f>
+        <v>43.75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="39" t="s">
+        <v>197</v>
+      </c>
+      <c r="B27" s="40">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="39" t="s">
+        <v>198</v>
+      </c>
+      <c r="B28">
+        <v>720</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated training program and bulk program
</commit_message>
<xml_diff>
--- a/extra/studio cibi proteici.xlsx
+++ b/extra/studio cibi proteici.xlsx
@@ -1,27 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Documents\uni\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CA2918-6389-4D4E-A9DE-099C7A5EEA2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4380F78-90DA-4B51-BF6C-B13696643A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="4" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
     <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
     <sheet name="Foglio3" sheetId="3" r:id="rId3"/>
     <sheet name="Foglio4" sheetId="4" r:id="rId4"/>
+    <sheet name="lean bulk last semester" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -63,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="208">
   <si>
     <t>proteine</t>
   </si>
@@ -666,6 +678,27 @@
   </si>
   <si>
     <t>250g pasta integrale</t>
+  </si>
+  <si>
+    <t>target cal</t>
+  </si>
+  <si>
+    <t>target pro</t>
+  </si>
+  <si>
+    <t>target fat</t>
+  </si>
+  <si>
+    <t>160g</t>
+  </si>
+  <si>
+    <t>92g</t>
+  </si>
+  <si>
+    <t>target fiber</t>
+  </si>
+  <si>
+    <t>40g</t>
   </si>
 </sst>
 </file>
@@ -919,12 +952,14 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
-    <cellStyle name="Percentuale" xfId="2" builtinId="5"/>
-    <cellStyle name="Valuta" xfId="1" builtinId="4"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Per cent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -1114,7 +1149,7 @@
     <tableColumn id="1" xr3:uid="{30081959-5619-4B55-B7D9-1175EC07AC45}" name="/100g" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{14FCB0BC-8DE4-4AA7-8660-575F63F8B8A6}" name="proteine" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{C0B50CE8-FDFE-49A8-8945-F7C5D2CD5713}" name="calorie" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{419A7849-565C-4737-B49A-97B34AC7F736}" name="rapporto proteine/calorie" dataDxfId="2" dataCellStyle="Percentuale">
+    <tableColumn id="4" xr3:uid="{419A7849-565C-4737-B49A-97B34AC7F736}" name="rapporto proteine/calorie" dataDxfId="2">
       <calculatedColumnFormula>B2/C2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{FA12BE60-94F7-4342-93BD-B6B457295831}" name="prezzo/kg" dataDxfId="1"/>
@@ -1127,9 +1162,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1167,7 +1202,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1273,7 +1308,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1415,7 +1450,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1425,23 +1460,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99DE0696-3519-4FAA-80C4-80DCCEE4AE17}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F6" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="8" max="8" width="33.28515625" customWidth="1"/>
+    <col min="8" max="8" width="33.33203125" customWidth="1"/>
     <col min="13" max="13" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -1461,7 +1496,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -1501,7 +1536,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -1547,7 +1582,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -1596,7 +1631,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
@@ -1645,7 +1680,7 @@
         <v>1.6559999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>24</v>
       </c>
@@ -1694,7 +1729,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
@@ -1742,7 +1777,7 @@
         <v>4.5860000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
@@ -1764,7 +1799,7 @@
         <v>1.6877637130801688</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -1786,7 +1821,7 @@
         <v>2.8235294117647061</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
@@ -1826,7 +1861,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
@@ -1873,7 +1908,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
@@ -1925,7 +1960,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>21</v>
       </c>
@@ -1977,7 +2012,7 @@
         <v>1.6559999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>20</v>
       </c>
@@ -2018,7 +2053,7 @@
         <v>2.0205000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>5</v>
       </c>
@@ -2065,7 +2100,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>9</v>
       </c>
@@ -2100,7 +2135,7 @@
         <v>5.5164999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>10</v>
       </c>
@@ -2122,7 +2157,7 @@
         <v>3.7593984962406015</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>26</v>
       </c>
@@ -2144,7 +2179,7 @@
         <v>1.8950437317784257</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>28</v>
       </c>
@@ -2184,7 +2219,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
@@ -2232,7 +2267,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>27</v>
       </c>
@@ -2284,7 +2319,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>25</v>
       </c>
@@ -2336,7 +2371,7 @@
         <v>1.6559999999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>19</v>
       </c>
@@ -2377,7 +2412,7 @@
         <v>0.28299999999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>16</v>
       </c>
@@ -2416,7 +2451,7 @@
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>29</v>
       </c>
@@ -2451,7 +2486,7 @@
         <v>4.4490000000000007</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>86</v>
       </c>
@@ -2473,7 +2508,7 @@
         <v>3.1153846153846154</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D27" s="1"/>
       <c r="E27" s="2"/>
       <c r="J27" s="15" t="s">
@@ -2483,7 +2518,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D28" s="1"/>
       <c r="E28" s="2"/>
       <c r="H28" t="s">
@@ -2508,7 +2543,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D29" s="1"/>
       <c r="E29" s="2"/>
       <c r="H29" t="s">
@@ -2537,7 +2572,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D30" s="1"/>
       <c r="E30" s="2"/>
       <c r="H30" t="s">
@@ -2570,7 +2605,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="M31" s="15" t="s">
         <v>42</v>
       </c>
@@ -2587,7 +2622,7 @@
         <v>1.4407199999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="M32" s="15" t="s">
         <v>41</v>
       </c>
@@ -2604,7 +2639,7 @@
         <v>0.28299999999999997</v>
       </c>
     </row>
-    <row r="33" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C33" s="1"/>
       <c r="D33" s="2"/>
       <c r="H33" t="s">
@@ -2615,7 +2650,7 @@
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
     </row>
-    <row r="34" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C34" s="1"/>
       <c r="D34" s="2"/>
       <c r="H34" t="s">
@@ -2635,27 +2670,27 @@
         <v>4.2337199999999999</v>
       </c>
     </row>
-    <row r="35" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
       <c r="H35" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:16" x14ac:dyDescent="0.3">
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:16" x14ac:dyDescent="0.3">
       <c r="E38" s="2"/>
     </row>
-    <row r="39" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:16" x14ac:dyDescent="0.3">
       <c r="E39" s="2"/>
     </row>
-    <row r="40" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:16" x14ac:dyDescent="0.3">
       <c r="E40" s="2"/>
     </row>
   </sheetData>
@@ -2676,17 +2711,17 @@
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" customWidth="1"/>
-    <col min="21" max="21" width="22.42578125" customWidth="1"/>
-    <col min="23" max="23" width="12.42578125" customWidth="1"/>
-    <col min="24" max="24" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" customWidth="1"/>
+    <col min="11" max="11" width="18.44140625" customWidth="1"/>
+    <col min="21" max="21" width="22.44140625" customWidth="1"/>
+    <col min="23" max="23" width="12.44140625" customWidth="1"/>
+    <col min="24" max="24" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="K1" s="15"/>
       <c r="L1" s="15" t="s">
         <v>1</v>
@@ -2705,7 +2740,7 @@
       <c r="W1" s="24"/>
       <c r="X1" s="23"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>53</v>
       </c>
@@ -2746,7 +2781,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
@@ -2795,7 +2830,7 @@
       <c r="W3" s="25"/>
       <c r="X3" s="25"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>0</v>
       </c>
@@ -2839,7 +2874,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>40</v>
       </c>
@@ -2887,7 +2922,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="K6" s="15" t="s">
         <v>81</v>
       </c>
@@ -2900,7 +2935,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>78</v>
       </c>
@@ -2909,7 +2944,7 @@
         <v>1943.0857142857144</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>79</v>
       </c>
@@ -2918,7 +2953,7 @@
         <v>151.56428571428572</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>80</v>
       </c>
@@ -2927,7 +2962,7 @@
         <v>4.1071428571428568</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>69</v>
       </c>
@@ -2977,7 +3012,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>63</v>
       </c>
@@ -3035,7 +3070,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>65</v>
       </c>
@@ -3097,7 +3132,7 @@
         <v>1.54</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>66</v>
       </c>
@@ -3159,7 +3194,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>67</v>
       </c>
@@ -3211,7 +3246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>70</v>
       </c>
@@ -3273,7 +3308,7 @@
         <v>4.0500000000000007</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>75</v>
       </c>
@@ -3311,7 +3346,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>63</v>
       </c>
@@ -3355,7 +3390,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>77</v>
       </c>
@@ -3402,7 +3437,7 @@
         <v>1.54</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
         <v>66</v>
       </c>
@@ -3449,7 +3484,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="15"/>
       <c r="B25" s="3">
         <v>0</v>
@@ -3486,7 +3521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
         <v>70</v>
       </c>
@@ -3546,23 +3581,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F24F6A85-44F0-41EA-9C90-606DC79AD939}">
   <dimension ref="A1:V130"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="93" workbookViewId="0">
-      <selection activeCell="O49" sqref="O49"/>
+    <sheetView zoomScale="93" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" customWidth="1"/>
-    <col min="14" max="14" width="22.28515625" customWidth="1"/>
-    <col min="15" max="15" width="9.85546875" customWidth="1"/>
-    <col min="19" max="19" width="21.28515625" customWidth="1"/>
-    <col min="20" max="20" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.33203125" customWidth="1"/>
+    <col min="14" max="14" width="22.33203125" customWidth="1"/>
+    <col min="15" max="15" width="9.88671875" customWidth="1"/>
+    <col min="19" max="19" width="21.33203125" customWidth="1"/>
+    <col min="20" max="20" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>45</v>
       </c>
@@ -3598,7 +3633,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -3644,7 +3679,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -3691,7 +3726,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -3738,7 +3773,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B5">
         <f>SUM(B2:B4)</f>
         <v>1978</v>
@@ -3779,7 +3814,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F6" s="15" t="s">
         <v>68</v>
       </c>
@@ -3810,7 +3845,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>96</v>
       </c>
@@ -3844,7 +3879,7 @@
         <v>88.461538461538453</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>98</v>
       </c>
@@ -3902,7 +3937,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>97</v>
       </c>
@@ -3960,7 +3995,7 @@
         <v>45.625</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>70</v>
       </c>
@@ -4018,7 +4053,7 @@
         <v>50.625</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F11" s="15" t="s">
         <v>110</v>
       </c>
@@ -4061,7 +4096,7 @@
         <v>30.932203389830509</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>96</v>
       </c>
@@ -4116,7 +4151,7 @@
         <v>34.745762711864408</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>100</v>
       </c>
@@ -4153,7 +4188,7 @@
         <v>27.738095238095241</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>99</v>
       </c>
@@ -4190,7 +4225,7 @@
         <v>32.999999999999993</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>70</v>
       </c>
@@ -4227,7 +4262,7 @@
         <v>25.306122448979593</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F16" s="15" t="s">
         <v>153</v>
       </c>
@@ -4249,7 +4284,7 @@
         <v>32.765957446808514</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>96</v>
       </c>
@@ -4283,7 +4318,7 @@
         <v>44.749999999999993</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>100</v>
       </c>
@@ -4320,7 +4355,7 @@
         <v>6.25</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>102</v>
       </c>
@@ -4357,7 +4392,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>63</v>
       </c>
@@ -4393,7 +4428,7 @@
         <v>17.045454545454547</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>101</v>
       </c>
@@ -4433,7 +4468,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>70</v>
       </c>
@@ -4494,7 +4529,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="F23" s="15" t="s">
         <v>179</v>
       </c>
@@ -4546,7 +4581,7 @@
         <v>1.6800000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="F24" s="15" t="s">
         <v>182</v>
       </c>
@@ -4598,7 +4633,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
         <v>136</v>
       </c>
@@ -4662,7 +4697,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
         <v>101</v>
       </c>
@@ -4729,7 +4764,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>63</v>
       </c>
@@ -4778,7 +4813,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>137</v>
       </c>
@@ -4822,7 +4857,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>139</v>
       </c>
@@ -4850,7 +4885,7 @@
       <c r="U29" s="3"/>
       <c r="V29" s="19"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
         <v>138</v>
       </c>
@@ -4897,13 +4932,13 @@
         <v>3.43</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31" s="15"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
         <v>134</v>
       </c>
@@ -4944,7 +4979,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="M33" t="s">
         <v>121</v>
       </c>
@@ -4982,7 +5017,7 @@
         <v>1.6519999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="N34" s="15" t="s">
         <v>122</v>
       </c>
@@ -5014,7 +5049,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="N35" s="15" t="s">
         <v>117</v>
       </c>
@@ -5046,7 +5081,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36" s="15" t="s">
         <v>136</v>
       </c>
@@ -5090,7 +5125,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A37" s="15" t="s">
         <v>101</v>
       </c>
@@ -5134,7 +5169,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38" s="15" t="s">
         <v>63</v>
       </c>
@@ -5158,7 +5193,7 @@
       <c r="U38" s="3"/>
       <c r="V38" s="19"/>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39" s="15" t="s">
         <v>137</v>
       </c>
@@ -5183,7 +5218,7 @@
       <c r="U39" s="3"/>
       <c r="V39" s="19"/>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A40" s="15" t="s">
         <v>140</v>
       </c>
@@ -5230,7 +5265,7 @@
         <v>3.4670000000000005</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A41" s="15" t="s">
         <v>138</v>
       </c>
@@ -5260,7 +5295,7 @@
       </c>
       <c r="S41" s="32"/>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A42" s="15"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -5290,7 +5325,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A43" s="15" t="s">
         <v>134</v>
       </c>
@@ -5334,7 +5369,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
       <c r="S44" s="15" t="s">
         <v>134</v>
       </c>
@@ -5351,7 +5386,7 @@
         <v>3.9070000000000005</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A45" s="15" t="s">
         <v>147</v>
       </c>
@@ -5389,7 +5424,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A46" s="15" t="s">
         <v>131</v>
       </c>
@@ -5448,7 +5483,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A47" s="15" t="s">
         <v>114</v>
       </c>
@@ -5510,7 +5545,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A48" s="15" t="s">
         <v>142</v>
       </c>
@@ -5572,7 +5607,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A49" s="15" t="s">
         <v>101</v>
       </c>
@@ -5634,7 +5669,7 @@
         <v>3.8270000000000004</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A50" s="15" t="s">
         <v>138</v>
       </c>
@@ -5670,7 +5705,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A51" s="15"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -5695,7 +5730,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A52" s="15"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -5709,7 +5744,7 @@
       <c r="P52" s="3"/>
       <c r="Q52" s="19"/>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A53" s="15" t="s">
         <v>70</v>
       </c>
@@ -5756,7 +5791,7 @@
         <v>4.9633333333333329</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A55" s="15" t="s">
         <v>143</v>
       </c>
@@ -5794,7 +5829,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A56" s="15"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -5830,7 +5865,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A57" s="15" t="s">
         <v>108</v>
       </c>
@@ -5871,7 +5906,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A58" s="15"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -5904,7 +5939,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A59" s="15" t="s">
         <v>134</v>
       </c>
@@ -5951,13 +5986,13 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.3">
       <c r="N60" s="15"/>
       <c r="O60" s="3"/>
       <c r="P60" s="3"/>
       <c r="Q60" s="19"/>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A61" s="15" t="s">
         <v>144</v>
       </c>
@@ -5987,7 +6022,7 @@
       <c r="P61" s="3"/>
       <c r="Q61" s="3"/>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A62" s="15" t="s">
         <v>141</v>
       </c>
@@ -6034,7 +6069,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A63" s="15"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -6070,7 +6105,7 @@
         <v>4.41</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A64" s="15"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -6088,7 +6123,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="15" t="s">
         <v>134</v>
       </c>
@@ -6132,7 +6167,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N66" s="15" t="s">
         <v>138</v>
       </c>
@@ -6149,7 +6184,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="15" t="s">
         <v>149</v>
       </c>
@@ -6190,7 +6225,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="15" t="s">
         <v>150</v>
       </c>
@@ -6237,7 +6272,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="15"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -6273,7 +6308,7 @@
         <v>1.68</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="15"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -6309,7 +6344,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="15" t="s">
         <v>134</v>
       </c>
@@ -6356,7 +6391,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N72" s="15" t="s">
         <v>167</v>
       </c>
@@ -6373,7 +6408,7 @@
         <v>0.245</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="15" t="s">
         <v>151</v>
       </c>
@@ -6402,7 +6437,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="15" t="s">
         <v>152</v>
       </c>
@@ -6431,7 +6466,7 @@
         <v>4.4783333333333335</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="15" t="s">
         <v>142</v>
       </c>
@@ -6448,7 +6483,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" s="15" t="s">
         <v>154</v>
       </c>
@@ -6465,7 +6500,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" s="15" t="s">
         <v>134</v>
       </c>
@@ -6482,7 +6517,7 @@
         <v>3.9420000000000002</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" s="15" t="s">
         <v>173</v>
       </c>
@@ -6508,7 +6543,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="36" t="s">
         <v>174</v>
       </c>
@@ -6540,7 +6575,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="36" t="s">
         <v>138</v>
       </c>
@@ -6572,7 +6607,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="15" t="s">
         <v>101</v>
       </c>
@@ -6604,7 +6639,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="15" t="s">
         <v>168</v>
       </c>
@@ -6636,7 +6671,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="37" t="s">
         <v>165</v>
       </c>
@@ -6668,7 +6703,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="37" t="s">
         <v>176</v>
       </c>
@@ -6700,7 +6735,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="15"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -6721,7 +6756,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="15"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -6731,7 +6766,7 @@
       <c r="H88" s="3"/>
       <c r="I88" s="19"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="15"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -6741,7 +6776,7 @@
       <c r="H89" s="3"/>
       <c r="I89" s="19"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="15"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -6751,7 +6786,7 @@
       <c r="H90" s="3"/>
       <c r="I90" s="19"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="15" t="s">
         <v>134</v>
       </c>
@@ -6783,7 +6818,7 @@
         <v>4.7633333333333336</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="15" t="s">
         <v>173</v>
       </c>
@@ -6809,7 +6844,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="36" t="s">
         <v>174</v>
       </c>
@@ -6841,7 +6876,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="36" t="s">
         <v>138</v>
       </c>
@@ -6873,7 +6908,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="15" t="s">
         <v>101</v>
       </c>
@@ -6905,7 +6940,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="15" t="s">
         <v>168</v>
       </c>
@@ -6937,7 +6972,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="37" t="s">
         <v>165</v>
       </c>
@@ -6969,7 +7004,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="37" t="s">
         <v>181</v>
       </c>
@@ -7001,7 +7036,7 @@
         <v>1.125</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="15"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
@@ -7019,7 +7054,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="15"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
@@ -7029,7 +7064,7 @@
       <c r="H101" s="3"/>
       <c r="I101" s="19"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="15"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
@@ -7039,7 +7074,7 @@
       <c r="H102" s="3"/>
       <c r="I102" s="19"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="15"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
@@ -7049,7 +7084,7 @@
       <c r="H103" s="3"/>
       <c r="I103" s="19"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="15" t="s">
         <v>134</v>
       </c>
@@ -7081,7 +7116,7 @@
         <v>4.708333333333333</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="15" t="s">
         <v>173</v>
       </c>
@@ -7107,7 +7142,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" s="36" t="s">
         <v>174</v>
       </c>
@@ -7139,7 +7174,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" s="36" t="s">
         <v>138</v>
       </c>
@@ -7171,7 +7206,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" s="15" t="s">
         <v>101</v>
       </c>
@@ -7203,7 +7238,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" s="15" t="s">
         <v>168</v>
       </c>
@@ -7235,7 +7270,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" s="37" t="s">
         <v>165</v>
       </c>
@@ -7267,7 +7302,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" s="37" t="s">
         <v>185</v>
       </c>
@@ -7299,7 +7334,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="15"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
@@ -7320,7 +7355,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" s="15"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
@@ -7330,7 +7365,7 @@
       <c r="H114" s="3"/>
       <c r="I114" s="19"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" s="15"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
@@ -7340,7 +7375,7 @@
       <c r="H115" s="3"/>
       <c r="I115" s="19"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" s="15"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
@@ -7350,7 +7385,7 @@
       <c r="H116" s="3"/>
       <c r="I116" s="19"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" s="15" t="s">
         <v>134</v>
       </c>
@@ -7382,7 +7417,7 @@
         <v>4.5458333333333334</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" s="15" t="s">
         <v>173</v>
       </c>
@@ -7408,7 +7443,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" s="36" t="s">
         <v>174</v>
       </c>
@@ -7440,7 +7475,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" s="36" t="s">
         <v>138</v>
       </c>
@@ -7472,7 +7507,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" s="15" t="s">
         <v>101</v>
       </c>
@@ -7504,7 +7539,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" s="15" t="s">
         <v>168</v>
       </c>
@@ -7536,7 +7571,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" s="37" t="s">
         <v>165</v>
       </c>
@@ -7568,7 +7603,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" s="37" t="s">
         <v>138</v>
       </c>
@@ -7600,7 +7635,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" s="15"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
@@ -7621,7 +7656,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="15"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
@@ -7631,7 +7666,7 @@
       <c r="H127" s="3"/>
       <c r="I127" s="19"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" s="15"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
@@ -7641,7 +7676,7 @@
       <c r="H128" s="3"/>
       <c r="I128" s="19"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="15"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
@@ -7651,7 +7686,7 @@
       <c r="H129" s="3"/>
       <c r="I129" s="19"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" s="15" t="s">
         <v>134</v>
       </c>
@@ -7694,18 +7729,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1786E1A-8123-4323-AA3C-08DDA05A7259}">
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
-    <col min="13" max="13" width="19.28515625" customWidth="1"/>
+    <col min="13" max="13" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="15" t="s">
         <v>45</v>
@@ -7723,7 +7758,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>62</v>
       </c>
@@ -7745,7 +7780,7 @@
         <v>27.52293577981651</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>63</v>
       </c>
@@ -7765,7 +7800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>68</v>
       </c>
@@ -7811,7 +7846,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>30</v>
       </c>
@@ -7863,7 +7898,7 @@
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>103</v>
       </c>
@@ -7915,7 +7950,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>104</v>
       </c>
@@ -7967,7 +8002,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>109</v>
       </c>
@@ -8019,7 +8054,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>110</v>
       </c>
@@ -8059,7 +8094,7 @@
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>111</v>
       </c>
@@ -8111,7 +8146,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>155</v>
       </c>
@@ -8163,7 +8198,7 @@
         <v>4.75</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>112</v>
       </c>
@@ -8185,7 +8220,7 @@
         <v>32.999999999999993</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
         <v>116</v>
       </c>
@@ -8210,7 +8245,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>153</v>
       </c>
@@ -8235,7 +8270,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>163</v>
       </c>
@@ -8260,7 +8295,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>169</v>
       </c>
@@ -8285,7 +8320,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>170</v>
       </c>
@@ -8307,7 +8342,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>171</v>
       </c>
@@ -8329,7 +8364,7 @@
         <v>17.045454545454547</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>172</v>
       </c>
@@ -8351,7 +8386,7 @@
         <v>7.8602620087336241</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>175</v>
       </c>
@@ -8373,7 +8408,7 @@
         <v>22.891566265060241</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>179</v>
       </c>
@@ -8395,7 +8430,7 @@
         <v>15.714285714285715</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>182</v>
       </c>
@@ -8417,7 +8452,7 @@
         <v>24.444444444444443</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>183</v>
       </c>
@@ -8439,7 +8474,7 @@
         <v>37.333333333333336</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
         <v>186</v>
       </c>
@@ -8461,7 +8496,7 @@
         <v>29.571428571428573</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
         <v>189</v>
       </c>
@@ -8483,7 +8518,7 @@
         <v>15.789473684210526</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
         <v>190</v>
       </c>
@@ -8505,20 +8540,67 @@
         <v>43.75</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="39" t="s">
         <v>197</v>
       </c>
-      <c r="B27" s="40">
+      <c r="B27" s="32">
         <v>277</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="39" t="s">
         <v>198</v>
       </c>
       <c r="B28">
         <v>720</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{715CF0DF-138B-4B49-BC97-299FF5018F54}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="8.88671875" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="40">
+        <v>2750</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>204</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>205</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edited foods and uni docs
</commit_message>
<xml_diff>
--- a/extra/studio cibi proteici.xlsx
+++ b/extra/studio cibi proteici.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Documents\uni\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4380F78-90DA-4B51-BF6C-B13696643A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2B5A89-416F-4693-A088-70F2898BD0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="4" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
+    <workbookView xWindow="28680" yWindow="-3420" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -23,17 +23,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -75,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="247">
   <si>
     <t>proteine</t>
   </si>
@@ -689,27 +678,144 @@
     <t>target fat</t>
   </si>
   <si>
-    <t>160g</t>
-  </si>
-  <si>
-    <t>92g</t>
-  </si>
-  <si>
     <t>target fiber</t>
   </si>
   <si>
-    <t>40g</t>
+    <t>daily</t>
+  </si>
+  <si>
+    <t>weekly</t>
+  </si>
+  <si>
+    <t>(6 days)</t>
+  </si>
+  <si>
+    <t>foods (100g)</t>
+  </si>
+  <si>
+    <t>fat</t>
+  </si>
+  <si>
+    <t>food</t>
+  </si>
+  <si>
+    <t>fiber</t>
+  </si>
+  <si>
+    <t>1/3 litro latte esse</t>
+  </si>
+  <si>
+    <t>200g emmenthal</t>
+  </si>
+  <si>
+    <t>200g petto di pollo smart</t>
+  </si>
+  <si>
+    <t>500g yogurt bianco smart</t>
+  </si>
+  <si>
+    <t>100ml latte intero esse</t>
+  </si>
+  <si>
+    <t>micronutrients to add</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>beta carotene</t>
+  </si>
+  <si>
+    <t>thiamine</t>
+  </si>
+  <si>
+    <t>0,5mg</t>
+  </si>
+  <si>
+    <t>0,4mg</t>
+  </si>
+  <si>
+    <t>folic acid</t>
+  </si>
+  <si>
+    <t>300mg</t>
+  </si>
+  <si>
+    <t>vitamin c</t>
+  </si>
+  <si>
+    <t>vitamin b6</t>
+  </si>
+  <si>
+    <t>75mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vitamin d </t>
+  </si>
+  <si>
+    <t>15ug</t>
+  </si>
+  <si>
+    <t>vitamin e</t>
+  </si>
+  <si>
+    <t>vitamin k</t>
+  </si>
+  <si>
+    <t>12mg</t>
+  </si>
+  <si>
+    <t>83ug</t>
+  </si>
+  <si>
+    <t>copper</t>
+  </si>
+  <si>
+    <t>iron</t>
+  </si>
+  <si>
+    <t>magnesium</t>
+  </si>
+  <si>
+    <t>mangenese</t>
+  </si>
+  <si>
+    <t>potassium</t>
+  </si>
+  <si>
+    <t>0,6mg</t>
+  </si>
+  <si>
+    <t>15mg</t>
+  </si>
+  <si>
+    <t>120mg</t>
+  </si>
+  <si>
+    <t>1,8mg</t>
+  </si>
+  <si>
+    <t>2,4g</t>
+  </si>
+  <si>
+    <t>2600ug</t>
+  </si>
+  <si>
+    <t>https://meal.food-nutrients-calculator.com/?aliments=5693-200,130-100,113-300,29-200,502157-500</t>
+  </si>
+  <si>
+    <t>100g (2) uova smart</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-410]_-;\-* #,##0.00\ [$€-410]_-;_-* &quot;-&quot;??\ [$€-410]_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -742,6 +848,21 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1B1B1B"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -782,7 +903,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -901,13 +1022,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -952,16 +1085,247 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="22">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-410]_-;\-* #,##0.00\ [$€-410]_-;_-* &quot;-&quot;??\ [$€-410]_-;_-@_-"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -1127,7 +1491,9 @@
       </border>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{41B1897F-CCDB-4CBB-9BE1-92B702ABC669}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1140,20 +1506,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84F67106-4EFF-43B6-B540-766A1D8E564D}" name="Tabella1" displayName="Tabella1" ref="A1:F26" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84F67106-4EFF-43B6-B540-766A1D8E564D}" name="Tabella1" displayName="Tabella1" ref="A1:F26" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
   <autoFilter ref="A1:F26" xr:uid="{84F67106-4EFF-43B6-B540-766A1D8E564D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F25">
     <sortCondition descending="1" ref="D1:D25"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{30081959-5619-4B55-B7D9-1175EC07AC45}" name="/100g" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{14FCB0BC-8DE4-4AA7-8660-575F63F8B8A6}" name="proteine" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{C0B50CE8-FDFE-49A8-8945-F7C5D2CD5713}" name="calorie" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{419A7849-565C-4737-B49A-97B34AC7F736}" name="rapporto proteine/calorie" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{30081959-5619-4B55-B7D9-1175EC07AC45}" name="/100g" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{14FCB0BC-8DE4-4AA7-8660-575F63F8B8A6}" name="proteine" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{C0B50CE8-FDFE-49A8-8945-F7C5D2CD5713}" name="calorie" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{419A7849-565C-4737-B49A-97B34AC7F736}" name="rapporto proteine/calorie" dataDxfId="14">
       <calculatedColumnFormula>B2/C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{FA12BE60-94F7-4342-93BD-B6B457295831}" name="prezzo/kg" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{616FE227-9C0F-4D3A-A972-663A04B87FDE}" name="rapporto proteine/€" dataDxfId="0">
+    <tableColumn id="5" xr3:uid="{FA12BE60-94F7-4342-93BD-B6B457295831}" name="prezzo/kg" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{616FE227-9C0F-4D3A-A972-663A04B87FDE}" name="rapporto proteine/€" dataDxfId="12">
       <calculatedColumnFormula>B2/E2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1161,10 +1527,34 @@
 </table>
 </file>
 
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{ECDFEEA9-AA58-4204-A8C7-634A63CB75E6}" name="Table2" displayName="Table2" ref="A1:H22" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+  <autoFilter ref="A1:H22" xr:uid="{ECDFEEA9-AA58-4204-A8C7-634A63CB75E6}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H22">
+    <sortCondition descending="1" ref="H1:H22"/>
+  </sortState>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{AB4A45E1-B89A-4707-8479-BFF4F0659BF8}" name="foods (100g)" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{470D54CE-B5A5-41F6-95A8-DD7E923ED244}" name="cal" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{E694C129-0B2F-4C17-9437-94D714E9FD4B}" name="pro" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{E0C3B141-BD31-4EC9-A404-86508C0E7FD7}" name="fat" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{03502587-F9AA-4481-A3E0-2A5A7867FA98}" name="fiber" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{D7F14DF8-B895-41DB-ACB2-D51384C142B1}" name="eur" dataDxfId="2" dataCellStyle="Currency"/>
+    <tableColumn id="5" xr3:uid="{B148E6D9-D950-47D2-BE5C-B98C6182553A}" name="pro/cal" dataDxfId="1">
+      <calculatedColumnFormula>C2/B2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{C3CF0D3F-CCE3-45AB-918F-D28A95B39AAC}" name="pro/eur" dataDxfId="0">
+      <calculatedColumnFormula>C2/F2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1202,7 +1592,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1308,7 +1698,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1450,7 +1840,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1464,19 +1854,19 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="8" max="8" width="33.33203125" customWidth="1"/>
+    <col min="8" max="8" width="33.28515625" customWidth="1"/>
     <col min="13" max="13" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -1496,7 +1886,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -1536,7 +1926,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -1582,7 +1972,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -1631,7 +2021,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
@@ -1680,7 +2070,7 @@
         <v>1.6559999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>24</v>
       </c>
@@ -1729,7 +2119,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
@@ -1777,7 +2167,7 @@
         <v>4.5860000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
@@ -1799,7 +2189,7 @@
         <v>1.6877637130801688</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -1821,7 +2211,7 @@
         <v>2.8235294117647061</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
@@ -1861,7 +2251,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
@@ -1908,7 +2298,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
@@ -1960,7 +2350,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>21</v>
       </c>
@@ -2012,7 +2402,7 @@
         <v>1.6559999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>20</v>
       </c>
@@ -2053,7 +2443,7 @@
         <v>2.0205000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>5</v>
       </c>
@@ -2100,7 +2490,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>9</v>
       </c>
@@ -2135,7 +2525,7 @@
         <v>5.5164999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>10</v>
       </c>
@@ -2157,7 +2547,7 @@
         <v>3.7593984962406015</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>26</v>
       </c>
@@ -2179,7 +2569,7 @@
         <v>1.8950437317784257</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>28</v>
       </c>
@@ -2219,7 +2609,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
@@ -2267,7 +2657,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>27</v>
       </c>
@@ -2319,7 +2709,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>25</v>
       </c>
@@ -2371,7 +2761,7 @@
         <v>1.6559999999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>19</v>
       </c>
@@ -2412,7 +2802,7 @@
         <v>0.28299999999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>16</v>
       </c>
@@ -2451,7 +2841,7 @@
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>29</v>
       </c>
@@ -2486,7 +2876,7 @@
         <v>4.4490000000000007</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>86</v>
       </c>
@@ -2508,7 +2898,7 @@
         <v>3.1153846153846154</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D27" s="1"/>
       <c r="E27" s="2"/>
       <c r="J27" s="15" t="s">
@@ -2518,7 +2908,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
       <c r="E28" s="2"/>
       <c r="H28" t="s">
@@ -2543,7 +2933,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D29" s="1"/>
       <c r="E29" s="2"/>
       <c r="H29" t="s">
@@ -2572,7 +2962,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D30" s="1"/>
       <c r="E30" s="2"/>
       <c r="H30" t="s">
@@ -2605,7 +2995,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M31" s="15" t="s">
         <v>42</v>
       </c>
@@ -2622,7 +3012,7 @@
         <v>1.4407199999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M32" s="15" t="s">
         <v>41</v>
       </c>
@@ -2639,7 +3029,7 @@
         <v>0.28299999999999997</v>
       </c>
     </row>
-    <row r="33" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C33" s="1"/>
       <c r="D33" s="2"/>
       <c r="H33" t="s">
@@ -2650,7 +3040,7 @@
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
     </row>
-    <row r="34" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C34" s="1"/>
       <c r="D34" s="2"/>
       <c r="H34" t="s">
@@ -2670,27 +3060,27 @@
         <v>4.2337199999999999</v>
       </c>
     </row>
-    <row r="35" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
       <c r="H35" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E38" s="2"/>
     </row>
-    <row r="39" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E39" s="2"/>
     </row>
-    <row r="40" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E40" s="2"/>
     </row>
   </sheetData>
@@ -2711,17 +3101,17 @@
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" customWidth="1"/>
-    <col min="11" max="11" width="18.44140625" customWidth="1"/>
-    <col min="21" max="21" width="22.44140625" customWidth="1"/>
-    <col min="23" max="23" width="12.44140625" customWidth="1"/>
-    <col min="24" max="24" width="9.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="21" max="21" width="22.42578125" customWidth="1"/>
+    <col min="23" max="23" width="12.42578125" customWidth="1"/>
+    <col min="24" max="24" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="K1" s="15"/>
       <c r="L1" s="15" t="s">
         <v>1</v>
@@ -2740,7 +3130,7 @@
       <c r="W1" s="24"/>
       <c r="X1" s="23"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>53</v>
       </c>
@@ -2781,7 +3171,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
@@ -2830,7 +3220,7 @@
       <c r="W3" s="25"/>
       <c r="X3" s="25"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>0</v>
       </c>
@@ -2874,7 +3264,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>40</v>
       </c>
@@ -2922,7 +3312,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="K6" s="15" t="s">
         <v>81</v>
       </c>
@@ -2935,7 +3325,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>78</v>
       </c>
@@ -2944,7 +3334,7 @@
         <v>1943.0857142857144</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>79</v>
       </c>
@@ -2953,7 +3343,7 @@
         <v>151.56428571428572</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>80</v>
       </c>
@@ -2962,7 +3352,7 @@
         <v>4.1071428571428568</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>69</v>
       </c>
@@ -3012,7 +3402,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>63</v>
       </c>
@@ -3070,7 +3460,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>65</v>
       </c>
@@ -3132,7 +3522,7 @@
         <v>1.54</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>66</v>
       </c>
@@ -3194,7 +3584,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>67</v>
       </c>
@@ -3246,7 +3636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>70</v>
       </c>
@@ -3308,7 +3698,7 @@
         <v>4.0500000000000007</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>75</v>
       </c>
@@ -3346,7 +3736,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>63</v>
       </c>
@@ -3390,7 +3780,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>77</v>
       </c>
@@ -3437,7 +3827,7 @@
         <v>1.54</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>66</v>
       </c>
@@ -3484,7 +3874,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
       <c r="B25" s="3">
         <v>0</v>
@@ -3521,7 +3911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>70</v>
       </c>
@@ -3585,19 +3975,19 @@
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" customWidth="1"/>
-    <col min="14" max="14" width="22.33203125" customWidth="1"/>
-    <col min="15" max="15" width="9.88671875" customWidth="1"/>
-    <col min="19" max="19" width="21.33203125" customWidth="1"/>
-    <col min="20" max="20" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" customWidth="1"/>
+    <col min="14" max="14" width="22.28515625" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" customWidth="1"/>
+    <col min="19" max="19" width="21.28515625" customWidth="1"/>
+    <col min="20" max="20" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>45</v>
       </c>
@@ -3633,7 +4023,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -3679,7 +4069,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -3726,7 +4116,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -3773,7 +4163,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B5">
         <f>SUM(B2:B4)</f>
         <v>1978</v>
@@ -3814,7 +4204,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F6" s="15" t="s">
         <v>68</v>
       </c>
@@ -3845,7 +4235,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>96</v>
       </c>
@@ -3879,7 +4269,7 @@
         <v>88.461538461538453</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>98</v>
       </c>
@@ -3937,7 +4327,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>97</v>
       </c>
@@ -3995,7 +4385,7 @@
         <v>45.625</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>70</v>
       </c>
@@ -4053,7 +4443,7 @@
         <v>50.625</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F11" s="15" t="s">
         <v>110</v>
       </c>
@@ -4096,7 +4486,7 @@
         <v>30.932203389830509</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>96</v>
       </c>
@@ -4151,7 +4541,7 @@
         <v>34.745762711864408</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>100</v>
       </c>
@@ -4188,7 +4578,7 @@
         <v>27.738095238095241</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>99</v>
       </c>
@@ -4225,7 +4615,7 @@
         <v>32.999999999999993</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>70</v>
       </c>
@@ -4262,7 +4652,7 @@
         <v>25.306122448979593</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F16" s="15" t="s">
         <v>153</v>
       </c>
@@ -4284,7 +4674,7 @@
         <v>32.765957446808514</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>96</v>
       </c>
@@ -4318,7 +4708,7 @@
         <v>44.749999999999993</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>100</v>
       </c>
@@ -4355,7 +4745,7 @@
         <v>6.25</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>102</v>
       </c>
@@ -4392,7 +4782,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>63</v>
       </c>
@@ -4428,7 +4818,7 @@
         <v>17.045454545454547</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>101</v>
       </c>
@@ -4468,7 +4858,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>70</v>
       </c>
@@ -4529,7 +4919,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F23" s="15" t="s">
         <v>179</v>
       </c>
@@ -4581,7 +4971,7 @@
         <v>1.6800000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F24" s="15" t="s">
         <v>182</v>
       </c>
@@ -4633,7 +5023,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>136</v>
       </c>
@@ -4697,7 +5087,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>101</v>
       </c>
@@ -4764,7 +5154,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>63</v>
       </c>
@@ -4813,7 +5203,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>137</v>
       </c>
@@ -4857,7 +5247,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>139</v>
       </c>
@@ -4885,7 +5275,7 @@
       <c r="U29" s="3"/>
       <c r="V29" s="19"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>138</v>
       </c>
@@ -4932,13 +5322,13 @@
         <v>3.43</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
         <v>134</v>
       </c>
@@ -4979,7 +5369,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M33" t="s">
         <v>121</v>
       </c>
@@ -5017,7 +5407,7 @@
         <v>1.6519999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="N34" s="15" t="s">
         <v>122</v>
       </c>
@@ -5049,7 +5439,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="N35" s="15" t="s">
         <v>117</v>
       </c>
@@ -5081,7 +5471,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
         <v>136</v>
       </c>
@@ -5125,7 +5515,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
         <v>101</v>
       </c>
@@ -5169,7 +5559,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
         <v>63</v>
       </c>
@@ -5193,7 +5583,7 @@
       <c r="U38" s="3"/>
       <c r="V38" s="19"/>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
         <v>137</v>
       </c>
@@ -5218,7 +5608,7 @@
       <c r="U39" s="3"/>
       <c r="V39" s="19"/>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
         <v>140</v>
       </c>
@@ -5265,7 +5655,7 @@
         <v>3.4670000000000005</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
         <v>138</v>
       </c>
@@ -5295,7 +5685,7 @@
       </c>
       <c r="S41" s="32"/>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="15"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -5325,7 +5715,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
         <v>134</v>
       </c>
@@ -5369,7 +5759,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="S44" s="15" t="s">
         <v>134</v>
       </c>
@@ -5386,7 +5776,7 @@
         <v>3.9070000000000005</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
         <v>147</v>
       </c>
@@ -5424,7 +5814,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
         <v>131</v>
       </c>
@@ -5483,7 +5873,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
         <v>114</v>
       </c>
@@ -5545,7 +5935,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
         <v>142</v>
       </c>
@@ -5607,7 +5997,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="s">
         <v>101</v>
       </c>
@@ -5669,7 +6059,7 @@
         <v>3.8270000000000004</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" s="15" t="s">
         <v>138</v>
       </c>
@@ -5705,7 +6095,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="15"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -5730,7 +6120,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="15"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -5744,7 +6134,7 @@
       <c r="P52" s="3"/>
       <c r="Q52" s="19"/>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="15" t="s">
         <v>70</v>
       </c>
@@ -5791,7 +6181,7 @@
         <v>4.9633333333333329</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="s">
         <v>143</v>
       </c>
@@ -5829,7 +6219,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="15"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -5865,7 +6255,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="15" t="s">
         <v>108</v>
       </c>
@@ -5906,7 +6296,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" s="15"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -5939,7 +6329,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="s">
         <v>134</v>
       </c>
@@ -5986,13 +6376,13 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="N60" s="15"/>
       <c r="O60" s="3"/>
       <c r="P60" s="3"/>
       <c r="Q60" s="19"/>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="s">
         <v>144</v>
       </c>
@@ -6022,7 +6412,7 @@
       <c r="P61" s="3"/>
       <c r="Q61" s="3"/>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62" s="15" t="s">
         <v>141</v>
       </c>
@@ -6069,7 +6459,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A63" s="15"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -6105,7 +6495,7 @@
         <v>4.41</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A64" s="15"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -6123,7 +6513,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="15" t="s">
         <v>134</v>
       </c>
@@ -6167,7 +6557,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N66" s="15" t="s">
         <v>138</v>
       </c>
@@ -6184,7 +6574,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="15" t="s">
         <v>149</v>
       </c>
@@ -6225,7 +6615,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="15" t="s">
         <v>150</v>
       </c>
@@ -6272,7 +6662,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="15"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -6308,7 +6698,7 @@
         <v>1.68</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="15"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -6344,7 +6734,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="15" t="s">
         <v>134</v>
       </c>
@@ -6391,7 +6781,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N72" s="15" t="s">
         <v>167</v>
       </c>
@@ -6408,7 +6798,7 @@
         <v>0.245</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="15" t="s">
         <v>151</v>
       </c>
@@ -6437,7 +6827,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="15" t="s">
         <v>152</v>
       </c>
@@ -6466,7 +6856,7 @@
         <v>4.4783333333333335</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="15" t="s">
         <v>142</v>
       </c>
@@ -6483,7 +6873,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" s="15" t="s">
         <v>154</v>
       </c>
@@ -6500,7 +6890,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" s="15" t="s">
         <v>134</v>
       </c>
@@ -6517,7 +6907,7 @@
         <v>3.9420000000000002</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="15" t="s">
         <v>173</v>
       </c>
@@ -6543,7 +6933,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="36" t="s">
         <v>174</v>
       </c>
@@ -6575,7 +6965,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="36" t="s">
         <v>138</v>
       </c>
@@ -6607,7 +6997,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="15" t="s">
         <v>101</v>
       </c>
@@ -6639,7 +7029,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="15" t="s">
         <v>168</v>
       </c>
@@ -6671,7 +7061,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="37" t="s">
         <v>165</v>
       </c>
@@ -6703,7 +7093,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="37" t="s">
         <v>176</v>
       </c>
@@ -6735,7 +7125,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="15"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -6756,7 +7146,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="15"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -6766,7 +7156,7 @@
       <c r="H88" s="3"/>
       <c r="I88" s="19"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="15"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -6776,7 +7166,7 @@
       <c r="H89" s="3"/>
       <c r="I89" s="19"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="15"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -6786,7 +7176,7 @@
       <c r="H90" s="3"/>
       <c r="I90" s="19"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="15" t="s">
         <v>134</v>
       </c>
@@ -6818,7 +7208,7 @@
         <v>4.7633333333333336</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="15" t="s">
         <v>173</v>
       </c>
@@ -6844,7 +7234,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="36" t="s">
         <v>174</v>
       </c>
@@ -6876,7 +7266,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="36" t="s">
         <v>138</v>
       </c>
@@ -6908,7 +7298,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="15" t="s">
         <v>101</v>
       </c>
@@ -6940,7 +7330,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="15" t="s">
         <v>168</v>
       </c>
@@ -6972,7 +7362,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="37" t="s">
         <v>165</v>
       </c>
@@ -7004,7 +7394,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="37" t="s">
         <v>181</v>
       </c>
@@ -7036,7 +7426,7 @@
         <v>1.125</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="15"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
@@ -7054,7 +7444,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="15"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
@@ -7064,7 +7454,7 @@
       <c r="H101" s="3"/>
       <c r="I101" s="19"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="15"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
@@ -7074,7 +7464,7 @@
       <c r="H102" s="3"/>
       <c r="I102" s="19"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="15"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
@@ -7084,7 +7474,7 @@
       <c r="H103" s="3"/>
       <c r="I103" s="19"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="15" t="s">
         <v>134</v>
       </c>
@@ -7116,7 +7506,7 @@
         <v>4.708333333333333</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="15" t="s">
         <v>173</v>
       </c>
@@ -7142,7 +7532,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="36" t="s">
         <v>174</v>
       </c>
@@ -7174,7 +7564,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="36" t="s">
         <v>138</v>
       </c>
@@ -7206,7 +7596,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="15" t="s">
         <v>101</v>
       </c>
@@ -7238,7 +7628,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="15" t="s">
         <v>168</v>
       </c>
@@ -7270,7 +7660,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="37" t="s">
         <v>165</v>
       </c>
@@ -7302,7 +7692,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="37" t="s">
         <v>185</v>
       </c>
@@ -7334,7 +7724,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="15"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
@@ -7355,7 +7745,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="15"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
@@ -7365,7 +7755,7 @@
       <c r="H114" s="3"/>
       <c r="I114" s="19"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="15"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
@@ -7375,7 +7765,7 @@
       <c r="H115" s="3"/>
       <c r="I115" s="19"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="15"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
@@ -7385,7 +7775,7 @@
       <c r="H116" s="3"/>
       <c r="I116" s="19"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="15" t="s">
         <v>134</v>
       </c>
@@ -7417,7 +7807,7 @@
         <v>4.5458333333333334</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="15" t="s">
         <v>173</v>
       </c>
@@ -7443,7 +7833,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="36" t="s">
         <v>174</v>
       </c>
@@ -7475,7 +7865,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="36" t="s">
         <v>138</v>
       </c>
@@ -7507,7 +7897,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="15" t="s">
         <v>101</v>
       </c>
@@ -7539,7 +7929,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="15" t="s">
         <v>168</v>
       </c>
@@ -7571,7 +7961,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="37" t="s">
         <v>165</v>
       </c>
@@ -7603,7 +7993,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="37" t="s">
         <v>138</v>
       </c>
@@ -7635,7 +8025,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="15"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
@@ -7656,7 +8046,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="15"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
@@ -7666,7 +8056,7 @@
       <c r="H127" s="3"/>
       <c r="I127" s="19"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="15"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
@@ -7676,7 +8066,7 @@
       <c r="H128" s="3"/>
       <c r="I128" s="19"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="15"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
@@ -7686,7 +8076,7 @@
       <c r="H129" s="3"/>
       <c r="I129" s="19"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="15" t="s">
         <v>134</v>
       </c>
@@ -7730,17 +8120,17 @@
   <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
-    <col min="13" max="13" width="19.33203125" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="15" t="s">
         <v>45</v>
@@ -7758,7 +8148,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>62</v>
       </c>
@@ -7780,7 +8170,7 @@
         <v>27.52293577981651</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>63</v>
       </c>
@@ -7800,7 +8190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>68</v>
       </c>
@@ -7846,7 +8236,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>30</v>
       </c>
@@ -7898,7 +8288,7 @@
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>103</v>
       </c>
@@ -7950,7 +8340,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>104</v>
       </c>
@@ -8002,7 +8392,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>109</v>
       </c>
@@ -8054,7 +8444,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>110</v>
       </c>
@@ -8094,7 +8484,7 @@
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>111</v>
       </c>
@@ -8146,7 +8536,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>155</v>
       </c>
@@ -8198,7 +8588,7 @@
         <v>4.75</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>112</v>
       </c>
@@ -8220,7 +8610,7 @@
         <v>32.999999999999993</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>116</v>
       </c>
@@ -8245,7 +8635,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>153</v>
       </c>
@@ -8270,7 +8660,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>163</v>
       </c>
@@ -8295,7 +8685,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>169</v>
       </c>
@@ -8320,7 +8710,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>170</v>
       </c>
@@ -8342,7 +8732,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>171</v>
       </c>
@@ -8364,7 +8754,7 @@
         <v>17.045454545454547</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>172</v>
       </c>
@@ -8386,7 +8776,7 @@
         <v>7.8602620087336241</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>175</v>
       </c>
@@ -8408,7 +8798,7 @@
         <v>22.891566265060241</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>179</v>
       </c>
@@ -8430,7 +8820,7 @@
         <v>15.714285714285715</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>182</v>
       </c>
@@ -8452,7 +8842,7 @@
         <v>24.444444444444443</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>183</v>
       </c>
@@ -8474,7 +8864,7 @@
         <v>37.333333333333336</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>186</v>
       </c>
@@ -8496,7 +8886,7 @@
         <v>29.571428571428573</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>189</v>
       </c>
@@ -8518,7 +8908,7 @@
         <v>15.789473684210526</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>190</v>
       </c>
@@ -8540,7 +8930,7 @@
         <v>43.75</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="39" t="s">
         <v>197</v>
       </c>
@@ -8548,7 +8938,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="39" t="s">
         <v>198</v>
       </c>
@@ -8563,47 +8953,939 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{715CF0DF-138B-4B49-BC97-299FF5018F54}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:U35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="26" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
+    <col min="16" max="16" width="22" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="44" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>209</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>211</v>
+      </c>
+      <c r="F1" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" s="46" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="3">
+        <v>209</v>
+      </c>
+      <c r="C2" s="3">
+        <v>13</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="19">
+        <v>0.22</v>
+      </c>
+      <c r="G2" s="21">
+        <f t="shared" ref="G2:G22" si="0">C2/B2</f>
+        <v>6.2200956937799042E-2</v>
+      </c>
+      <c r="H2" s="21">
+        <f t="shared" ref="H2:H22" si="1">C2/F2</f>
+        <v>59.090909090909093</v>
+      </c>
+      <c r="P2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="40" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" s="3">
+        <v>126</v>
+      </c>
+      <c r="C3" s="3">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="19">
+        <v>0.4</v>
+      </c>
+      <c r="G3" s="21">
+        <f t="shared" si="0"/>
+        <v>0.14206349206349206</v>
+      </c>
+      <c r="H3" s="21">
+        <f t="shared" si="1"/>
+        <v>44.749999999999993</v>
+      </c>
+      <c r="P3" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q3" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="R3" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="S3" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="T3" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="U3" s="50" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="40" t="s">
+        <v>183</v>
+      </c>
+      <c r="B4" s="3">
+        <v>382</v>
+      </c>
+      <c r="C4" s="3">
+        <v>28</v>
+      </c>
+      <c r="D4" s="3">
+        <v>30</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="22">
+        <v>0.75</v>
+      </c>
+      <c r="G4" s="21">
+        <f t="shared" si="0"/>
+        <v>7.3298429319371722E-2</v>
+      </c>
+      <c r="H4" s="21">
+        <f t="shared" si="1"/>
+        <v>37.333333333333336</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q4" s="3">
+        <f>B12</f>
+        <v>136</v>
+      </c>
+      <c r="R4" s="3">
+        <f>C12</f>
+        <v>12.4</v>
+      </c>
+      <c r="S4" s="3">
+        <f t="shared" ref="S4:U4" si="2">D12</f>
+        <v>9.5</v>
+      </c>
+      <c r="T4" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U4" s="19">
+        <f t="shared" si="2"/>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="40" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="3">
+        <v>51</v>
+      </c>
+      <c r="C5" s="3">
+        <v>5.3</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="19">
+        <v>0.15</v>
+      </c>
+      <c r="G5" s="21">
+        <f t="shared" si="0"/>
+        <v>0.10392156862745097</v>
+      </c>
+      <c r="H5" s="13">
+        <f t="shared" si="1"/>
+        <v>35.333333333333336</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q5" s="3">
+        <f>B6*3.33</f>
+        <v>216.45000000000002</v>
+      </c>
+      <c r="R5" s="3">
+        <f t="shared" ref="R5:U5" si="3">C6*3.33</f>
+        <v>10.988999999999999</v>
+      </c>
+      <c r="S5" s="3">
+        <f t="shared" si="3"/>
+        <v>11.988000000000001</v>
+      </c>
+      <c r="T5" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U5" s="19">
+        <f t="shared" si="3"/>
+        <v>0.33300000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="40" t="s">
+        <v>216</v>
+      </c>
+      <c r="B6" s="3">
+        <v>65</v>
+      </c>
+      <c r="C6" s="3">
+        <v>3.3</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3.6</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="G6" s="21">
+        <f t="shared" si="0"/>
+        <v>5.0769230769230768E-2</v>
+      </c>
+      <c r="H6" s="13">
+        <f t="shared" si="1"/>
+        <v>32.999999999999993</v>
+      </c>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="19"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="40" t="s">
+        <v>153</v>
+      </c>
+      <c r="B7" s="3">
+        <v>169</v>
+      </c>
+      <c r="C7" s="3">
+        <v>15.4</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="19">
+        <v>0.47</v>
+      </c>
+      <c r="G7" s="21">
+        <f t="shared" si="0"/>
+        <v>9.1124260355029588E-2</v>
+      </c>
+      <c r="H7" s="13">
+        <f t="shared" si="1"/>
+        <v>32.765957446808514</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q7" s="3">
+        <f>B10*2</f>
+        <v>200</v>
+      </c>
+      <c r="R7" s="3">
+        <f t="shared" ref="R7:U7" si="4">C10*2</f>
+        <v>46.6</v>
+      </c>
+      <c r="S7" s="3">
+        <f t="shared" si="4"/>
+        <v>1.6</v>
+      </c>
+      <c r="T7" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="U7" s="3">
+        <f t="shared" si="4"/>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="B8" s="3">
+        <v>115</v>
+      </c>
+      <c r="C8" s="3">
+        <v>9</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="G8" s="21">
+        <f t="shared" si="0"/>
+        <v>7.8260869565217397E-2</v>
+      </c>
+      <c r="H8" s="13">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q8" s="3">
+        <f>B4*2</f>
+        <v>764</v>
+      </c>
+      <c r="R8" s="3">
+        <f t="shared" ref="R8:U8" si="5">C4*2</f>
+        <v>56</v>
+      </c>
+      <c r="S8" s="3">
+        <f t="shared" si="5"/>
+        <v>60</v>
+      </c>
+      <c r="T8" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U8" s="3">
+        <f t="shared" si="5"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="42" t="s">
+        <v>186</v>
+      </c>
+      <c r="B9" s="30">
+        <v>146</v>
+      </c>
+      <c r="C9" s="30">
+        <v>20.7</v>
+      </c>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="47">
+        <v>0.7</v>
+      </c>
+      <c r="G9" s="30">
+        <f t="shared" si="0"/>
+        <v>0.14178082191780822</v>
+      </c>
+      <c r="H9" s="43">
+        <f t="shared" si="1"/>
+        <v>29.571428571428573</v>
+      </c>
+      <c r="P9" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q9" s="3">
+        <f>B5*5</f>
+        <v>255</v>
+      </c>
+      <c r="R9" s="3">
+        <f t="shared" ref="R9:U9" si="6">C5*5</f>
+        <v>26.5</v>
+      </c>
+      <c r="S9" s="3">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="T9" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U9" s="3">
+        <f t="shared" si="6"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="B10" s="3">
+        <v>100</v>
+      </c>
+      <c r="C10" s="3">
+        <v>23.3</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="G10" s="21">
+        <f t="shared" si="0"/>
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="H10" s="13">
+        <f t="shared" si="1"/>
+        <v>29.125</v>
+      </c>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="19"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="3">
+        <v>123</v>
+      </c>
+      <c r="C11" s="3">
+        <v>30</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="19">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="G11" s="21">
+        <f t="shared" si="0"/>
+        <v>0.24390243902439024</v>
+      </c>
+      <c r="H11" s="13">
+        <f t="shared" si="1"/>
+        <v>27.52293577981651</v>
+      </c>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="19"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="40" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" s="3">
+        <v>136</v>
+      </c>
+      <c r="C12" s="3">
+        <v>12.4</v>
+      </c>
+      <c r="D12" s="3">
+        <v>9.5</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="19">
+        <v>0.49</v>
+      </c>
+      <c r="G12" s="21">
+        <f t="shared" si="0"/>
+        <v>9.1176470588235303E-2</v>
+      </c>
+      <c r="H12" s="13">
+        <f t="shared" si="1"/>
+        <v>25.306122448979593</v>
+      </c>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="19"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="40" t="s">
+        <v>182</v>
+      </c>
+      <c r="B13" s="3">
+        <v>315</v>
+      </c>
+      <c r="C13" s="3">
+        <v>22</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="22">
+        <v>0.9</v>
+      </c>
+      <c r="G13" s="21">
+        <f t="shared" si="0"/>
+        <v>6.9841269841269843E-2</v>
+      </c>
+      <c r="H13" s="13">
+        <f t="shared" si="1"/>
+        <v>24.444444444444443</v>
+      </c>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="19"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="B14" s="3">
+        <v>331</v>
+      </c>
+      <c r="C14" s="3">
+        <v>19</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="19">
+        <v>0.83</v>
+      </c>
+      <c r="G14" s="21">
+        <f t="shared" si="0"/>
+        <v>5.7401812688821753E-2</v>
+      </c>
+      <c r="H14" s="13">
+        <f t="shared" si="1"/>
+        <v>22.891566265060241</v>
+      </c>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="19"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="3">
+        <v>84</v>
+      </c>
+      <c r="C15" s="3">
+        <v>16.7</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="G15" s="21">
+        <f t="shared" si="0"/>
+        <v>0.1988095238095238</v>
+      </c>
+      <c r="H15" s="13">
+        <f t="shared" si="1"/>
+        <v>20.874999999999996</v>
+      </c>
+      <c r="P15" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q15" s="15">
+        <f>SUM(Q4:Q14)</f>
+        <v>1571.45</v>
+      </c>
+      <c r="R15" s="15">
+        <f t="shared" ref="R15:U15" si="7">SUM(R4:R14)</f>
+        <v>152.489</v>
+      </c>
+      <c r="S15" s="15">
+        <f t="shared" si="7"/>
+        <v>83.587999999999994</v>
+      </c>
+      <c r="T15" s="15">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="U15" s="15">
+        <f t="shared" si="7"/>
+        <v>4.673</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="40" t="s">
+        <v>171</v>
+      </c>
+      <c r="B16" s="3">
+        <v>180</v>
+      </c>
+      <c r="C16" s="3">
+        <v>15</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="19">
+        <v>0.88</v>
+      </c>
+      <c r="G16" s="21">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="H16" s="13">
+        <f t="shared" si="1"/>
+        <v>17.045454545454547</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="B17" s="3">
+        <v>350</v>
+      </c>
+      <c r="C17" s="3">
+        <v>3</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="19">
+        <v>0.19</v>
+      </c>
+      <c r="G17" s="21">
+        <f t="shared" si="0"/>
+        <v>8.5714285714285719E-3</v>
+      </c>
+      <c r="H17" s="13">
+        <f t="shared" si="1"/>
+        <v>15.789473684210526</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="B18" s="21">
+        <v>49</v>
+      </c>
+      <c r="C18" s="21">
+        <v>5.5</v>
+      </c>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="19">
+        <v>0.35</v>
+      </c>
+      <c r="G18" s="21">
+        <f t="shared" si="0"/>
+        <v>0.11224489795918367</v>
+      </c>
+      <c r="H18" s="13">
+        <f t="shared" si="1"/>
+        <v>15.714285714285715</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" s="3">
+        <v>75</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="19">
+        <v>0.18</v>
+      </c>
+      <c r="G19" s="21">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="H19" s="13">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333339</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="B20" s="3">
+        <v>96</v>
+      </c>
+      <c r="C20" s="3">
+        <v>18</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="19">
+        <v>2.29</v>
+      </c>
+      <c r="G20" s="21">
+        <f t="shared" si="0"/>
+        <v>0.1875</v>
+      </c>
+      <c r="H20" s="13">
+        <f t="shared" si="1"/>
+        <v>7.8602620087336241</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="40" t="s">
+        <v>169</v>
+      </c>
+      <c r="B21" s="3">
+        <v>206</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="19">
+        <v>0.4</v>
+      </c>
+      <c r="G21" s="21">
+        <f t="shared" si="0"/>
+        <v>1.2135922330097087E-2</v>
+      </c>
+      <c r="H21" s="13">
+        <f t="shared" si="1"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="11">
+        <v>185</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="49">
+        <v>0.33</v>
+      </c>
+      <c r="G22" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="43">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O22" s="52" t="s">
+        <v>245</v>
+      </c>
+      <c r="P22" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q22" s="15" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P23" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q23" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P24" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q24" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P25" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q25" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I26" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="J26" s="40" t="s">
         <v>201</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="K26" s="15" t="s">
         <v>202</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="L26" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="M26" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="P26" s="51" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q26" s="51" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I27" s="3"/>
+      <c r="J27" s="41">
+        <v>2750</v>
+      </c>
+      <c r="K27" s="41">
+        <v>160</v>
+      </c>
+      <c r="L27" s="41">
+        <v>92</v>
+      </c>
+      <c r="M27" s="41">
+        <v>40</v>
+      </c>
+      <c r="P27" s="51" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q27" s="51" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I28" s="15" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="40">
-        <v>2750</v>
-      </c>
-      <c r="B2" s="40" t="s">
+      <c r="J28" s="40" t="s">
+        <v>201</v>
+      </c>
+      <c r="K28" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="L28" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="M28" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="C2" s="40" t="s">
-        <v>205</v>
-      </c>
-      <c r="D2" s="40" t="s">
+      <c r="P28" s="51" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q28" s="51" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I29" s="3" t="s">
         <v>207</v>
       </c>
+      <c r="J29" s="3">
+        <f>J27*6</f>
+        <v>16500</v>
+      </c>
+      <c r="K29" s="3">
+        <f t="shared" ref="K29:M29" si="8">K27*6</f>
+        <v>960</v>
+      </c>
+      <c r="L29" s="3">
+        <f t="shared" si="8"/>
+        <v>552</v>
+      </c>
+      <c r="M29" s="3">
+        <f t="shared" si="8"/>
+        <v>240</v>
+      </c>
+      <c r="P29" s="51" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q29" s="51" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P30" s="51" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q30" s="51" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P31" s="51" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q31" s="51" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P32" s="51" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q32" s="51" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="33" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P33" s="51" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q33" s="51" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="34" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P34" s="51" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q34" s="51" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="35" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P35" s="51" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q35" s="51" t="s">
+        <v>243</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="O22" r:id="rId1" xr:uid="{FC8C911A-DFC8-416F-8E8E-2C5CBBC615A0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated food studies and added eoa docs
</commit_message>
<xml_diff>
--- a/extra/studio cibi proteici.xlsx
+++ b/extra/studio cibi proteici.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Documents\uni\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2B5A89-416F-4693-A088-70F2898BD0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAD1413-965C-4B3B-9EC3-A6CD3D880685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-3420" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="4" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -64,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="250">
   <si>
     <t>proteine</t>
   </si>
@@ -702,9 +713,6 @@
     <t>fiber</t>
   </si>
   <si>
-    <t>1/3 litro latte esse</t>
-  </si>
-  <si>
     <t>200g emmenthal</t>
   </si>
   <si>
@@ -805,6 +813,18 @@
   </si>
   <si>
     <t>100g (2) uova smart</t>
+  </si>
+  <si>
+    <t>proteine caseina myprotein (2.5kg)</t>
+  </si>
+  <si>
+    <t>1/3 litro latte intero esse</t>
+  </si>
+  <si>
+    <t>vegetable/ fruit (one piece or 100g)</t>
+  </si>
+  <si>
+    <t>carota (1p)</t>
   </si>
 </sst>
 </file>
@@ -815,7 +835,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-410]_-;\-* #,##0.00\ [$€-410]_-;_-* &quot;-&quot;??\ [$€-410]_-;_-@_-"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -860,6 +880,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1040,7 +1066,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1094,12 +1120,11 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1287,6 +1312,13 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1296,13 +1328,6 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1528,7 +1553,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{ECDFEEA9-AA58-4204-A8C7-634A63CB75E6}" name="Table2" displayName="Table2" ref="A1:H22" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{ECDFEEA9-AA58-4204-A8C7-634A63CB75E6}" name="Table2" displayName="Table2" ref="A1:H22" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
   <autoFilter ref="A1:H22" xr:uid="{ECDFEEA9-AA58-4204-A8C7-634A63CB75E6}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H22">
     <sortCondition descending="1" ref="H1:H22"/>
@@ -1551,10 +1576,31 @@
 </table>
 </file>
 
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{609641A4-1B41-4323-842C-EAE1B2CC5340}" name="Table3" displayName="Table3" ref="J1:O3" totalsRowShown="0">
+  <autoFilter ref="J1:O3" xr:uid="{609641A4-1B41-4323-842C-EAE1B2CC5340}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{AFFA0E04-5377-4ABC-A10E-5E9276D01F89}" name="vegetable/ fruit (one piece or 100g)"/>
+    <tableColumn id="2" xr3:uid="{14CCCA25-3E27-4EBE-9A0B-D763D2E26F7C}" name="cal">
+      <calculatedColumnFormula>41*0.75</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{A50C35CD-EFD1-4103-B4F8-F6EF213AD527}" name="pro"/>
+    <tableColumn id="4" xr3:uid="{6023BCD6-4DF2-4394-8650-24DB72E38C6E}" name="fat">
+      <calculatedColumnFormula>0.2*0.75</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{30C3AAC5-EBE2-4F02-B9C4-493716BB0A00}" name="fiber">
+      <calculatedColumnFormula>2.7*0.75</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{CF56D516-2CC9-4785-A42A-00DE8FC927E9}" name="eur"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1592,7 +1638,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1698,7 +1744,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1840,7 +1886,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1854,19 +1900,19 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="8" max="8" width="33.28515625" customWidth="1"/>
+    <col min="8" max="8" width="33.33203125" customWidth="1"/>
     <col min="13" max="13" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -1886,7 +1932,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -1926,7 +1972,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -1972,7 +2018,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -2021,7 +2067,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
@@ -2070,7 +2116,7 @@
         <v>1.6559999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>24</v>
       </c>
@@ -2119,7 +2165,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
@@ -2167,7 +2213,7 @@
         <v>4.5860000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
@@ -2189,7 +2235,7 @@
         <v>1.6877637130801688</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -2211,7 +2257,7 @@
         <v>2.8235294117647061</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
@@ -2251,7 +2297,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
@@ -2298,7 +2344,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
@@ -2350,7 +2396,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>21</v>
       </c>
@@ -2402,7 +2448,7 @@
         <v>1.6559999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>20</v>
       </c>
@@ -2443,7 +2489,7 @@
         <v>2.0205000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>5</v>
       </c>
@@ -2490,7 +2536,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>9</v>
       </c>
@@ -2525,7 +2571,7 @@
         <v>5.5164999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>10</v>
       </c>
@@ -2547,7 +2593,7 @@
         <v>3.7593984962406015</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>26</v>
       </c>
@@ -2569,7 +2615,7 @@
         <v>1.8950437317784257</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>28</v>
       </c>
@@ -2609,7 +2655,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
@@ -2657,7 +2703,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>27</v>
       </c>
@@ -2709,7 +2755,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>25</v>
       </c>
@@ -2761,7 +2807,7 @@
         <v>1.6559999999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>19</v>
       </c>
@@ -2802,7 +2848,7 @@
         <v>0.28299999999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>16</v>
       </c>
@@ -2841,7 +2887,7 @@
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>29</v>
       </c>
@@ -2876,7 +2922,7 @@
         <v>4.4490000000000007</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>86</v>
       </c>
@@ -2898,7 +2944,7 @@
         <v>3.1153846153846154</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D27" s="1"/>
       <c r="E27" s="2"/>
       <c r="J27" s="15" t="s">
@@ -2908,7 +2954,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D28" s="1"/>
       <c r="E28" s="2"/>
       <c r="H28" t="s">
@@ -2933,7 +2979,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D29" s="1"/>
       <c r="E29" s="2"/>
       <c r="H29" t="s">
@@ -2962,7 +3008,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D30" s="1"/>
       <c r="E30" s="2"/>
       <c r="H30" t="s">
@@ -2995,7 +3041,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="M31" s="15" t="s">
         <v>42</v>
       </c>
@@ -3012,7 +3058,7 @@
         <v>1.4407199999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="M32" s="15" t="s">
         <v>41</v>
       </c>
@@ -3029,7 +3075,7 @@
         <v>0.28299999999999997</v>
       </c>
     </row>
-    <row r="33" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C33" s="1"/>
       <c r="D33" s="2"/>
       <c r="H33" t="s">
@@ -3040,7 +3086,7 @@
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
     </row>
-    <row r="34" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C34" s="1"/>
       <c r="D34" s="2"/>
       <c r="H34" t="s">
@@ -3060,27 +3106,27 @@
         <v>4.2337199999999999</v>
       </c>
     </row>
-    <row r="35" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
       <c r="H35" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:16" x14ac:dyDescent="0.3">
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:16" x14ac:dyDescent="0.3">
       <c r="E38" s="2"/>
     </row>
-    <row r="39" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:16" x14ac:dyDescent="0.3">
       <c r="E39" s="2"/>
     </row>
-    <row r="40" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:16" x14ac:dyDescent="0.3">
       <c r="E40" s="2"/>
     </row>
   </sheetData>
@@ -3101,17 +3147,17 @@
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" customWidth="1"/>
-    <col min="21" max="21" width="22.42578125" customWidth="1"/>
-    <col min="23" max="23" width="12.42578125" customWidth="1"/>
-    <col min="24" max="24" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" customWidth="1"/>
+    <col min="11" max="11" width="18.44140625" customWidth="1"/>
+    <col min="21" max="21" width="22.44140625" customWidth="1"/>
+    <col min="23" max="23" width="12.44140625" customWidth="1"/>
+    <col min="24" max="24" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="K1" s="15"/>
       <c r="L1" s="15" t="s">
         <v>1</v>
@@ -3130,7 +3176,7 @@
       <c r="W1" s="24"/>
       <c r="X1" s="23"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>53</v>
       </c>
@@ -3171,7 +3217,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
@@ -3220,7 +3266,7 @@
       <c r="W3" s="25"/>
       <c r="X3" s="25"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>0</v>
       </c>
@@ -3264,7 +3310,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>40</v>
       </c>
@@ -3312,7 +3358,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="K6" s="15" t="s">
         <v>81</v>
       </c>
@@ -3325,7 +3371,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>78</v>
       </c>
@@ -3334,7 +3380,7 @@
         <v>1943.0857142857144</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>79</v>
       </c>
@@ -3343,7 +3389,7 @@
         <v>151.56428571428572</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>80</v>
       </c>
@@ -3352,7 +3398,7 @@
         <v>4.1071428571428568</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>69</v>
       </c>
@@ -3402,7 +3448,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>63</v>
       </c>
@@ -3460,7 +3506,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>65</v>
       </c>
@@ -3522,7 +3568,7 @@
         <v>1.54</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>66</v>
       </c>
@@ -3584,7 +3630,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>67</v>
       </c>
@@ -3636,7 +3682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>70</v>
       </c>
@@ -3698,7 +3744,7 @@
         <v>4.0500000000000007</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>75</v>
       </c>
@@ -3736,7 +3782,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>63</v>
       </c>
@@ -3780,7 +3826,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>77</v>
       </c>
@@ -3827,7 +3873,7 @@
         <v>1.54</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
         <v>66</v>
       </c>
@@ -3874,7 +3920,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="15"/>
       <c r="B25" s="3">
         <v>0</v>
@@ -3911,7 +3957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
         <v>70</v>
       </c>
@@ -3975,19 +4021,19 @@
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" customWidth="1"/>
-    <col min="14" max="14" width="22.28515625" customWidth="1"/>
-    <col min="15" max="15" width="9.85546875" customWidth="1"/>
-    <col min="19" max="19" width="21.28515625" customWidth="1"/>
-    <col min="20" max="20" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.33203125" customWidth="1"/>
+    <col min="14" max="14" width="22.33203125" customWidth="1"/>
+    <col min="15" max="15" width="9.88671875" customWidth="1"/>
+    <col min="19" max="19" width="21.33203125" customWidth="1"/>
+    <col min="20" max="20" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>45</v>
       </c>
@@ -4023,7 +4069,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -4069,7 +4115,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -4116,7 +4162,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -4163,7 +4209,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B5">
         <f>SUM(B2:B4)</f>
         <v>1978</v>
@@ -4204,7 +4250,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F6" s="15" t="s">
         <v>68</v>
       </c>
@@ -4235,7 +4281,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>96</v>
       </c>
@@ -4269,7 +4315,7 @@
         <v>88.461538461538453</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>98</v>
       </c>
@@ -4327,7 +4373,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>97</v>
       </c>
@@ -4385,7 +4431,7 @@
         <v>45.625</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>70</v>
       </c>
@@ -4443,7 +4489,7 @@
         <v>50.625</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F11" s="15" t="s">
         <v>110</v>
       </c>
@@ -4486,7 +4532,7 @@
         <v>30.932203389830509</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>96</v>
       </c>
@@ -4541,7 +4587,7 @@
         <v>34.745762711864408</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>100</v>
       </c>
@@ -4578,7 +4624,7 @@
         <v>27.738095238095241</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>99</v>
       </c>
@@ -4615,7 +4661,7 @@
         <v>32.999999999999993</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>70</v>
       </c>
@@ -4652,7 +4698,7 @@
         <v>25.306122448979593</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F16" s="15" t="s">
         <v>153</v>
       </c>
@@ -4674,7 +4720,7 @@
         <v>32.765957446808514</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>96</v>
       </c>
@@ -4708,7 +4754,7 @@
         <v>44.749999999999993</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>100</v>
       </c>
@@ -4745,7 +4791,7 @@
         <v>6.25</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>102</v>
       </c>
@@ -4782,7 +4828,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>63</v>
       </c>
@@ -4818,7 +4864,7 @@
         <v>17.045454545454547</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>101</v>
       </c>
@@ -4858,7 +4904,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>70</v>
       </c>
@@ -4919,7 +4965,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="F23" s="15" t="s">
         <v>179</v>
       </c>
@@ -4971,7 +5017,7 @@
         <v>1.6800000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="F24" s="15" t="s">
         <v>182</v>
       </c>
@@ -5023,7 +5069,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
         <v>136</v>
       </c>
@@ -5087,7 +5133,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
         <v>101</v>
       </c>
@@ -5154,7 +5200,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>63</v>
       </c>
@@ -5203,7 +5249,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>137</v>
       </c>
@@ -5247,7 +5293,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>139</v>
       </c>
@@ -5275,7 +5321,7 @@
       <c r="U29" s="3"/>
       <c r="V29" s="19"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
         <v>138</v>
       </c>
@@ -5322,13 +5368,13 @@
         <v>3.43</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31" s="15"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
         <v>134</v>
       </c>
@@ -5369,7 +5415,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="M33" t="s">
         <v>121</v>
       </c>
@@ -5407,7 +5453,7 @@
         <v>1.6519999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="N34" s="15" t="s">
         <v>122</v>
       </c>
@@ -5439,7 +5485,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="N35" s="15" t="s">
         <v>117</v>
       </c>
@@ -5471,7 +5517,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36" s="15" t="s">
         <v>136</v>
       </c>
@@ -5515,7 +5561,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A37" s="15" t="s">
         <v>101</v>
       </c>
@@ -5559,7 +5605,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38" s="15" t="s">
         <v>63</v>
       </c>
@@ -5583,7 +5629,7 @@
       <c r="U38" s="3"/>
       <c r="V38" s="19"/>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39" s="15" t="s">
         <v>137</v>
       </c>
@@ -5608,7 +5654,7 @@
       <c r="U39" s="3"/>
       <c r="V39" s="19"/>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A40" s="15" t="s">
         <v>140</v>
       </c>
@@ -5655,7 +5701,7 @@
         <v>3.4670000000000005</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A41" s="15" t="s">
         <v>138</v>
       </c>
@@ -5685,7 +5731,7 @@
       </c>
       <c r="S41" s="32"/>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A42" s="15"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -5715,7 +5761,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A43" s="15" t="s">
         <v>134</v>
       </c>
@@ -5759,7 +5805,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
       <c r="S44" s="15" t="s">
         <v>134</v>
       </c>
@@ -5776,7 +5822,7 @@
         <v>3.9070000000000005</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A45" s="15" t="s">
         <v>147</v>
       </c>
@@ -5814,7 +5860,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A46" s="15" t="s">
         <v>131</v>
       </c>
@@ -5873,7 +5919,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A47" s="15" t="s">
         <v>114</v>
       </c>
@@ -5935,7 +5981,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A48" s="15" t="s">
         <v>142</v>
       </c>
@@ -5997,7 +6043,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A49" s="15" t="s">
         <v>101</v>
       </c>
@@ -6059,7 +6105,7 @@
         <v>3.8270000000000004</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A50" s="15" t="s">
         <v>138</v>
       </c>
@@ -6095,7 +6141,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A51" s="15"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -6120,7 +6166,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A52" s="15"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -6134,7 +6180,7 @@
       <c r="P52" s="3"/>
       <c r="Q52" s="19"/>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A53" s="15" t="s">
         <v>70</v>
       </c>
@@ -6181,7 +6227,7 @@
         <v>4.9633333333333329</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A55" s="15" t="s">
         <v>143</v>
       </c>
@@ -6219,7 +6265,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A56" s="15"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -6255,7 +6301,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A57" s="15" t="s">
         <v>108</v>
       </c>
@@ -6296,7 +6342,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A58" s="15"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -6329,7 +6375,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A59" s="15" t="s">
         <v>134</v>
       </c>
@@ -6376,13 +6422,13 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.3">
       <c r="N60" s="15"/>
       <c r="O60" s="3"/>
       <c r="P60" s="3"/>
       <c r="Q60" s="19"/>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A61" s="15" t="s">
         <v>144</v>
       </c>
@@ -6412,7 +6458,7 @@
       <c r="P61" s="3"/>
       <c r="Q61" s="3"/>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A62" s="15" t="s">
         <v>141</v>
       </c>
@@ -6459,7 +6505,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A63" s="15"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -6495,7 +6541,7 @@
         <v>4.41</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A64" s="15"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -6513,7 +6559,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="15" t="s">
         <v>134</v>
       </c>
@@ -6557,7 +6603,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N66" s="15" t="s">
         <v>138</v>
       </c>
@@ -6574,7 +6620,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="15" t="s">
         <v>149</v>
       </c>
@@ -6615,7 +6661,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="15" t="s">
         <v>150</v>
       </c>
@@ -6662,7 +6708,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="15"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -6698,7 +6744,7 @@
         <v>1.68</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="15"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -6734,7 +6780,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="15" t="s">
         <v>134</v>
       </c>
@@ -6781,7 +6827,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N72" s="15" t="s">
         <v>167</v>
       </c>
@@ -6798,7 +6844,7 @@
         <v>0.245</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="15" t="s">
         <v>151</v>
       </c>
@@ -6827,7 +6873,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="15" t="s">
         <v>152</v>
       </c>
@@ -6856,7 +6902,7 @@
         <v>4.4783333333333335</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="15" t="s">
         <v>142</v>
       </c>
@@ -6873,7 +6919,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" s="15" t="s">
         <v>154</v>
       </c>
@@ -6890,7 +6936,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" s="15" t="s">
         <v>134</v>
       </c>
@@ -6907,7 +6953,7 @@
         <v>3.9420000000000002</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" s="15" t="s">
         <v>173</v>
       </c>
@@ -6933,7 +6979,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="36" t="s">
         <v>174</v>
       </c>
@@ -6965,7 +7011,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="36" t="s">
         <v>138</v>
       </c>
@@ -6997,7 +7043,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="15" t="s">
         <v>101</v>
       </c>
@@ -7029,7 +7075,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="15" t="s">
         <v>168</v>
       </c>
@@ -7061,7 +7107,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="37" t="s">
         <v>165</v>
       </c>
@@ -7093,7 +7139,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="37" t="s">
         <v>176</v>
       </c>
@@ -7125,7 +7171,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="15"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -7146,7 +7192,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="15"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -7156,7 +7202,7 @@
       <c r="H88" s="3"/>
       <c r="I88" s="19"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="15"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -7166,7 +7212,7 @@
       <c r="H89" s="3"/>
       <c r="I89" s="19"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="15"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -7176,7 +7222,7 @@
       <c r="H90" s="3"/>
       <c r="I90" s="19"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="15" t="s">
         <v>134</v>
       </c>
@@ -7208,7 +7254,7 @@
         <v>4.7633333333333336</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="15" t="s">
         <v>173</v>
       </c>
@@ -7234,7 +7280,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="36" t="s">
         <v>174</v>
       </c>
@@ -7266,7 +7312,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="36" t="s">
         <v>138</v>
       </c>
@@ -7298,7 +7344,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="15" t="s">
         <v>101</v>
       </c>
@@ -7330,7 +7376,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="15" t="s">
         <v>168</v>
       </c>
@@ -7362,7 +7408,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="37" t="s">
         <v>165</v>
       </c>
@@ -7394,7 +7440,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="37" t="s">
         <v>181</v>
       </c>
@@ -7426,7 +7472,7 @@
         <v>1.125</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="15"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
@@ -7444,7 +7490,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="15"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
@@ -7454,7 +7500,7 @@
       <c r="H101" s="3"/>
       <c r="I101" s="19"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="15"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
@@ -7464,7 +7510,7 @@
       <c r="H102" s="3"/>
       <c r="I102" s="19"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="15"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
@@ -7474,7 +7520,7 @@
       <c r="H103" s="3"/>
       <c r="I103" s="19"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="15" t="s">
         <v>134</v>
       </c>
@@ -7506,7 +7552,7 @@
         <v>4.708333333333333</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="15" t="s">
         <v>173</v>
       </c>
@@ -7532,7 +7578,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" s="36" t="s">
         <v>174</v>
       </c>
@@ -7564,7 +7610,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" s="36" t="s">
         <v>138</v>
       </c>
@@ -7596,7 +7642,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" s="15" t="s">
         <v>101</v>
       </c>
@@ -7628,7 +7674,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" s="15" t="s">
         <v>168</v>
       </c>
@@ -7660,7 +7706,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" s="37" t="s">
         <v>165</v>
       </c>
@@ -7692,7 +7738,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" s="37" t="s">
         <v>185</v>
       </c>
@@ -7724,7 +7770,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="15"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
@@ -7745,7 +7791,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" s="15"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
@@ -7755,7 +7801,7 @@
       <c r="H114" s="3"/>
       <c r="I114" s="19"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" s="15"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
@@ -7765,7 +7811,7 @@
       <c r="H115" s="3"/>
       <c r="I115" s="19"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" s="15"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
@@ -7775,7 +7821,7 @@
       <c r="H116" s="3"/>
       <c r="I116" s="19"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" s="15" t="s">
         <v>134</v>
       </c>
@@ -7807,7 +7853,7 @@
         <v>4.5458333333333334</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" s="15" t="s">
         <v>173</v>
       </c>
@@ -7833,7 +7879,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" s="36" t="s">
         <v>174</v>
       </c>
@@ -7865,7 +7911,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" s="36" t="s">
         <v>138</v>
       </c>
@@ -7897,7 +7943,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" s="15" t="s">
         <v>101</v>
       </c>
@@ -7929,7 +7975,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" s="15" t="s">
         <v>168</v>
       </c>
@@ -7961,7 +8007,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" s="37" t="s">
         <v>165</v>
       </c>
@@ -7993,7 +8039,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" s="37" t="s">
         <v>138</v>
       </c>
@@ -8025,7 +8071,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" s="15"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
@@ -8046,7 +8092,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="15"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
@@ -8056,7 +8102,7 @@
       <c r="H127" s="3"/>
       <c r="I127" s="19"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" s="15"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
@@ -8066,7 +8112,7 @@
       <c r="H128" s="3"/>
       <c r="I128" s="19"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="15"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
@@ -8076,7 +8122,7 @@
       <c r="H129" s="3"/>
       <c r="I129" s="19"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" s="15" t="s">
         <v>134</v>
       </c>
@@ -8123,14 +8169,14 @@
       <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
-    <col min="13" max="13" width="19.28515625" customWidth="1"/>
+    <col min="13" max="13" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="15" t="s">
         <v>45</v>
@@ -8148,7 +8194,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>62</v>
       </c>
@@ -8170,7 +8216,7 @@
         <v>27.52293577981651</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>63</v>
       </c>
@@ -8190,7 +8236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>68</v>
       </c>
@@ -8236,7 +8282,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>30</v>
       </c>
@@ -8288,7 +8334,7 @@
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>103</v>
       </c>
@@ -8340,7 +8386,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>104</v>
       </c>
@@ -8392,7 +8438,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>109</v>
       </c>
@@ -8444,7 +8490,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>110</v>
       </c>
@@ -8484,7 +8530,7 @@
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>111</v>
       </c>
@@ -8536,7 +8582,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>155</v>
       </c>
@@ -8588,7 +8634,7 @@
         <v>4.75</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>112</v>
       </c>
@@ -8610,7 +8656,7 @@
         <v>32.999999999999993</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
         <v>116</v>
       </c>
@@ -8635,7 +8681,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>153</v>
       </c>
@@ -8660,7 +8706,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>163</v>
       </c>
@@ -8685,7 +8731,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>169</v>
       </c>
@@ -8710,7 +8756,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>170</v>
       </c>
@@ -8732,7 +8778,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>171</v>
       </c>
@@ -8754,7 +8800,7 @@
         <v>17.045454545454547</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>172</v>
       </c>
@@ -8776,7 +8822,7 @@
         <v>7.8602620087336241</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>175</v>
       </c>
@@ -8798,7 +8844,7 @@
         <v>22.891566265060241</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>179</v>
       </c>
@@ -8820,7 +8866,7 @@
         <v>15.714285714285715</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>182</v>
       </c>
@@ -8842,7 +8888,7 @@
         <v>24.444444444444443</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>183</v>
       </c>
@@ -8864,7 +8910,7 @@
         <v>37.333333333333336</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
         <v>186</v>
       </c>
@@ -8886,7 +8932,7 @@
         <v>29.571428571428573</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
         <v>189</v>
       </c>
@@ -8908,7 +8954,7 @@
         <v>15.789473684210526</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
         <v>190</v>
       </c>
@@ -8930,7 +8976,7 @@
         <v>43.75</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="39" t="s">
         <v>197</v>
       </c>
@@ -8938,7 +8984,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="39" t="s">
         <v>198</v>
       </c>
@@ -8953,24 +8999,25 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{715CF0DF-138B-4B49-BC97-299FF5018F54}">
-  <dimension ref="A1:U35"/>
+  <dimension ref="A1:W34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="26" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="29.88671875" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" style="26" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" customWidth="1"/>
+    <col min="10" max="10" width="33.21875" customWidth="1"/>
     <col min="13" max="13" width="12" customWidth="1"/>
-    <col min="16" max="16" width="22" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" style="26"/>
+    <col min="18" max="18" width="22" customWidth="1"/>
+    <col min="23" max="23" width="9.109375" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
         <v>208</v>
       </c>
@@ -8986,7 +9033,7 @@
       <c r="E1" s="45" t="s">
         <v>211</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="47" t="s">
         <v>87</v>
       </c>
       <c r="G1" s="45" t="s">
@@ -8995,8 +9042,26 @@
       <c r="H1" s="46" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="J1" s="51" t="s">
+        <v>248</v>
+      </c>
+      <c r="K1" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="M1" s="51" t="s">
+        <v>209</v>
+      </c>
+      <c r="N1" s="51" t="s">
+        <v>211</v>
+      </c>
+      <c r="O1" s="51" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
         <v>110</v>
       </c>
@@ -9012,18 +9077,39 @@
         <v>0.22</v>
       </c>
       <c r="G2" s="21">
-        <f t="shared" ref="G2:G22" si="0">C2/B2</f>
+        <f>C2/B2</f>
         <v>6.2200956937799042E-2</v>
       </c>
       <c r="H2" s="21">
-        <f t="shared" ref="H2:H22" si="1">C2/F2</f>
+        <f>C2/F2</f>
         <v>59.090909090909093</v>
       </c>
-      <c r="P2" t="s">
+      <c r="J2" t="s">
+        <v>249</v>
+      </c>
+      <c r="K2">
+        <f>41*0.75</f>
+        <v>30.75</v>
+      </c>
+      <c r="L2">
+        <v>0.75</v>
+      </c>
+      <c r="M2">
+        <f>0.2*0.75</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="N2">
+        <f>2.7*0.75</f>
+        <v>2.0250000000000004</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="R2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="40" t="s">
         <v>163</v>
       </c>
@@ -9039,601 +9125,615 @@
         <v>0.4</v>
       </c>
       <c r="G3" s="21">
-        <f t="shared" si="0"/>
+        <f>C3/B3</f>
         <v>0.14206349206349206</v>
       </c>
       <c r="H3" s="21">
-        <f t="shared" si="1"/>
+        <f>C3/F3</f>
         <v>44.749999999999993</v>
       </c>
-      <c r="P3" s="15" t="s">
+      <c r="K3">
+        <f>41*0.75</f>
+        <v>30.75</v>
+      </c>
+      <c r="M3">
+        <f>0.2*0.75</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="N3">
+        <f>2.7*0.75</f>
+        <v>2.0250000000000004</v>
+      </c>
+      <c r="R3" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="Q3" s="15" t="s">
+      <c r="S3" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="R3" s="15" t="s">
+      <c r="T3" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="S3" s="15" t="s">
+      <c r="U3" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="T3" s="15" t="s">
+      <c r="V3" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="U3" s="50" t="s">
+      <c r="W3" s="49" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="40" t="s">
-        <v>183</v>
+        <v>246</v>
       </c>
       <c r="B4" s="3">
-        <v>382</v>
+        <v>358</v>
       </c>
       <c r="C4" s="3">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="D4" s="3">
-        <v>30</v>
+        <v>1.2</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="22">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="G4" s="21">
+        <f>C4/B4</f>
+        <v>0.22905027932960895</v>
+      </c>
+      <c r="H4" s="21">
+        <f>C4/F4</f>
+        <v>40.796019900497519</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="S4" s="3">
+        <f>B13</f>
+        <v>136</v>
+      </c>
+      <c r="T4" s="3">
+        <f t="shared" ref="T4:W4" si="0">C13</f>
+        <v>12.4</v>
+      </c>
+      <c r="U4" s="3">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
+      <c r="V4" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A5" s="40" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" s="3">
+        <v>382</v>
+      </c>
+      <c r="C5" s="3">
+        <v>28</v>
+      </c>
+      <c r="D5" s="3">
+        <v>30</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="22">
         <v>0.75</v>
       </c>
-      <c r="G4" s="21">
-        <f t="shared" si="0"/>
+      <c r="G5" s="21">
+        <f>C5/B5</f>
         <v>7.3298429319371722E-2</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H5" s="13">
+        <f>C5/F5</f>
+        <v>37.333333333333336</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="S5" s="3">
+        <f>B7*3.33</f>
+        <v>216.45000000000002</v>
+      </c>
+      <c r="T5" s="3">
+        <f t="shared" ref="T5:W5" si="1">C7*3.33</f>
+        <v>10.988999999999999</v>
+      </c>
+      <c r="U5" s="3">
         <f t="shared" si="1"/>
-        <v>37.333333333333336</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="Q4" s="3">
-        <f>B12</f>
-        <v>136</v>
-      </c>
-      <c r="R4" s="3">
-        <f>C12</f>
-        <v>12.4</v>
-      </c>
-      <c r="S4" s="3">
-        <f t="shared" ref="S4:U4" si="2">D12</f>
-        <v>9.5</v>
-      </c>
-      <c r="T4" s="3">
-        <f t="shared" si="2"/>
+        <v>11.988000000000001</v>
+      </c>
+      <c r="V5" s="3">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U4" s="19">
-        <f t="shared" si="2"/>
-        <v>0.49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
+      <c r="W5" s="3">
+        <f t="shared" si="1"/>
+        <v>0.33300000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A6" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B6" s="3">
         <v>51</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C6" s="3">
         <v>5.3</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D6" s="3">
         <v>0.1</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="19">
-        <v>0.15</v>
-      </c>
-      <c r="G5" s="21">
-        <f t="shared" si="0"/>
-        <v>0.10392156862745097</v>
-      </c>
-      <c r="H5" s="13">
-        <f t="shared" si="1"/>
-        <v>35.333333333333336</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="Q5" s="3">
-        <f>B6*3.33</f>
-        <v>216.45000000000002</v>
-      </c>
-      <c r="R5" s="3">
-        <f t="shared" ref="R5:U5" si="3">C6*3.33</f>
-        <v>10.988999999999999</v>
-      </c>
-      <c r="S5" s="3">
-        <f t="shared" si="3"/>
-        <v>11.988000000000001</v>
-      </c>
-      <c r="T5" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U5" s="19">
-        <f t="shared" si="3"/>
-        <v>0.33300000000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="40" t="s">
-        <v>216</v>
-      </c>
-      <c r="B6" s="3">
-        <v>65</v>
-      </c>
-      <c r="C6" s="3">
-        <v>3.3</v>
-      </c>
-      <c r="D6" s="3">
-        <v>3.6</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="19">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="G6" s="21">
-        <f t="shared" si="0"/>
-        <v>5.0769230769230768E-2</v>
+        <f>C6/B6</f>
+        <v>0.10392156862745097</v>
       </c>
       <c r="H6" s="13">
-        <f t="shared" si="1"/>
-        <v>32.999999999999993</v>
-      </c>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
+        <f>C6/F6</f>
+        <v>35.333333333333336</v>
+      </c>
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
-      <c r="U6" s="19"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="19"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="40" t="s">
-        <v>153</v>
+        <v>215</v>
       </c>
       <c r="B7" s="3">
-        <v>169</v>
+        <v>65</v>
       </c>
       <c r="C7" s="3">
-        <v>15.4</v>
-      </c>
-      <c r="D7" s="3"/>
+        <v>3.3</v>
+      </c>
+      <c r="D7" s="3">
+        <v>3.6</v>
+      </c>
       <c r="E7" s="3"/>
       <c r="F7" s="19">
-        <v>0.47</v>
+        <v>0.1</v>
       </c>
       <c r="G7" s="21">
-        <f t="shared" si="0"/>
-        <v>9.1124260355029588E-2</v>
+        <f>C7/B7</f>
+        <v>5.0769230769230768E-2</v>
       </c>
       <c r="H7" s="13">
-        <f t="shared" si="1"/>
-        <v>32.765957446808514</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="Q7" s="3">
-        <f>B10*2</f>
+        <f>C7/F7</f>
+        <v>32.999999999999993</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="S7" s="3">
+        <f>B11*2</f>
         <v>200</v>
       </c>
-      <c r="R7" s="3">
-        <f t="shared" ref="R7:U7" si="4">C10*2</f>
+      <c r="T7" s="3">
+        <f t="shared" ref="T7:W7" si="2">C11*2</f>
         <v>46.6</v>
       </c>
-      <c r="S7" s="3">
-        <f t="shared" si="4"/>
+      <c r="U7" s="3">
+        <f t="shared" si="2"/>
         <v>1.6</v>
       </c>
-      <c r="T7" s="3">
-        <f t="shared" si="4"/>
+      <c r="V7" s="3">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U7" s="3">
-        <f t="shared" si="4"/>
+      <c r="W7" s="3">
+        <f t="shared" si="2"/>
         <v>1.6</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="40" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="B8" s="3">
-        <v>115</v>
+        <v>169</v>
       </c>
       <c r="C8" s="3">
-        <v>9</v>
+        <v>15.4</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="19">
+        <v>0.47</v>
+      </c>
+      <c r="G8" s="21">
+        <f>C8/B8</f>
+        <v>9.1124260355029588E-2</v>
+      </c>
+      <c r="H8" s="13">
+        <f>C8/F8</f>
+        <v>32.765957446808514</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="S8" s="3">
+        <f>B5*2</f>
+        <v>764</v>
+      </c>
+      <c r="T8" s="3">
+        <f t="shared" ref="T8:W8" si="3">C5*2</f>
+        <v>56</v>
+      </c>
+      <c r="U8" s="3">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="V8" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="W8" s="3">
+        <f t="shared" si="3"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A9" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B9" s="11">
+        <v>115</v>
+      </c>
+      <c r="C9" s="11">
+        <v>9</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="48">
         <v>0.3</v>
       </c>
-      <c r="G8" s="21">
-        <f t="shared" si="0"/>
+      <c r="G9" s="30">
+        <f>C9/B9</f>
         <v>7.8260869565217397E-2</v>
       </c>
-      <c r="H8" s="13">
-        <f t="shared" si="1"/>
+      <c r="H9" s="43">
+        <f>C9/F9</f>
         <v>30</v>
       </c>
-      <c r="P8" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q8" s="3">
-        <f>B4*2</f>
-        <v>764</v>
-      </c>
-      <c r="R8" s="3">
-        <f t="shared" ref="R8:U8" si="5">C4*2</f>
-        <v>56</v>
-      </c>
-      <c r="S8" s="3">
-        <f t="shared" si="5"/>
-        <v>60</v>
-      </c>
-      <c r="T8" s="3">
-        <f t="shared" si="5"/>
+      <c r="R9" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="S9" s="3">
+        <f>B6*5</f>
+        <v>255</v>
+      </c>
+      <c r="T9" s="3">
+        <f t="shared" ref="T9:W9" si="4">C6*5</f>
+        <v>26.5</v>
+      </c>
+      <c r="U9" s="3">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="V9" s="3">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U8" s="3">
-        <f t="shared" si="5"/>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="42" t="s">
+      <c r="W9" s="3">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A10" s="40" t="s">
         <v>186</v>
       </c>
-      <c r="B9" s="30">
+      <c r="B10" s="21">
         <v>146</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C10" s="21">
         <v>20.7</v>
       </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="47">
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="22">
         <v>0.7</v>
       </c>
-      <c r="G9" s="30">
-        <f t="shared" si="0"/>
+      <c r="G10" s="21">
+        <f>C10/B10</f>
         <v>0.14178082191780822</v>
       </c>
-      <c r="H9" s="43">
-        <f t="shared" si="1"/>
+      <c r="H10" s="13">
+        <f>C10/F10</f>
         <v>29.571428571428573</v>
       </c>
-      <c r="P9" s="18" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q9" s="3">
-        <f>B5*5</f>
-        <v>255</v>
-      </c>
-      <c r="R9" s="3">
-        <f t="shared" ref="R9:U9" si="6">C5*5</f>
-        <v>26.5</v>
-      </c>
-      <c r="S9" s="3">
-        <f t="shared" si="6"/>
-        <v>0.5</v>
-      </c>
-      <c r="T9" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="U9" s="3">
-        <f t="shared" si="6"/>
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="40" t="s">
-        <v>155</v>
-      </c>
-      <c r="B10" s="3">
-        <v>100</v>
-      </c>
-      <c r="C10" s="3">
-        <v>23.3</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="19">
-        <v>0.8</v>
-      </c>
-      <c r="G10" s="21">
-        <f t="shared" si="0"/>
-        <v>0.23300000000000001</v>
-      </c>
-      <c r="H10" s="13">
-        <f t="shared" si="1"/>
-        <v>29.125</v>
-      </c>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
-      <c r="U10" s="19"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="19"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="40" t="s">
-        <v>62</v>
+        <v>155</v>
       </c>
       <c r="B11" s="3">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="C11" s="3">
-        <v>30</v>
-      </c>
-      <c r="D11" s="3"/>
+        <v>23.3</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.8</v>
+      </c>
       <c r="E11" s="3"/>
       <c r="F11" s="19">
-        <v>1.0900000000000001</v>
+        <v>0.8</v>
       </c>
       <c r="G11" s="21">
-        <f t="shared" si="0"/>
-        <v>0.24390243902439024</v>
+        <f>C11/B11</f>
+        <v>0.23300000000000001</v>
       </c>
       <c r="H11" s="13">
-        <f t="shared" si="1"/>
-        <v>27.52293577981651</v>
-      </c>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
+        <f>C11/F11</f>
+        <v>29.125</v>
+      </c>
       <c r="R11" s="3"/>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
-      <c r="U11" s="19"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="19"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="40" t="s">
-        <v>116</v>
+        <v>62</v>
       </c>
       <c r="B12" s="3">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="C12" s="3">
-        <v>12.4</v>
-      </c>
-      <c r="D12" s="3">
-        <v>9.5</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="19">
-        <v>0.49</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="G12" s="21">
-        <f t="shared" si="0"/>
-        <v>9.1176470588235303E-2</v>
+        <f>C12/B12</f>
+        <v>0.24390243902439024</v>
       </c>
       <c r="H12" s="13">
-        <f t="shared" si="1"/>
-        <v>25.306122448979593</v>
-      </c>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
+        <f>C12/F12</f>
+        <v>27.52293577981651</v>
+      </c>
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
-      <c r="U12" s="19"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="19"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="40" t="s">
-        <v>182</v>
+        <v>116</v>
       </c>
       <c r="B13" s="3">
-        <v>315</v>
+        <v>136</v>
       </c>
       <c r="C13" s="3">
-        <v>22</v>
-      </c>
-      <c r="D13" s="3"/>
+        <v>12.4</v>
+      </c>
+      <c r="D13" s="3">
+        <v>9.5</v>
+      </c>
       <c r="E13" s="3"/>
-      <c r="F13" s="22">
-        <v>0.9</v>
+      <c r="F13" s="19">
+        <v>0.49</v>
       </c>
       <c r="G13" s="21">
-        <f t="shared" si="0"/>
-        <v>6.9841269841269843E-2</v>
+        <f>C13/B13</f>
+        <v>9.1176470588235303E-2</v>
       </c>
       <c r="H13" s="13">
-        <f t="shared" si="1"/>
-        <v>24.444444444444443</v>
-      </c>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
+        <f>C13/F13</f>
+        <v>25.306122448979593</v>
+      </c>
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
-      <c r="U13" s="19"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="19"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="40" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="B14" s="3">
-        <v>331</v>
+        <v>315</v>
       </c>
       <c r="C14" s="3">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="19">
-        <v>0.83</v>
+      <c r="F14" s="22">
+        <v>0.9</v>
       </c>
       <c r="G14" s="21">
-        <f t="shared" si="0"/>
-        <v>5.7401812688821753E-2</v>
+        <f>C14/B14</f>
+        <v>6.9841269841269843E-2</v>
       </c>
       <c r="H14" s="13">
-        <f t="shared" si="1"/>
-        <v>22.891566265060241</v>
-      </c>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
+        <f>C14/F14</f>
+        <v>24.444444444444443</v>
+      </c>
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
-      <c r="U14" s="19"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="19"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="40" t="s">
-        <v>111</v>
+        <v>175</v>
       </c>
       <c r="B15" s="3">
-        <v>84</v>
+        <v>331</v>
       </c>
       <c r="C15" s="3">
-        <v>16.7</v>
+        <v>19</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="19">
-        <v>0.8</v>
+        <v>0.83</v>
       </c>
       <c r="G15" s="21">
-        <f t="shared" si="0"/>
-        <v>0.1988095238095238</v>
+        <f>C15/B15</f>
+        <v>5.7401812688821753E-2</v>
       </c>
       <c r="H15" s="13">
-        <f t="shared" si="1"/>
-        <v>20.874999999999996</v>
-      </c>
-      <c r="P15" s="15" t="s">
+        <f>C15/F15</f>
+        <v>22.891566265060241</v>
+      </c>
+      <c r="R15" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="Q15" s="15">
-        <f>SUM(Q4:Q14)</f>
+      <c r="S15" s="15">
+        <f>SUM(S4:S14)</f>
         <v>1571.45</v>
       </c>
-      <c r="R15" s="15">
-        <f t="shared" ref="R15:U15" si="7">SUM(R4:R14)</f>
+      <c r="T15" s="15">
+        <f t="shared" ref="T15:W15" si="5">SUM(T4:T14)</f>
         <v>152.489</v>
       </c>
-      <c r="S15" s="15">
-        <f t="shared" si="7"/>
+      <c r="U15" s="15">
+        <f t="shared" si="5"/>
         <v>83.587999999999994</v>
       </c>
-      <c r="T15" s="15">
-        <f t="shared" si="7"/>
+      <c r="V15" s="15">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="U15" s="15">
-        <f t="shared" si="7"/>
+      <c r="W15" s="15">
+        <f t="shared" si="5"/>
         <v>4.673</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="40" t="s">
-        <v>171</v>
+        <v>111</v>
       </c>
       <c r="B16" s="3">
-        <v>180</v>
+        <v>84</v>
       </c>
       <c r="C16" s="3">
-        <v>15</v>
+        <v>16.7</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="19">
-        <v>0.88</v>
+        <v>0.8</v>
       </c>
       <c r="G16" s="21">
-        <f t="shared" si="0"/>
-        <v>8.3333333333333329E-2</v>
+        <f>C16/B16</f>
+        <v>0.1988095238095238</v>
       </c>
       <c r="H16" s="13">
-        <f t="shared" si="1"/>
-        <v>17.045454545454547</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+        <f>C16/F16</f>
+        <v>20.874999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="40" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="B17" s="3">
-        <v>350</v>
+        <v>180</v>
       </c>
       <c r="C17" s="3">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="19">
+        <v>0.88</v>
+      </c>
+      <c r="G17" s="21">
+        <f>C17/B17</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="H17" s="13">
+        <f>C17/F17</f>
+        <v>17.045454545454547</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="B18" s="3">
+        <v>350</v>
+      </c>
+      <c r="C18" s="3">
+        <v>3</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="19">
         <v>0.19</v>
       </c>
-      <c r="G17" s="21">
-        <f t="shared" si="0"/>
+      <c r="G18" s="21">
+        <f>C18/B18</f>
         <v>8.5714285714285719E-3</v>
       </c>
-      <c r="H17" s="13">
-        <f t="shared" si="1"/>
+      <c r="H18" s="13">
+        <f>C18/F18</f>
         <v>15.789473684210526</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="40" t="s">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="40" t="s">
         <v>179</v>
       </c>
-      <c r="B18" s="21">
+      <c r="B19" s="21">
         <v>49</v>
       </c>
-      <c r="C18" s="21">
+      <c r="C19" s="21">
         <v>5.5</v>
       </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="19">
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="19">
         <v>0.35</v>
       </c>
-      <c r="G18" s="21">
-        <f t="shared" si="0"/>
+      <c r="G19" s="21">
+        <f>C19/B19</f>
         <v>0.11224489795918367</v>
       </c>
-      <c r="H18" s="13">
-        <f t="shared" si="1"/>
+      <c r="H19" s="13">
+        <f>C19/F19</f>
         <v>15.714285714285715</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="B19" s="3">
-        <v>75</v>
-      </c>
-      <c r="C19" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="19">
-        <v>0.18</v>
-      </c>
-      <c r="G19" s="21">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-      <c r="H19" s="13">
-        <f t="shared" si="1"/>
-        <v>8.3333333333333339</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="40" t="s">
         <v>172</v>
       </c>
@@ -9649,39 +9749,48 @@
         <v>2.29</v>
       </c>
       <c r="G20" s="21">
-        <f t="shared" si="0"/>
+        <f>C20/B20</f>
         <v>0.1875</v>
       </c>
       <c r="H20" s="13">
-        <f t="shared" si="1"/>
+        <f>C20/F20</f>
         <v>7.8602620087336241</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="40" t="s">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" s="42" t="s">
         <v>169</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="11">
         <v>206</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="11">
         <v>2.5</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="19">
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="48">
         <v>0.4</v>
       </c>
-      <c r="G21" s="21">
-        <f t="shared" si="0"/>
+      <c r="G21" s="30">
+        <f>C21/B21</f>
         <v>1.2135922330097087E-2</v>
       </c>
-      <c r="H21" s="13">
-        <f t="shared" si="1"/>
+      <c r="H21" s="43">
+        <f>C21/F21</f>
         <v>6.25</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q21" s="50" t="s">
+        <v>244</v>
+      </c>
+      <c r="R21" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="S21" s="15" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="42" t="s">
         <v>63</v>
       </c>
@@ -9691,201 +9800,191 @@
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
-      <c r="F22" s="49">
+      <c r="F22" s="48">
         <v>0.33</v>
       </c>
       <c r="G22" s="30">
-        <f t="shared" si="0"/>
+        <f>C22/B22</f>
         <v>0</v>
       </c>
       <c r="H22" s="43">
-        <f t="shared" si="1"/>
+        <f>C22/F22</f>
         <v>0</v>
       </c>
-      <c r="O22" s="52" t="s">
-        <v>245</v>
-      </c>
-      <c r="P22" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="Q22" s="15" t="s">
+      <c r="R22" s="3" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="P23" s="3" t="s">
+      <c r="S22" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R23" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="Q23" s="3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="P24" s="3" t="s">
+      <c r="S23" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="Q24" s="3" t="s">
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R24" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="S24" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="P25" s="3" t="s">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="I25" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="J25" s="40" t="s">
+        <v>201</v>
+      </c>
+      <c r="K25" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="L25" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="M25" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="R25" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="S25" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="I26" s="3"/>
+      <c r="J26" s="41">
+        <v>2750</v>
+      </c>
+      <c r="K26" s="41">
+        <v>160</v>
+      </c>
+      <c r="L26" s="41">
+        <v>92</v>
+      </c>
+      <c r="M26" s="41">
+        <v>40</v>
+      </c>
+      <c r="R26" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="S26" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="Q25" s="3" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="I26" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="J26" s="40" t="s">
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="I27" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="J27" s="40" t="s">
         <v>201</v>
       </c>
-      <c r="K26" s="15" t="s">
+      <c r="K27" s="15" t="s">
         <v>202</v>
       </c>
-      <c r="L26" s="15" t="s">
+      <c r="L27" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="M26" s="15" t="s">
+      <c r="M27" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="P26" s="51" t="s">
-        <v>223</v>
-      </c>
-      <c r="Q26" s="51" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="I27" s="3"/>
-      <c r="J27" s="41">
-        <v>2750</v>
-      </c>
-      <c r="K27" s="41">
-        <v>160</v>
-      </c>
-      <c r="L27" s="41">
-        <v>92</v>
-      </c>
-      <c r="M27" s="41">
-        <v>40</v>
-      </c>
-      <c r="P27" s="51" t="s">
-        <v>225</v>
-      </c>
-      <c r="Q27" s="51" t="s">
+      <c r="R27" s="3" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="I28" s="15" t="s">
-        <v>206</v>
-      </c>
-      <c r="J28" s="40" t="s">
-        <v>201</v>
-      </c>
-      <c r="K28" s="15" t="s">
-        <v>202</v>
-      </c>
-      <c r="L28" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="M28" s="15" t="s">
-        <v>204</v>
-      </c>
-      <c r="P28" s="51" t="s">
+      <c r="S27" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="Q28" s="51" t="s">
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="I28" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="J28" s="3">
+        <f>J26*6</f>
+        <v>16500</v>
+      </c>
+      <c r="K28" s="3">
+        <f t="shared" ref="K28:M28" si="6">K26*6</f>
+        <v>960</v>
+      </c>
+      <c r="L28" s="3">
+        <f t="shared" si="6"/>
+        <v>552</v>
+      </c>
+      <c r="M28" s="3">
+        <f t="shared" si="6"/>
+        <v>240</v>
+      </c>
+      <c r="R28" s="3" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="I29" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="J29" s="3">
-        <f>J27*6</f>
-        <v>16500</v>
-      </c>
-      <c r="K29" s="3">
-        <f t="shared" ref="K29:M29" si="8">K27*6</f>
-        <v>960</v>
-      </c>
-      <c r="L29" s="3">
-        <f t="shared" si="8"/>
-        <v>552</v>
-      </c>
-      <c r="M29" s="3">
-        <f t="shared" si="8"/>
+      <c r="S28" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R29" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="S29" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R30" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="S30" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R31" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="S31" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R32" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="S32" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="P29" s="51" t="s">
-        <v>230</v>
-      </c>
-      <c r="Q29" s="51" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="P30" s="51" t="s">
-        <v>231</v>
-      </c>
-      <c r="Q30" s="51" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="P31" s="51" t="s">
-        <v>234</v>
-      </c>
-      <c r="Q31" s="51" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="P32" s="51" t="s">
-        <v>235</v>
-      </c>
-      <c r="Q32" s="51" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="33" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P33" s="51" t="s">
+    </row>
+    <row r="33" spans="18:19" x14ac:dyDescent="0.3">
+      <c r="R33" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="Q33" s="51" t="s">
+      <c r="S33" s="3" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="34" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P34" s="51" t="s">
+    <row r="34" spans="18:19" x14ac:dyDescent="0.3">
+      <c r="R34" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="Q34" s="51" t="s">
+      <c r="S34" s="3" t="s">
         <v>242</v>
-      </c>
-    </row>
-    <row r="35" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P35" s="51" t="s">
-        <v>238</v>
-      </c>
-      <c r="Q35" s="51" t="s">
-        <v>243</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O22" r:id="rId1" xr:uid="{FC8C911A-DFC8-416F-8E8E-2C5CBBC615A0}"/>
+    <hyperlink ref="Q21" r:id="rId1" xr:uid="{FC8C911A-DFC8-416F-8E8E-2C5CBBC615A0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added files for reti logiche and ingsw projects
</commit_message>
<xml_diff>
--- a/extra/studio cibi proteici.xlsx
+++ b/extra/studio cibi proteici.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Documents\uni\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B39A0D-29E8-42FA-B8CB-1358C7131185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E4D70A-9F1D-4B41-A820-F5B9ECA5FF37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
   </bookViews>
@@ -873,16 +873,16 @@
     <t>peperone (1p-200g)</t>
   </si>
   <si>
-    <t>1 peperone</t>
-  </si>
-  <si>
     <t>cavolfiore (1/4p-250g)</t>
   </si>
   <si>
-    <t>1/4 di cavolfiore</t>
-  </si>
-  <si>
     <t>250g riso bianco smart (5kg)</t>
+  </si>
+  <si>
+    <t>1/4 di cavolfiore (250g)</t>
+  </si>
+  <si>
+    <t>1 peperone (200g)</t>
   </si>
 </sst>
 </file>
@@ -1142,7 +1142,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1206,7 +1206,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -9086,8 +9085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{715CF0DF-138B-4B49-BC97-299FF5018F54}">
   <dimension ref="A1:AH34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9423,7 +9422,7 @@
         <v>35.333333333333336</v>
       </c>
       <c r="J6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K6">
         <f>30*2.5</f>
@@ -9763,7 +9762,7 @@
         <v>25.306122448979593</v>
       </c>
       <c r="R13" s="56" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="S13" s="3">
         <f>K5</f>
@@ -9856,8 +9855,8 @@
         <f t="shared" si="1"/>
         <v>22.891566265060241</v>
       </c>
-      <c r="R15" s="60" t="s">
-        <v>272</v>
+      <c r="R15" s="59" t="s">
+        <v>270</v>
       </c>
       <c r="S15" s="3">
         <f>B18*2.5</f>
@@ -10139,7 +10138,7 @@
       <c r="AA23" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="AB23" s="58" t="s">
+      <c r="AB23" s="57" t="s">
         <v>224</v>
       </c>
     </row>
@@ -10150,7 +10149,7 @@
       <c r="S24" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="U24" s="57" t="s">
+      <c r="U24" s="3" t="s">
         <v>263</v>
       </c>
       <c r="V24" s="17" t="s">
@@ -10162,19 +10161,19 @@
       <c r="X24" s="37" t="s">
         <v>228</v>
       </c>
-      <c r="Y24" s="57" t="s">
+      <c r="Y24" s="3" t="s">
         <v>264</v>
       </c>
       <c r="Z24" s="37" t="s">
         <v>232</v>
       </c>
-      <c r="AA24" s="57" t="s">
+      <c r="AA24" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="AB24" s="59" t="s">
+      <c r="AB24" s="58" t="s">
         <v>233</v>
       </c>
-      <c r="AC24" s="57" t="s">
+      <c r="AC24" s="3" t="s">
         <v>266</v>
       </c>
       <c r="AD24" s="17" t="s">
@@ -10183,13 +10182,13 @@
       <c r="AE24" s="37" t="s">
         <v>262</v>
       </c>
-      <c r="AF24" s="57" t="s">
+      <c r="AF24" s="3" t="s">
         <v>260</v>
       </c>
       <c r="AG24" s="37" t="s">
         <v>236</v>
       </c>
-      <c r="AH24" s="57" t="s">
+      <c r="AH24" s="3" t="s">
         <v>267</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added ingsw uml doc and edited protein studies
</commit_message>
<xml_diff>
--- a/extra/studio cibi proteici.xlsx
+++ b/extra/studio cibi proteici.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Documents\uni\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E4D70A-9F1D-4B41-A820-F5B9ECA5FF37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE4AD3EA-0A90-4A3A-8494-D5D849D43447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{F59D9EA6-31E6-4D8C-9410-A8BE9A94645C}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Foglio3" sheetId="3" r:id="rId3"/>
     <sheet name="Foglio4" sheetId="4" r:id="rId4"/>
     <sheet name="lean bulk last semester" sheetId="5" r:id="rId5"/>
+    <sheet name="lbls - updated table" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="283">
   <si>
     <t>proteine</t>
   </si>
@@ -883,6 +884,36 @@
   </si>
   <si>
     <t>1 peperone (200g)</t>
+  </si>
+  <si>
+    <t>trita suino esse</t>
+  </si>
+  <si>
+    <t>100g uova smart (2)</t>
+  </si>
+  <si>
+    <t>1/2 litro latte intero esse</t>
+  </si>
+  <si>
+    <t>1/2 cipolla</t>
+  </si>
+  <si>
+    <t>cipolla (1p-150g)</t>
+  </si>
+  <si>
+    <t>1/bottiglia passata di pomodoro smart</t>
+  </si>
+  <si>
+    <t>bottiglia passata di pomodoro smart</t>
+  </si>
+  <si>
+    <t>100g emmenthal</t>
+  </si>
+  <si>
+    <t>200g trita suino esse</t>
+  </si>
+  <si>
+    <t>1/2 bottiglia passata di pomodoro smart</t>
   </si>
 </sst>
 </file>
@@ -893,7 +924,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-410]_-;\-* #,##0.00\ [$€-410]_-;_-* &quot;-&quot;??\ [$€-410]_-;_-@_-"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -948,8 +979,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1004,8 +1042,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor theme="8"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1135,6 +1179,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1142,7 +1195,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1209,6 +1262,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1216,7 +1274,448 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="43">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="8"/>
+        </left>
+        <right style="thin">
+          <color theme="8"/>
+        </right>
+        <top style="thin">
+          <color theme="8"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="8"/>
+          <bgColor theme="8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -1615,20 +2114,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84F67106-4EFF-43B6-B540-766A1D8E564D}" name="Tabella1" displayName="Tabella1" ref="A1:F26" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84F67106-4EFF-43B6-B540-766A1D8E564D}" name="Tabella1" displayName="Tabella1" ref="A1:F26" totalsRowShown="0" headerRowDxfId="42" headerRowBorderDxfId="41" tableBorderDxfId="40" totalsRowBorderDxfId="39">
   <autoFilter ref="A1:F26" xr:uid="{84F67106-4EFF-43B6-B540-766A1D8E564D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F25">
     <sortCondition descending="1" ref="D1:D25"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{30081959-5619-4B55-B7D9-1175EC07AC45}" name="/100g" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{14FCB0BC-8DE4-4AA7-8660-575F63F8B8A6}" name="proteine" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{C0B50CE8-FDFE-49A8-8945-F7C5D2CD5713}" name="calorie" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{419A7849-565C-4737-B49A-97B34AC7F736}" name="rapporto proteine/calorie" dataDxfId="14">
+    <tableColumn id="1" xr3:uid="{30081959-5619-4B55-B7D9-1175EC07AC45}" name="/100g" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{14FCB0BC-8DE4-4AA7-8660-575F63F8B8A6}" name="proteine" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{C0B50CE8-FDFE-49A8-8945-F7C5D2CD5713}" name="calorie" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{419A7849-565C-4737-B49A-97B34AC7F736}" name="rapporto proteine/calorie" dataDxfId="35">
       <calculatedColumnFormula>B2/C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{FA12BE60-94F7-4342-93BD-B6B457295831}" name="prezzo/kg" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{616FE227-9C0F-4D3A-A972-663A04B87FDE}" name="rapporto proteine/€" dataDxfId="12">
+    <tableColumn id="5" xr3:uid="{FA12BE60-94F7-4342-93BD-B6B457295831}" name="prezzo/kg" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{616FE227-9C0F-4D3A-A972-663A04B87FDE}" name="rapporto proteine/€" dataDxfId="33">
       <calculatedColumnFormula>B2/E2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1637,22 +2136,22 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{ECDFEEA9-AA58-4204-A8C7-634A63CB75E6}" name="Table2" displayName="Table2" ref="A1:H22" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
-  <autoFilter ref="A1:H22" xr:uid="{ECDFEEA9-AA58-4204-A8C7-634A63CB75E6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{ECDFEEA9-AA58-4204-A8C7-634A63CB75E6}" name="Table2" displayName="Table2" ref="A1:H23" totalsRowShown="0" headerRowDxfId="32" headerRowBorderDxfId="31" tableBorderDxfId="30" totalsRowBorderDxfId="29">
+  <autoFilter ref="A1:H23" xr:uid="{ECDFEEA9-AA58-4204-A8C7-634A63CB75E6}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H22">
     <sortCondition descending="1" ref="H1:H22"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{AB4A45E1-B89A-4707-8479-BFF4F0659BF8}" name="foods (100g)" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{470D54CE-B5A5-41F6-95A8-DD7E923ED244}" name="cal" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{E694C129-0B2F-4C17-9437-94D714E9FD4B}" name="pro" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{E0C3B141-BD31-4EC9-A404-86508C0E7FD7}" name="fat" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{03502587-F9AA-4481-A3E0-2A5A7867FA98}" name="fiber" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{D7F14DF8-B895-41DB-ACB2-D51384C142B1}" name="eur" dataDxfId="2" dataCellStyle="Currency"/>
-    <tableColumn id="5" xr3:uid="{B148E6D9-D950-47D2-BE5C-B98C6182553A}" name="pro/cal" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{AB4A45E1-B89A-4707-8479-BFF4F0659BF8}" name="foods (100g)" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{470D54CE-B5A5-41F6-95A8-DD7E923ED244}" name="cal" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{E694C129-0B2F-4C17-9437-94D714E9FD4B}" name="pro" dataDxfId="26"/>
+    <tableColumn id="9" xr3:uid="{E0C3B141-BD31-4EC9-A404-86508C0E7FD7}" name="fat" dataDxfId="25"/>
+    <tableColumn id="10" xr3:uid="{03502587-F9AA-4481-A3E0-2A5A7867FA98}" name="fiber" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{D7F14DF8-B895-41DB-ACB2-D51384C142B1}" name="eur" dataDxfId="23" dataCellStyle="Currency"/>
+    <tableColumn id="5" xr3:uid="{B148E6D9-D950-47D2-BE5C-B98C6182553A}" name="pro/cal" dataDxfId="22">
       <calculatedColumnFormula>C2/B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C3CF0D3F-CCE3-45AB-918F-D28A95B39AAC}" name="pro/eur" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{C3CF0D3F-CCE3-45AB-918F-D28A95B39AAC}" name="pro/eur" dataDxfId="21">
       <calculatedColumnFormula>C2/F2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1676,6 +2175,45 @@
       <calculatedColumnFormula>2.7*0.75</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{CF56D516-2CC9-4785-A42A-00DE8FC927E9}" name="eur"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{99F0CE33-D728-49D2-B79B-6B0343599F72}" name="Table25" displayName="Table25" ref="A1:H15" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+  <autoFilter ref="A1:H15" xr:uid="{99F0CE33-D728-49D2-B79B-6B0343599F72}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H15">
+    <sortCondition descending="1" ref="H1:H15"/>
+  </sortState>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{1E787288-78B0-4898-9AFE-B4908D7E70EB}" name="foods (100g)" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{16EF61D3-EC73-4581-8C26-4A96E58362A6}" name="cal" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{A1CCA726-992F-44C7-9B18-283B7D69DFE4}" name="pro" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{9B7FAD1D-91B2-4D76-A9F5-D67715008BF3}" name="fat" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{E472F880-C8EC-4BB6-94DA-A869EB84C6E4}" name="fiber" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{F1A7C1B0-E074-484C-81CB-201FC855F703}" name="eur" dataDxfId="11" dataCellStyle="Currency"/>
+    <tableColumn id="5" xr3:uid="{011C7AC3-52B0-44D3-9F4A-1BCFE7ABF791}" name="pro/cal" dataDxfId="10">
+      <calculatedColumnFormula>C2/B2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{DB36C708-6AD8-4EC5-94B3-1C34F1FBE19E}" name="pro/eur" dataDxfId="9">
+      <calculatedColumnFormula>C2/F2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{72A2D424-7821-4D1B-8547-C40DB318AA37}" name="Table5" displayName="Table5" ref="J1:O5" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
+  <autoFilter ref="J1:O5" xr:uid="{72A2D424-7821-4D1B-8547-C40DB318AA37}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{53493349-48E5-4EC9-BF29-36FBAD8F3055}" name="vegetable/ fruit (one piece or 100g)" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{AE5AA126-BD67-4127-A484-BD7668807123}" name="cal" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{6842870C-B1E6-47AD-BD5F-31118A902694}" name="pro" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{827719EF-DEC9-451A-8EFF-041DE89F27E8}" name="fat" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{BA433ED4-5652-416C-86E1-A963BBC8FD78}" name="fiber" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{DC87421C-D955-4D1D-B58C-5212292B68D4}" name="eur" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9085,8 +9623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{715CF0DF-138B-4B49-BC97-299FF5018F54}">
   <dimension ref="A1:AH34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2:W17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10111,6 +10649,32 @@
       </c>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A23" s="42" t="s">
+        <v>273</v>
+      </c>
+      <c r="B23" s="11">
+        <v>240</v>
+      </c>
+      <c r="C23" s="11">
+        <v>19</v>
+      </c>
+      <c r="D23" s="11">
+        <v>15</v>
+      </c>
+      <c r="E23" s="11">
+        <v>0</v>
+      </c>
+      <c r="F23" s="61">
+        <v>0.75</v>
+      </c>
+      <c r="G23" s="30">
+        <f>C23/B23</f>
+        <v>7.9166666666666663E-2</v>
+      </c>
+      <c r="H23" s="43">
+        <f>C23/F23</f>
+        <v>25.333333333333332</v>
+      </c>
       <c r="R23" s="3" t="s">
         <v>219</v>
       </c>
@@ -10348,4 +10912,1168 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95CD8901-08BD-42CE-8325-B44B1BCFAADA}">
+  <dimension ref="A1:V24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="U34" sqref="U34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" customWidth="1"/>
+    <col min="7" max="8" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="36" customWidth="1"/>
+    <col min="17" max="17" width="39.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="44" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>209</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>211</v>
+      </c>
+      <c r="F1" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" s="46" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" s="62" t="s">
+        <v>247</v>
+      </c>
+      <c r="K1" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="M1" s="62" t="s">
+        <v>209</v>
+      </c>
+      <c r="N1" s="62" t="s">
+        <v>211</v>
+      </c>
+      <c r="O1" s="62" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="3">
+        <v>209</v>
+      </c>
+      <c r="C2" s="3">
+        <v>13</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="19">
+        <v>0.22</v>
+      </c>
+      <c r="G2" s="21">
+        <f t="shared" ref="G2:G15" si="0">C2/B2</f>
+        <v>6.2200956937799042E-2</v>
+      </c>
+      <c r="H2" s="21">
+        <f t="shared" ref="H2:H15" si="1">C2/F2</f>
+        <v>59.090909090909093</v>
+      </c>
+      <c r="J2" s="60" t="s">
+        <v>250</v>
+      </c>
+      <c r="K2" s="60">
+        <f>41*0.75</f>
+        <v>30.75</v>
+      </c>
+      <c r="L2" s="60">
+        <v>0.75</v>
+      </c>
+      <c r="M2" s="60">
+        <f>0.2*0.75</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="N2" s="60">
+        <f>2.7*0.75</f>
+        <v>2.0250000000000004</v>
+      </c>
+      <c r="O2" s="60">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="40" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" s="3">
+        <v>126</v>
+      </c>
+      <c r="C3" s="3">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="19">
+        <v>0.4</v>
+      </c>
+      <c r="G3" s="21">
+        <f t="shared" si="0"/>
+        <v>0.14206349206349206</v>
+      </c>
+      <c r="H3" s="21">
+        <f t="shared" si="1"/>
+        <v>44.749999999999993</v>
+      </c>
+      <c r="J3" s="60" t="s">
+        <v>254</v>
+      </c>
+      <c r="K3" s="60">
+        <v>76</v>
+      </c>
+      <c r="L3" s="60">
+        <v>1.2</v>
+      </c>
+      <c r="M3" s="60">
+        <v>0.3</v>
+      </c>
+      <c r="N3" s="60">
+        <v>1.19</v>
+      </c>
+      <c r="O3" s="60">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="40" t="s">
+        <v>245</v>
+      </c>
+      <c r="B4" s="3">
+        <v>358</v>
+      </c>
+      <c r="C4" s="3">
+        <v>82</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="22">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="G4" s="21">
+        <f t="shared" si="0"/>
+        <v>0.22905027932960895</v>
+      </c>
+      <c r="H4" s="21">
+        <f t="shared" si="1"/>
+        <v>40.796019900497519</v>
+      </c>
+      <c r="J4" s="60" t="s">
+        <v>277</v>
+      </c>
+      <c r="K4" s="60">
+        <f>28*1.5</f>
+        <v>42</v>
+      </c>
+      <c r="L4" s="60">
+        <v>1.5</v>
+      </c>
+      <c r="M4" s="60">
+        <v>0</v>
+      </c>
+      <c r="N4" s="60">
+        <v>1.5</v>
+      </c>
+      <c r="O4" s="60">
+        <f>0.15*1.5</f>
+        <v>0.22499999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="40" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" s="3">
+        <v>382</v>
+      </c>
+      <c r="C5" s="3">
+        <v>28</v>
+      </c>
+      <c r="D5" s="3">
+        <v>30</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="22">
+        <v>0.75</v>
+      </c>
+      <c r="G5" s="21">
+        <f t="shared" si="0"/>
+        <v>7.3298429319371722E-2</v>
+      </c>
+      <c r="H5" s="13">
+        <f t="shared" si="1"/>
+        <v>37.333333333333336</v>
+      </c>
+      <c r="J5" s="64" t="s">
+        <v>279</v>
+      </c>
+      <c r="K5" s="64">
+        <f>28*6.8</f>
+        <v>190.4</v>
+      </c>
+      <c r="L5" s="64">
+        <f>1.5*6.8</f>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="M5" s="64">
+        <f>0.1*6.8</f>
+        <v>0.68</v>
+      </c>
+      <c r="N5" s="64">
+        <f>1.3*6.8</f>
+        <v>8.84</v>
+      </c>
+      <c r="O5" s="64">
+        <f>0.98</f>
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="40" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="3">
+        <v>51</v>
+      </c>
+      <c r="C6" s="3">
+        <v>5.3</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="19">
+        <v>0.15</v>
+      </c>
+      <c r="G6" s="21">
+        <f t="shared" si="0"/>
+        <v>0.10392156862745097</v>
+      </c>
+      <c r="H6" s="13">
+        <f t="shared" si="1"/>
+        <v>35.333333333333336</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="40" t="s">
+        <v>215</v>
+      </c>
+      <c r="B7" s="3">
+        <v>65</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3.3</v>
+      </c>
+      <c r="D7" s="3">
+        <v>3.6</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="G7" s="21">
+        <f t="shared" si="0"/>
+        <v>5.0769230769230768E-2</v>
+      </c>
+      <c r="H7" s="13">
+        <f t="shared" si="1"/>
+        <v>32.999999999999993</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="40" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" s="3">
+        <v>169</v>
+      </c>
+      <c r="C8" s="3">
+        <v>15.4</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="19">
+        <v>0.47</v>
+      </c>
+      <c r="G8" s="21">
+        <f t="shared" si="0"/>
+        <v>9.1124260355029588E-2</v>
+      </c>
+      <c r="H8" s="13">
+        <f t="shared" si="1"/>
+        <v>32.765957446808514</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="B9" s="3">
+        <v>100</v>
+      </c>
+      <c r="C9" s="3">
+        <v>23.3</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="G9" s="21">
+        <f t="shared" si="0"/>
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="H9" s="13">
+        <f t="shared" si="1"/>
+        <v>29.125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="3">
+        <v>123</v>
+      </c>
+      <c r="C10" s="3">
+        <v>30</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="19">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="G10" s="21">
+        <f t="shared" si="0"/>
+        <v>0.24390243902439024</v>
+      </c>
+      <c r="H10" s="13">
+        <f t="shared" si="1"/>
+        <v>27.52293577981651</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="O10" s="26"/>
+      <c r="Q10" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="V10" s="26"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="40" t="s">
+        <v>273</v>
+      </c>
+      <c r="B11" s="3">
+        <v>240</v>
+      </c>
+      <c r="C11" s="3">
+        <v>19</v>
+      </c>
+      <c r="D11" s="3">
+        <v>15</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="22">
+        <v>0.75</v>
+      </c>
+      <c r="G11" s="21">
+        <f t="shared" si="0"/>
+        <v>7.9166666666666663E-2</v>
+      </c>
+      <c r="H11" s="13">
+        <f t="shared" si="1"/>
+        <v>25.333333333333332</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="L11" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="M11" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="N11" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="O11" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q11" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="R11" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="S11" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="T11" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="U11" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="V11" s="49" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="40" t="s">
+        <v>274</v>
+      </c>
+      <c r="B12" s="3">
+        <v>136</v>
+      </c>
+      <c r="C12" s="3">
+        <v>12.4</v>
+      </c>
+      <c r="D12" s="3">
+        <v>9.5</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="19">
+        <v>0.49</v>
+      </c>
+      <c r="G12" s="21">
+        <f t="shared" si="0"/>
+        <v>9.1176470588235303E-2</v>
+      </c>
+      <c r="H12" s="13">
+        <f t="shared" si="1"/>
+        <v>25.306122448979593</v>
+      </c>
+      <c r="J12" s="55" t="s">
+        <v>244</v>
+      </c>
+      <c r="K12" s="3">
+        <f>Table25[[#This Row],[cal]]</f>
+        <v>136</v>
+      </c>
+      <c r="L12" s="3">
+        <f>Table25[[#This Row],[pro]]</f>
+        <v>12.4</v>
+      </c>
+      <c r="M12" s="3">
+        <f>Table25[[#This Row],[fat]]</f>
+        <v>9.5</v>
+      </c>
+      <c r="N12" s="3">
+        <f>Table25[[#This Row],[fiber]]</f>
+        <v>0</v>
+      </c>
+      <c r="O12" s="3">
+        <f>Table25[[#This Row],[eur]]</f>
+        <v>0.49</v>
+      </c>
+      <c r="Q12" s="55" t="s">
+        <v>244</v>
+      </c>
+      <c r="R12" s="3">
+        <f>Table25[[#This Row],[cal]]</f>
+        <v>136</v>
+      </c>
+      <c r="S12" s="3">
+        <f>Table25[[#This Row],[pro]]</f>
+        <v>12.4</v>
+      </c>
+      <c r="T12" s="3">
+        <f>Table25[[#This Row],[fat]]</f>
+        <v>9.5</v>
+      </c>
+      <c r="U12" s="3">
+        <f>Table25[[#This Row],[fiber]]</f>
+        <v>0</v>
+      </c>
+      <c r="V12" s="3">
+        <f>Table25[[#This Row],[eur]]</f>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="B13" s="3">
+        <v>331</v>
+      </c>
+      <c r="C13" s="3">
+        <v>19</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="19">
+        <v>0.83</v>
+      </c>
+      <c r="G13" s="21">
+        <f t="shared" si="0"/>
+        <v>5.7401812688821753E-2</v>
+      </c>
+      <c r="H13" s="13">
+        <f t="shared" si="1"/>
+        <v>22.891566265060241</v>
+      </c>
+      <c r="J13" s="55" t="s">
+        <v>275</v>
+      </c>
+      <c r="K13" s="3">
+        <f>B7*5</f>
+        <v>325</v>
+      </c>
+      <c r="L13" s="3">
+        <f t="shared" ref="L13:O13" si="2">C7*5</f>
+        <v>16.5</v>
+      </c>
+      <c r="M13" s="3">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="N13" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="3">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="Q13" s="55" t="s">
+        <v>275</v>
+      </c>
+      <c r="R13" s="3">
+        <f>B7*5</f>
+        <v>325</v>
+      </c>
+      <c r="S13" s="3">
+        <f t="shared" ref="S13:V13" si="3">C7*5</f>
+        <v>16.5</v>
+      </c>
+      <c r="T13" s="3">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="U13" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V13" s="3">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="42" t="s">
+        <v>189</v>
+      </c>
+      <c r="B14" s="11">
+        <v>350</v>
+      </c>
+      <c r="C14" s="11">
+        <v>3</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11">
+        <v>1.4</v>
+      </c>
+      <c r="F14" s="48">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G14" s="30">
+        <f t="shared" si="0"/>
+        <v>8.5714285714285719E-3</v>
+      </c>
+      <c r="H14" s="43">
+        <f t="shared" si="1"/>
+        <v>21.428571428571427</v>
+      </c>
+      <c r="J14" s="56" t="s">
+        <v>255</v>
+      </c>
+      <c r="K14" s="3">
+        <f>K3</f>
+        <v>76</v>
+      </c>
+      <c r="L14" s="3">
+        <f t="shared" ref="L14:O14" si="4">L3</f>
+        <v>1.2</v>
+      </c>
+      <c r="M14" s="3">
+        <f t="shared" si="4"/>
+        <v>0.3</v>
+      </c>
+      <c r="N14" s="3">
+        <f t="shared" si="4"/>
+        <v>1.19</v>
+      </c>
+      <c r="O14" s="3">
+        <f t="shared" si="4"/>
+        <v>0.1</v>
+      </c>
+      <c r="Q14" s="56" t="s">
+        <v>255</v>
+      </c>
+      <c r="R14" s="3">
+        <f>K3</f>
+        <v>76</v>
+      </c>
+      <c r="S14" s="3">
+        <f t="shared" ref="S14:V14" si="5">L3</f>
+        <v>1.2</v>
+      </c>
+      <c r="T14" s="3">
+        <f t="shared" si="5"/>
+        <v>0.3</v>
+      </c>
+      <c r="U14" s="3">
+        <f t="shared" si="5"/>
+        <v>1.19</v>
+      </c>
+      <c r="V14" s="3">
+        <f t="shared" si="5"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="11">
+        <v>185</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="48">
+        <v>0.33</v>
+      </c>
+      <c r="G15" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="43">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="19"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="19"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="J16" s="55" t="s">
+        <v>213</v>
+      </c>
+      <c r="K16" s="3">
+        <f>B9*2</f>
+        <v>200</v>
+      </c>
+      <c r="L16" s="3">
+        <f t="shared" ref="L16:O16" si="6">C9*2</f>
+        <v>46.6</v>
+      </c>
+      <c r="M16" s="3">
+        <f t="shared" si="6"/>
+        <v>1.6</v>
+      </c>
+      <c r="N16" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="O16" s="3">
+        <f t="shared" si="6"/>
+        <v>1.6</v>
+      </c>
+      <c r="Q16" s="55" t="s">
+        <v>281</v>
+      </c>
+      <c r="R16" s="3">
+        <f>B11*2</f>
+        <v>480</v>
+      </c>
+      <c r="S16" s="3">
+        <f t="shared" ref="S16:V16" si="7">C11*2</f>
+        <v>38</v>
+      </c>
+      <c r="T16" s="3">
+        <f t="shared" si="7"/>
+        <v>30</v>
+      </c>
+      <c r="U16" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V16" s="3">
+        <f t="shared" si="7"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="J17" s="55" t="s">
+        <v>212</v>
+      </c>
+      <c r="K17" s="3">
+        <f>B5*2</f>
+        <v>764</v>
+      </c>
+      <c r="L17" s="3">
+        <f t="shared" ref="L17:O17" si="8">C5*2</f>
+        <v>56</v>
+      </c>
+      <c r="M17" s="3">
+        <f t="shared" si="8"/>
+        <v>60</v>
+      </c>
+      <c r="N17" s="3">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="3">
+        <f t="shared" si="8"/>
+        <v>1.5</v>
+      </c>
+      <c r="Q17" s="55" t="s">
+        <v>213</v>
+      </c>
+      <c r="R17" s="3">
+        <f>B9*2</f>
+        <v>200</v>
+      </c>
+      <c r="S17" s="3">
+        <f t="shared" ref="S17:V17" si="9">C9*2</f>
+        <v>46.6</v>
+      </c>
+      <c r="T17" s="3">
+        <f t="shared" si="9"/>
+        <v>1.6</v>
+      </c>
+      <c r="U17" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="V17" s="3">
+        <f t="shared" si="9"/>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="J18" s="55" t="s">
+        <v>214</v>
+      </c>
+      <c r="K18" s="3">
+        <f>B6*5</f>
+        <v>255</v>
+      </c>
+      <c r="L18" s="3">
+        <f t="shared" ref="L18:O18" si="10">C6*5</f>
+        <v>26.5</v>
+      </c>
+      <c r="M18" s="3">
+        <f t="shared" si="10"/>
+        <v>0.5</v>
+      </c>
+      <c r="N18" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="O18" s="3">
+        <f t="shared" si="10"/>
+        <v>0.75</v>
+      </c>
+      <c r="Q18" s="55" t="s">
+        <v>280</v>
+      </c>
+      <c r="R18" s="3">
+        <f>B5*1</f>
+        <v>382</v>
+      </c>
+      <c r="S18" s="3">
+        <f t="shared" ref="S18:V18" si="11">C5*1</f>
+        <v>28</v>
+      </c>
+      <c r="T18" s="3">
+        <f t="shared" si="11"/>
+        <v>30</v>
+      </c>
+      <c r="U18" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="V18" s="3">
+        <f t="shared" si="11"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="J19" s="56" t="s">
+        <v>251</v>
+      </c>
+      <c r="K19" s="3">
+        <f>K2</f>
+        <v>30.75</v>
+      </c>
+      <c r="L19" s="3">
+        <f t="shared" ref="L19:O19" si="12">L2</f>
+        <v>0.75</v>
+      </c>
+      <c r="M19" s="3">
+        <f t="shared" si="12"/>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="N19" s="3">
+        <f t="shared" si="12"/>
+        <v>2.0250000000000004</v>
+      </c>
+      <c r="O19" s="3">
+        <f t="shared" si="12"/>
+        <v>0.09</v>
+      </c>
+      <c r="Q19" s="56" t="s">
+        <v>251</v>
+      </c>
+      <c r="R19" s="3">
+        <f>K2</f>
+        <v>30.75</v>
+      </c>
+      <c r="S19" s="3">
+        <f t="shared" ref="S19:V19" si="13">L2</f>
+        <v>0.75</v>
+      </c>
+      <c r="T19" s="3">
+        <f t="shared" si="13"/>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="U19" s="3">
+        <f t="shared" si="13"/>
+        <v>2.0250000000000004</v>
+      </c>
+      <c r="V19" s="3">
+        <f t="shared" si="13"/>
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="B20" s="40" t="s">
+        <v>201</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="J20" s="56" t="s">
+        <v>276</v>
+      </c>
+      <c r="K20" s="3">
+        <f>K4*0.5</f>
+        <v>21</v>
+      </c>
+      <c r="L20" s="3">
+        <f t="shared" ref="L20:O20" si="14">L4*0.5</f>
+        <v>0.75</v>
+      </c>
+      <c r="M20" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="3">
+        <f t="shared" si="14"/>
+        <v>0.75</v>
+      </c>
+      <c r="O20" s="3">
+        <f t="shared" si="14"/>
+        <v>0.11249999999999999</v>
+      </c>
+      <c r="Q20" s="56" t="s">
+        <v>276</v>
+      </c>
+      <c r="R20" s="3">
+        <f>K4*0.5</f>
+        <v>21</v>
+      </c>
+      <c r="S20" s="3">
+        <f t="shared" ref="S20:V21" si="15">L4*0.5</f>
+        <v>0.75</v>
+      </c>
+      <c r="T20" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="U20" s="3">
+        <f t="shared" si="15"/>
+        <v>0.75</v>
+      </c>
+      <c r="V20" s="3">
+        <f t="shared" si="15"/>
+        <v>0.11249999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="41">
+        <v>2750</v>
+      </c>
+      <c r="C21" s="41">
+        <v>160</v>
+      </c>
+      <c r="D21" s="41">
+        <v>92</v>
+      </c>
+      <c r="E21" s="41">
+        <v>40</v>
+      </c>
+      <c r="J21" s="63" t="s">
+        <v>278</v>
+      </c>
+      <c r="K21" s="3">
+        <f>K5*0.5</f>
+        <v>95.2</v>
+      </c>
+      <c r="L21" s="3">
+        <f t="shared" ref="L21:O21" si="16">L5*0.5</f>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="M21" s="3">
+        <f t="shared" si="16"/>
+        <v>0.34</v>
+      </c>
+      <c r="N21" s="3">
+        <f t="shared" si="16"/>
+        <v>4.42</v>
+      </c>
+      <c r="O21" s="3">
+        <f t="shared" si="16"/>
+        <v>0.49</v>
+      </c>
+      <c r="Q21" s="63" t="s">
+        <v>282</v>
+      </c>
+      <c r="R21" s="3">
+        <f>K5*0.5</f>
+        <v>95.2</v>
+      </c>
+      <c r="S21" s="3">
+        <f t="shared" si="15"/>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="T21" s="3">
+        <f t="shared" si="15"/>
+        <v>0.34</v>
+      </c>
+      <c r="U21" s="3">
+        <f t="shared" si="15"/>
+        <v>4.42</v>
+      </c>
+      <c r="V21" s="3">
+        <f t="shared" si="15"/>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="B22" s="40" t="s">
+        <v>201</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="J22" s="59" t="s">
+        <v>270</v>
+      </c>
+      <c r="K22" s="3">
+        <f>B14*2.5</f>
+        <v>875</v>
+      </c>
+      <c r="L22" s="3">
+        <f>C14*2.5</f>
+        <v>7.5</v>
+      </c>
+      <c r="M22" s="3">
+        <f>D14*2.5</f>
+        <v>0</v>
+      </c>
+      <c r="N22" s="3">
+        <f>E14*2.5</f>
+        <v>3.5</v>
+      </c>
+      <c r="O22" s="3">
+        <f>F14*2.5</f>
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="Q22" s="59" t="s">
+        <v>270</v>
+      </c>
+      <c r="R22" s="3">
+        <f>B14*2.5</f>
+        <v>875</v>
+      </c>
+      <c r="S22" s="3">
+        <f t="shared" ref="S22:V22" si="17">C14*2.5</f>
+        <v>7.5</v>
+      </c>
+      <c r="T22" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="U22" s="3">
+        <f t="shared" si="17"/>
+        <v>3.5</v>
+      </c>
+      <c r="V22" s="3">
+        <f t="shared" si="17"/>
+        <v>0.35000000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B23" s="3">
+        <f>B21*6</f>
+        <v>16500</v>
+      </c>
+      <c r="C23" s="3">
+        <f t="shared" ref="C23:E23" si="18">C21*6</f>
+        <v>960</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="18"/>
+        <v>552</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="18"/>
+        <v>240</v>
+      </c>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="19"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="19"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="J24" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="K24" s="15">
+        <f>SUM(K12:K23)</f>
+        <v>2777.95</v>
+      </c>
+      <c r="L24" s="15">
+        <f>SUM(L12:L23)</f>
+        <v>173.29999999999998</v>
+      </c>
+      <c r="M24" s="15">
+        <f>SUM(M12:M23)</f>
+        <v>90.390000000000015</v>
+      </c>
+      <c r="N24" s="15">
+        <f>SUM(N12:N23)</f>
+        <v>11.885</v>
+      </c>
+      <c r="O24" s="15">
+        <f>SUM(O12:O23)</f>
+        <v>5.9824999999999999</v>
+      </c>
+      <c r="Q24" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="R24" s="15">
+        <f>SUM(R12:R23)</f>
+        <v>2620.9499999999998</v>
+      </c>
+      <c r="S24" s="15">
+        <f>SUM(S12:S23)</f>
+        <v>156.79999999999998</v>
+      </c>
+      <c r="T24" s="15">
+        <f>SUM(T12:T23)</f>
+        <v>89.890000000000015</v>
+      </c>
+      <c r="U24" s="15">
+        <f>SUM(U12:U23)</f>
+        <v>11.885</v>
+      </c>
+      <c r="V24" s="15">
+        <f>SUM(V12:V23)</f>
+        <v>5.982499999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="N5" formula="1"/>
+  </ignoredErrors>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>